<commit_message>
More robust Monte Carlo
Updated the Monte Carlo initialization to not be hardcoded for propellant parameters. Also fixed an error in the excel file where the units were in inches instead of meters
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -20,13 +20,14 @@
     <sheet name="Results 27-Aug-2017 14-34-48" sheetId="14" r:id="rId11"/>
     <sheet name="Results 27-Aug-2017 14-35-18" sheetId="15" r:id="rId12"/>
     <sheet name="Results 27-Aug-2017 14-35-43" sheetId="16" r:id="rId13"/>
+    <sheet name="Results 17-Sep-2017 13-34-09" sheetId="17" r:id="rId14"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="154">
   <si>
     <t>Total inert mass</t>
   </si>
@@ -480,6 +481,15 @@
   <si>
     <t>C2H6</t>
   </si>
+  <si>
+    <t>m^3</t>
+  </si>
+  <si>
+    <t>in^3 to m^3</t>
+  </si>
+  <si>
+    <t>in to m</t>
+  </si>
 </sst>
 </file>
 
@@ -554,7 +564,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -564,6 +574,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -8039,12 +8050,1719 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2:AA24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>-9.8077912946324943</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>46.425430387139727</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0.10254009728482141</v>
+      </c>
+      <c r="K2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2">
+        <v>35464.700908851999</v>
+      </c>
+      <c r="O2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" t="s">
+        <v>57</v>
+      </c>
+      <c r="V2">
+        <v>300</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z2">
+        <v>30.119651471379374</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1.2927625760784508E-4</v>
+      </c>
+      <c r="B3">
+        <v>-9.8077625504415149</v>
+      </c>
+      <c r="C3">
+        <v>-1.2679127000054134E-3</v>
+      </c>
+      <c r="D3">
+        <v>-8.1955544446884481E-8</v>
+      </c>
+      <c r="E3">
+        <v>3.7259000016548696E-6</v>
+      </c>
+      <c r="F3">
+        <v>46.425291961004376</v>
+      </c>
+      <c r="G3">
+        <v>-7.5977496586340368E-9</v>
+      </c>
+      <c r="H3">
+        <v>0.10387424140300441</v>
+      </c>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3">
+        <v>1.6055226058921335</v>
+      </c>
+      <c r="P3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" t="s">
+        <v>58</v>
+      </c>
+      <c r="V3">
+        <v>4</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>7.756575456470704E-4</v>
+      </c>
+      <c r="B4">
+        <v>-9.8076131154285786</v>
+      </c>
+      <c r="C4">
+        <v>-7.6074191148936118E-3</v>
+      </c>
+      <c r="D4">
+        <v>-2.9503849521676501E-6</v>
+      </c>
+      <c r="E4">
+        <v>2.235523225828826E-5</v>
+      </c>
+      <c r="F4">
+        <v>46.424599830327629</v>
+      </c>
+      <c r="G4">
+        <v>-2.7351488292655467E-7</v>
+      </c>
+      <c r="H4">
+        <v>0.11080988755459328</v>
+      </c>
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4">
+        <v>4.18964832968169</v>
+      </c>
+      <c r="P4" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q4">
+        <v>5887436.804562035</v>
+      </c>
+      <c r="U4" t="s">
+        <v>59</v>
+      </c>
+      <c r="V4">
+        <v>0.9</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4.0075639858431966E-3</v>
+      </c>
+      <c r="B5">
+        <v>-9.8067021172114792</v>
+      </c>
+      <c r="C5">
+        <v>-3.9303314184888742E-2</v>
+      </c>
+      <c r="D5">
+        <v>-7.8756727070909748E-5</v>
+      </c>
+      <c r="E5">
+        <v>1.1549708292688314E-4</v>
+      </c>
+      <c r="F5">
+        <v>46.421139176943903</v>
+      </c>
+      <c r="G5">
+        <v>-7.3007020574227435E-6</v>
+      </c>
+      <c r="H5">
+        <v>0.15308417521310441</v>
+      </c>
+      <c r="K5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5">
+        <v>251.05270641842867</v>
+      </c>
+      <c r="P5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q5">
+        <v>853.90017992824039</v>
+      </c>
+      <c r="U5" t="s">
+        <v>53</v>
+      </c>
+      <c r="V5">
+        <v>3</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2.0167096186823826E-2</v>
+      </c>
+      <c r="B6">
+        <v>-9.7933979606210322</v>
+      </c>
+      <c r="C6">
+        <v>-0.19769529882609704</v>
+      </c>
+      <c r="D6">
+        <v>-1.9939277550988723E-3</v>
+      </c>
+      <c r="E6">
+        <v>5.8094922280963065E-4</v>
+      </c>
+      <c r="F6">
+        <v>46.403835910025251</v>
+      </c>
+      <c r="G6">
+        <v>-1.8471367238977405E-4</v>
+      </c>
+      <c r="H6">
+        <v>0.77021359744104567</v>
+      </c>
+      <c r="K6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6">
+        <v>758.82951363981294</v>
+      </c>
+      <c r="P6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q6">
+        <v>724.70128514490443</v>
+      </c>
+      <c r="U6" t="s">
+        <v>60</v>
+      </c>
+      <c r="V6">
+        <v>300</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z6">
+        <v>1.8241469247509919E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5.0193406172259133E-2</v>
+      </c>
+      <c r="B7">
+        <v>-9.4776534591924424</v>
+      </c>
+      <c r="C7">
+        <v>-0.48908457865991584</v>
+      </c>
+      <c r="D7">
+        <v>-1.2325525762527318E-2</v>
+      </c>
+      <c r="E7">
+        <v>1.437228272185497E-3</v>
+      </c>
+      <c r="F7">
+        <v>46.371684406516465</v>
+      </c>
+      <c r="G7">
+        <v>-1.1305108328976616E-3</v>
+      </c>
+      <c r="H7">
+        <v>15.410338393092609</v>
+      </c>
+      <c r="P7" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q7">
+        <v>0.02</v>
+      </c>
+      <c r="U7" t="s">
+        <v>61</v>
+      </c>
+      <c r="V7">
+        <v>45</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7.4181148788984297E-2</v>
+      </c>
+      <c r="B8">
+        <v>-6.3831877085047086</v>
+      </c>
+      <c r="C8">
+        <v>-0.6922159833828424</v>
+      </c>
+      <c r="D8">
+        <v>-2.6631625412908859E-2</v>
+      </c>
+      <c r="E8">
+        <v>2.0341516879832482E-3</v>
+      </c>
+      <c r="F8">
+        <v>46.345998866359061</v>
+      </c>
+      <c r="G8">
+        <v>-2.2645954591146637E-3</v>
+      </c>
+      <c r="H8">
+        <v>158.81677398140698</v>
+      </c>
+      <c r="P8" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q8">
+        <v>14.494025702898089</v>
+      </c>
+      <c r="U8" t="s">
+        <v>62</v>
+      </c>
+      <c r="V8">
+        <v>8</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA8">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9.8168891405709474E-2</v>
+      </c>
+      <c r="B9">
+        <v>12.345317242511646</v>
+      </c>
+      <c r="C9">
+        <v>-0.66771102714926323</v>
+      </c>
+      <c r="D9">
+        <v>-4.3842209512288448E-2</v>
+      </c>
+      <c r="E9">
+        <v>1.9621408374169858E-3</v>
+      </c>
+      <c r="F9">
+        <v>46.320313326201664</v>
+      </c>
+      <c r="G9">
+        <v>-2.1071002610111265E-3</v>
+      </c>
+      <c r="H9">
+        <v>1026.2391294142767</v>
+      </c>
+      <c r="O9" t="s">
+        <v>54</v>
+      </c>
+      <c r="U9" t="s">
+        <v>63</v>
+      </c>
+      <c r="V9">
+        <v>45</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA9">
+        <v>6.8647640279612546E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.11929113903532224</v>
+      </c>
+      <c r="B10">
+        <v>32.787922415016681</v>
+      </c>
+      <c r="C10">
+        <v>-0.16331339536533884</v>
+      </c>
+      <c r="D10">
+        <v>-5.3393017859304434E-2</v>
+      </c>
+      <c r="E10">
+        <v>4.7991396696384206E-4</v>
+      </c>
+      <c r="F10">
+        <v>46.297696094210572</v>
+      </c>
+      <c r="G10">
+        <v>-1.2605269000301889E-4</v>
+      </c>
+      <c r="H10">
+        <v>1972.1855401625128</v>
+      </c>
+      <c r="P10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>30</v>
+      </c>
+      <c r="R10" t="s">
+        <v>150</v>
+      </c>
+      <c r="U10" t="s">
+        <v>64</v>
+      </c>
+      <c r="V10">
+        <v>15</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA10">
+        <v>1403.543030798616</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.14024201245843138</v>
+      </c>
+      <c r="B11">
+        <v>38.142741699470029</v>
+      </c>
+      <c r="C11">
+        <v>0.5959858762313498</v>
+      </c>
+      <c r="D11">
+        <v>-4.9047529098555656E-2</v>
+      </c>
+      <c r="E11">
+        <v>1.7513686461253697E-3</v>
+      </c>
+      <c r="F11">
+        <v>46.275262365900232</v>
+      </c>
+      <c r="G11">
+        <v>1.6787276995361476E-3</v>
+      </c>
+      <c r="H11">
+        <v>2219.0273820349198</v>
+      </c>
+      <c r="P11" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q11">
+        <v>4357255.0535812248</v>
+      </c>
+      <c r="U11" t="s">
+        <v>65</v>
+      </c>
+      <c r="V11">
+        <v>2068428</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA11">
+        <v>418.91268302269799</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.16576986796408499</v>
+      </c>
+      <c r="B12">
+        <v>38.960764809123937</v>
+      </c>
+      <c r="C12">
+        <v>1.5839653023928273</v>
+      </c>
+      <c r="D12">
+        <v>-2.1263450030724589E-2</v>
+      </c>
+      <c r="E12">
+        <v>4.6546539895057871E-3</v>
+      </c>
+      <c r="F12">
+        <v>46.247927707187266</v>
+      </c>
+      <c r="G12">
+        <v>1.1857646257259068E-2</v>
+      </c>
+      <c r="H12">
+        <v>2255.5586627628541</v>
+      </c>
+      <c r="P12" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q12">
+        <v>631.96616757961476</v>
+      </c>
+      <c r="U12" t="s">
+        <v>66</v>
+      </c>
+      <c r="V12">
+        <v>3252.5</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA12">
+        <v>51.640180265284449</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.2028158415777776</v>
+      </c>
+      <c r="B13">
+        <v>39.06989969524021</v>
+      </c>
+      <c r="C13">
+        <v>3.0299288660870594</v>
+      </c>
+      <c r="D13">
+        <v>6.4188435919922029E-2</v>
+      </c>
+      <c r="E13">
+        <v>8.9037834704296936E-3</v>
+      </c>
+      <c r="F13">
+        <v>46.208259704318955</v>
+      </c>
+      <c r="G13">
+        <v>4.3387883451102109E-2</v>
+      </c>
+      <c r="H13">
+        <v>2258.6984873221718</v>
+      </c>
+      <c r="P13" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q13">
+        <v>303.5087857798336</v>
+      </c>
+      <c r="U13" t="s">
+        <v>67</v>
+      </c>
+      <c r="V13">
+        <v>1.4356</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA13">
+        <v>0.14231669665470673</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.271597956530233</v>
+      </c>
+      <c r="B14">
+        <v>39.145381637707899</v>
+      </c>
+      <c r="C14">
+        <v>5.7198439074859131</v>
+      </c>
+      <c r="D14">
+        <v>0.36507261525430001</v>
+      </c>
+      <c r="E14">
+        <v>1.6808455485390596E-2</v>
+      </c>
+      <c r="F14">
+        <v>46.134609348637277</v>
+      </c>
+      <c r="G14">
+        <v>0.16108831832808365</v>
+      </c>
+      <c r="H14">
+        <v>2258.6984956874326</v>
+      </c>
+      <c r="P14" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q14">
+        <v>1.8117532128622611</v>
+      </c>
+      <c r="U14" t="s">
+        <v>68</v>
+      </c>
+      <c r="V14">
+        <v>238.91946992864425</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA14">
+        <v>12.358079530822401</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.61550853129250982</v>
+      </c>
+      <c r="B15">
+        <v>39.502175366391363</v>
+      </c>
+      <c r="C15">
+        <v>19.24466368763596</v>
+      </c>
+      <c r="D15">
+        <v>4.6543349894213044</v>
+      </c>
+      <c r="E15">
+        <v>5.6555515916489586E-2</v>
+      </c>
+      <c r="F15">
+        <v>45.766357570228898</v>
+      </c>
+      <c r="G15">
+        <v>1.8599645282553563</v>
+      </c>
+      <c r="H15">
+        <v>2258.6986149123559</v>
+      </c>
+      <c r="P15" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q15">
+        <v>5.9693600243141349E-3</v>
+      </c>
+      <c r="U15" t="s">
+        <v>69</v>
+      </c>
+      <c r="V15">
+        <v>1632.6274728336584</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA15">
+        <v>12071.729394727032</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2.335061405103894</v>
+      </c>
+      <c r="B16">
+        <v>40.772952798473398</v>
+      </c>
+      <c r="C16">
+        <v>88.388088703770862</v>
+      </c>
+      <c r="D16">
+        <v>96.881235571553631</v>
+      </c>
+      <c r="E16">
+        <v>0.26002234005831587</v>
+      </c>
+      <c r="F16">
+        <v>43.925098678187013</v>
+      </c>
+      <c r="G16">
+        <v>36.839973507059383</v>
+      </c>
+      <c r="H16">
+        <v>2258.7011666140793</v>
+      </c>
+      <c r="O16" t="s">
+        <v>53</v>
+      </c>
+      <c r="P16">
+        <v>16.305778915760349</v>
+      </c>
+      <c r="U16" t="s">
+        <v>70</v>
+      </c>
+      <c r="V16">
+        <v>1469.3647255502926</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA16">
+        <v>16.816005383766822</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4.1350614051038939</v>
+      </c>
+      <c r="B17">
+        <v>41.100450114177377</v>
+      </c>
+      <c r="C17">
+        <v>162.23290791611572</v>
+      </c>
+      <c r="D17">
+        <v>322.35124422027565</v>
+      </c>
+      <c r="E17">
+        <v>0.47848194056669435</v>
+      </c>
+      <c r="F17">
+        <v>41.997698796420458</v>
+      </c>
+      <c r="G17">
+        <v>120.58556074605099</v>
+      </c>
+      <c r="H17">
+        <v>2258.7073102314621</v>
+      </c>
+      <c r="U17" t="s">
+        <v>71</v>
+      </c>
+      <c r="V17">
+        <v>92063</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA17">
+        <v>0.14231669665470673</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5.9350614051038937</v>
+      </c>
+      <c r="B18">
+        <v>40.322824193608007</v>
+      </c>
+      <c r="C18">
+        <v>235.69391824914695</v>
+      </c>
+      <c r="D18">
+        <v>680.69680554115621</v>
+      </c>
+      <c r="E18">
+        <v>0.69799187701224341</v>
+      </c>
+      <c r="F18">
+        <v>40.070298914653904</v>
+      </c>
+      <c r="G18">
+        <v>249.87955181558138</v>
+      </c>
+      <c r="H18">
+        <v>2258.7168026892473</v>
+      </c>
+      <c r="U18" t="s">
+        <v>72</v>
+      </c>
+      <c r="V18">
+        <v>1.1724846115020683E-2</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA18">
+        <v>3.2496725269285611</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>7.7350614051038935</v>
+      </c>
+      <c r="B19">
+        <v>38.315161464121033</v>
+      </c>
+      <c r="C19">
+        <v>306.70403277691588</v>
+      </c>
+      <c r="D19">
+        <v>1169.3895035009539</v>
+      </c>
+      <c r="E19">
+        <v>0.91341113867191481</v>
+      </c>
+      <c r="F19">
+        <v>38.142899032887343</v>
+      </c>
+      <c r="G19">
+        <v>423.09604971673178</v>
+      </c>
+      <c r="H19">
+        <v>2258.7292243841011</v>
+      </c>
+      <c r="U19" t="s">
+        <v>73</v>
+      </c>
+      <c r="V19">
+        <v>1.4473248461150208</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA19">
+        <v>12071.729394727032</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>9.5350614051038942</v>
+      </c>
+      <c r="B20">
+        <v>30.244755523827379</v>
+      </c>
+      <c r="C20">
+        <v>367.06679612561959</v>
+      </c>
+      <c r="D20">
+        <v>1778.2819083295324</v>
+      </c>
+      <c r="E20">
+        <v>1.1009740992026333</v>
+      </c>
+      <c r="F20">
+        <v>36.215499151120795</v>
+      </c>
+      <c r="G20">
+        <v>808.14092150294027</v>
+      </c>
+      <c r="H20">
+        <v>2258.7438861744617</v>
+      </c>
+      <c r="U20" t="s">
+        <v>74</v>
+      </c>
+      <c r="V20">
+        <v>2277.1673604892039</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA20">
+        <v>5.6055260105447946</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>11.335061405103895</v>
+      </c>
+      <c r="B21">
+        <v>28.50210663734336</v>
+      </c>
+      <c r="C21">
+        <v>419.63630808798342</v>
+      </c>
+      <c r="D21">
+        <v>2486.7696395429675</v>
+      </c>
+      <c r="E21">
+        <v>1.2692610102668842</v>
+      </c>
+      <c r="F21">
+        <v>34.288099269354234</v>
+      </c>
+      <c r="G21">
+        <v>945.11054300983335</v>
+      </c>
+      <c r="H21">
+        <v>2258.7598586091476</v>
+      </c>
+      <c r="U21" t="s">
+        <v>75</v>
+      </c>
+      <c r="V21">
+        <v>511.9530936351627</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA21">
+        <v>1.47402546083458</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>13.135061405103896</v>
+      </c>
+      <c r="B22">
+        <v>27.747695695118601</v>
+      </c>
+      <c r="C22">
+        <v>470.16715391488958</v>
+      </c>
+      <c r="D22">
+        <v>3287.794186771669</v>
+      </c>
+      <c r="E22">
+        <v>1.4359104150184303</v>
+      </c>
+      <c r="F22">
+        <v>32.36069938758768</v>
+      </c>
+      <c r="G22">
+        <v>1043.3832829123908</v>
+      </c>
+      <c r="H22">
+        <v>2258.7765829926198</v>
+      </c>
+      <c r="U22" t="s">
+        <v>76</v>
+      </c>
+      <c r="V22">
+        <v>7.6065640140928826E-4</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA22">
+        <v>7.079551471379375</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>14.935061405103896</v>
+      </c>
+      <c r="B23">
+        <v>27.71505127976247</v>
+      </c>
+      <c r="C23">
+        <v>519.96559268235035</v>
+      </c>
+      <c r="D23">
+        <v>4178.9418171145389</v>
+      </c>
+      <c r="E23">
+        <v>1.6055226058921335</v>
+      </c>
+      <c r="F23">
+        <v>30.433299505821125</v>
+      </c>
+      <c r="G23">
+        <v>1116.7825018613376</v>
+      </c>
+      <c r="H23">
+        <v>2258.7936264296454</v>
+      </c>
+      <c r="U23" t="s">
+        <v>77</v>
+      </c>
+      <c r="V23">
+        <v>1.1790197802239573</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z23">
+        <v>46.425430387139727</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>15.226199262184329</v>
+      </c>
+      <c r="B24">
+        <v>-46.074113436410805</v>
+      </c>
+      <c r="C24">
+        <v>518.34740226205543</v>
+      </c>
+      <c r="D24">
+        <v>4330.9171071274659</v>
+      </c>
+      <c r="E24">
+        <v>1.6035636758097158</v>
+      </c>
+      <c r="F24">
+        <v>30.121555577313018</v>
+      </c>
+      <c r="G24">
+        <v>1092.454008577588</v>
+      </c>
+      <c r="H24">
+        <v>0.1225002407562564</v>
+      </c>
+      <c r="U24" t="s">
+        <v>78</v>
+      </c>
+      <c r="V24">
+        <v>3.1120697457323307E-2</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z24">
+        <v>0.35122515353734235</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>15.517337119264761</v>
+      </c>
+      <c r="B25">
+        <v>-44.013137494932387</v>
+      </c>
+      <c r="C25">
+        <v>505.24118431357897</v>
+      </c>
+      <c r="D25">
+        <v>4479.905166059325</v>
+      </c>
+      <c r="E25">
+        <v>1.565937230813754</v>
+      </c>
+      <c r="F25">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G25">
+        <v>1030.1865805750313</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="U25" t="s">
+        <v>79</v>
+      </c>
+      <c r="V25">
+        <v>1.2252243093434374</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>16.256611577516583</v>
+      </c>
+      <c r="B26">
+        <v>-39.429143578852475</v>
+      </c>
+      <c r="C26">
+        <v>474.45564385290498</v>
+      </c>
+      <c r="D26">
+        <v>4841.8272787679143</v>
+      </c>
+      <c r="E26">
+        <v>1.4772443744661743</v>
+      </c>
+      <c r="F26">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G26">
+        <v>892.11828147578092</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="U26" t="s">
+        <v>80</v>
+      </c>
+      <c r="V26">
+        <v>1.0707777120925304</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>18.056611577516584</v>
+      </c>
+      <c r="B27">
+        <v>-31.262076787071621</v>
+      </c>
+      <c r="C27">
+        <v>411.36859760890326</v>
+      </c>
+      <c r="D27">
+        <v>5636.8604514202198</v>
+      </c>
+      <c r="E27">
+        <v>1.2939107197441004</v>
+      </c>
+      <c r="F27">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G27">
+        <v>646.12907616386519</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="U27" t="s">
+        <v>81</v>
+      </c>
+      <c r="V27">
+        <v>0.11897530134361449</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>19.856611577516585</v>
+      </c>
+      <c r="B28">
+        <v>-25.726047221107418</v>
+      </c>
+      <c r="C28">
+        <v>360.3270175052678</v>
+      </c>
+      <c r="D28">
+        <v>6329.9037263062592</v>
+      </c>
+      <c r="E28">
+        <v>1.1436537526764154</v>
+      </c>
+      <c r="F28">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G28">
+        <v>479.38579510177169</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="U28" t="s">
+        <v>82</v>
+      </c>
+      <c r="V28">
+        <v>3.9199952989143322E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>21.656611577516585</v>
+      </c>
+      <c r="B29">
+        <v>-20.683641796122636</v>
+      </c>
+      <c r="C29">
+        <v>318.20670715150982</v>
+      </c>
+      <c r="D29">
+        <v>6939.335517572601</v>
+      </c>
+      <c r="E29">
+        <v>1.0181640228842104</v>
+      </c>
+      <c r="F29">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G29">
+        <v>327.51030112383739</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="U29" t="s">
+        <v>83</v>
+      </c>
+      <c r="V29">
+        <v>0.95180241074891592</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>23.456611577516586</v>
+      </c>
+      <c r="B30">
+        <v>-16.107302931671938</v>
+      </c>
+      <c r="C30">
+        <v>285.5100577142432</v>
+      </c>
+      <c r="D30">
+        <v>7481.4552356899412</v>
+      </c>
+      <c r="E30">
+        <v>0.92024016509444562</v>
+      </c>
+      <c r="F30">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G30">
+        <v>189.67256951165442</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="U30" t="s">
+        <v>84</v>
+      </c>
+      <c r="V30">
+        <v>1.3133720475721282E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>25.256611577516587</v>
+      </c>
+      <c r="B31">
+        <v>-14.486747732818774</v>
+      </c>
+      <c r="C31">
+        <v>258.14724622905459</v>
+      </c>
+      <c r="D31">
+        <v>7970.3296595988195</v>
+      </c>
+      <c r="E31">
+        <v>0.83762071771506375</v>
+      </c>
+      <c r="F31">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G31">
+        <v>140.86201173206513</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="U31" t="s">
+        <v>85</v>
+      </c>
+      <c r="V31">
+        <v>3.042625605637153E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>27.056611577516588</v>
+      </c>
+      <c r="B32">
+        <v>-13.383385918593365</v>
+      </c>
+      <c r="C32">
+        <v>233.10306101658057</v>
+      </c>
+      <c r="D32">
+        <v>8412.1577501838219</v>
+      </c>
+      <c r="E32">
+        <v>0.76099654181156406</v>
+      </c>
+      <c r="F32">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G32">
+        <v>107.62913844076701</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="U32" t="s">
+        <v>86</v>
+      </c>
+      <c r="V32">
+        <v>4.716079120895829</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>28.856611577516588</v>
+      </c>
+      <c r="B33">
+        <v>-12.54365033809666</v>
+      </c>
+      <c r="C33">
+        <v>209.80217478102637</v>
+      </c>
+      <c r="D33">
+        <v>8810.5449988516903</v>
+      </c>
+      <c r="E33">
+        <v>0.68875793113799766</v>
+      </c>
+      <c r="F33">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G33">
+        <v>82.336595428089765</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="U33" t="s">
+        <v>87</v>
+      </c>
+      <c r="V33">
+        <v>6.2241394914646614E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>30.656611577516589</v>
+      </c>
+      <c r="B34">
+        <v>-11.885057081192393</v>
+      </c>
+      <c r="C34">
+        <v>187.8428234406976</v>
+      </c>
+      <c r="D34">
+        <v>9168.2482933946103</v>
+      </c>
+      <c r="E34">
+        <v>0.61979644662841582</v>
+      </c>
+      <c r="F34">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G34">
+        <v>62.499996068732649</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="U34" t="s">
+        <v>88</v>
+      </c>
+      <c r="V34">
+        <v>2.4504486186868748</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>32.45661157751659</v>
+      </c>
+      <c r="B35">
+        <v>-11.378938763066278</v>
+      </c>
+      <c r="C35">
+        <v>166.92553498741663</v>
+      </c>
+      <c r="D35">
+        <v>9487.4031613239567</v>
+      </c>
+      <c r="E35">
+        <v>0.55329558072510077</v>
+      </c>
+      <c r="F35">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G35">
+        <v>47.255888723493371</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="U35" t="s">
+        <v>89</v>
+      </c>
+      <c r="V35">
+        <v>15.227977507951062</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34.256611577516587</v>
+      </c>
+      <c r="B36">
+        <v>-10.982357110089087</v>
+      </c>
+      <c r="C36">
+        <v>146.81366483100896</v>
+      </c>
+      <c r="D36">
+        <v>9769.6614530380084</v>
+      </c>
+      <c r="E36">
+        <v>0.48861537568756613</v>
+      </c>
+      <c r="F36">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G36">
+        <v>35.310987555876835</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="U36" t="s">
+        <v>90</v>
+      </c>
+      <c r="V36">
+        <v>7796.0101950022217</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36.056611577516584</v>
+      </c>
+      <c r="B37">
+        <v>-10.665514868255201</v>
+      </c>
+      <c r="C37">
+        <v>127.34130738002935</v>
+      </c>
+      <c r="D37">
+        <v>10016.315446691704</v>
+      </c>
+      <c r="E37">
+        <v>0.4253292357477591</v>
+      </c>
+      <c r="F37">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G37">
+        <v>25.76780966042968</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="U37" t="s">
+        <v>91</v>
+      </c>
+      <c r="V37">
+        <v>216.7836977873514</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37.856611577516581</v>
+      </c>
+      <c r="B38">
+        <v>-10.414966756042542</v>
+      </c>
+      <c r="C38">
+        <v>108.37718570770349</v>
+      </c>
+      <c r="D38">
+        <v>10228.394593743786</v>
+      </c>
+      <c r="E38">
+        <v>0.36311152645836192</v>
+      </c>
+      <c r="F38">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G38">
+        <v>18.221387843772334</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="U38" t="s">
+        <v>92</v>
+      </c>
+      <c r="V38">
+        <v>3.4229538063417969E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>39.656611577516578</v>
+      </c>
+      <c r="B39">
+        <v>-10.217279036644451</v>
+      </c>
+      <c r="C39">
+        <v>89.815560809891721</v>
+      </c>
+      <c r="D39">
+        <v>10406.714923253061</v>
+      </c>
+      <c r="E39">
+        <v>0.30171172479294261</v>
+      </c>
+      <c r="F39">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G39">
+        <v>12.267102635329994</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="U39" t="s">
+        <v>93</v>
+      </c>
+      <c r="V39">
+        <v>2088.8145712629162</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>41.456611577516576</v>
+      </c>
+      <c r="B40">
+        <v>-10.065061952273684</v>
+      </c>
+      <c r="C40">
+        <v>71.568239314940186</v>
+      </c>
+      <c r="D40">
+        <v>10551.919307922795</v>
+      </c>
+      <c r="E40">
+        <v>0.24093083183642092</v>
+      </c>
+      <c r="F40">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G40">
+        <v>7.6823771060929467</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="U40" t="s">
+        <v>94</v>
+      </c>
+      <c r="V40">
+        <v>0.22819692042278647</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>43.256611577516573</v>
+      </c>
+      <c r="B41">
+        <v>-9.9524843596793637</v>
+      </c>
+      <c r="C41">
+        <v>53.557615189212797</v>
+      </c>
+      <c r="D41">
+        <v>10664.502118560522</v>
+      </c>
+      <c r="E41">
+        <v>0.1806001990323525</v>
+      </c>
+      <c r="F41">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G41">
+        <v>4.2915792536650841</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="U41" t="s">
+        <v>95</v>
+      </c>
+      <c r="V41">
+        <v>353.70593406718717</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>45.05661157751657</v>
+      </c>
+      <c r="B42">
+        <v>-9.8737427626738388</v>
+      </c>
+      <c r="C42">
+        <v>35.718943557585348</v>
+      </c>
+      <c r="D42">
+        <v>10744.829742179767</v>
+      </c>
+      <c r="E42">
+        <v>0.12059084306700742</v>
+      </c>
+      <c r="F42">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G42">
+        <v>1.9199097955588336</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="U42" t="s">
+        <v>96</v>
+      </c>
+      <c r="V42">
+        <v>21.221507544513205</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>46.856611577516567</v>
+      </c>
+      <c r="B43">
+        <v>-9.8264416060948321</v>
+      </c>
+      <c r="C43">
+        <v>17.993399155439821</v>
+      </c>
+      <c r="D43">
+        <v>10793.158080358351</v>
+      </c>
+      <c r="E43">
+        <v>6.0791327641775958E-2</v>
+      </c>
+      <c r="F43">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G43">
+        <v>0.495215445206037</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="U43" t="s">
+        <v>97</v>
+      </c>
+      <c r="V43">
+        <v>5.8381244740097324</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>48.656611577516564</v>
+      </c>
+      <c r="B44">
+        <v>-9.8100050554196194</v>
+      </c>
+      <c r="C44">
+        <v>0.3253497082337411</v>
+      </c>
+      <c r="D44">
+        <v>10809.640491109594</v>
+      </c>
+      <c r="E44">
+        <v>1.0994755628840724E-3</v>
+      </c>
+      <c r="F44">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G44">
+        <v>1.5226747694900043E-4</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="U44" t="s">
+        <v>98</v>
+      </c>
+      <c r="V44">
+        <v>2.2862996865690977</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>49.199481150986415</v>
+      </c>
+      <c r="B45">
+        <v>-9.8087552087578285</v>
+      </c>
+      <c r="C45">
+        <v>-4.999999999999968</v>
+      </c>
+      <c r="D45">
+        <v>10808.371596590925</v>
+      </c>
+      <c r="E45">
+        <v>1.6896507451995363E-2</v>
+      </c>
+      <c r="F45">
+        <v>30.119651471379377</v>
+      </c>
+      <c r="G45">
+        <v>-3.7492678368827435E-2</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J21"/>
+  <dimension ref="A2:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8056,7 +9774,7 @@
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>146</v>
       </c>
@@ -8067,7 +9785,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -8078,7 +9796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -8089,7 +9807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -8100,7 +9818,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>126</v>
       </c>
@@ -8111,7 +9829,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -8122,7 +9840,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>123</v>
       </c>
@@ -8136,7 +9854,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>122</v>
       </c>
@@ -8147,7 +9865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -8159,7 +9877,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -8170,7 +9888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -8182,7 +9900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -8193,96 +9911,96 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G14" t="str">
-        <f>IF(F15="Single value","Value",IF(F15="Range of values","Start",IF(F15="Monte Carlo","Mean","ERROR")))</f>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C30" t="str">
+        <f>IF(B31="Single value","Value",IF(B31="Range of values","Start",IF(B31="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
       </c>
-      <c r="H14" t="str">
-        <f>IF(F15="Single value","",IF(F15="Range of values","Step",IF(F15="Monte Carlo","Standard deviation","ERROR")))</f>
+      <c r="D30" t="str">
+        <f>IF(B31="Single value","",IF(B31="Range of values","Step",IF(B31="Monte Carlo","Standard deviation","ERROR")))</f>
         <v/>
       </c>
-      <c r="I14" t="str">
-        <f>IF(F15="Single value","",IF(F15="Range of values","End",IF(F15="Monte Carlo","","ERROR")))</f>
+      <c r="E30" t="str">
+        <f>IF(B31="Single value","",IF(B31="Range of values","End",IF(B31="Monte Carlo","","ERROR")))</f>
         <v/>
       </c>
-      <c r="J14" t="s">
+      <c r="F30" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="3">
+      <c r="C31" s="3">
         <f>SUM(B:B)</f>
         <v>23.040136054421769</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" t="s">
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="G17" t="str">
-        <f>IF(F18="Single value","Value",IF(F18="Range of values","Start",IF(F18="Monte Carlo","Mean","ERROR")))</f>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C33" t="str">
+        <f>IF(B34="Single value","Value",IF(B34="Range of values","Start",IF(B34="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
       </c>
-      <c r="H17" t="str">
-        <f>IF(F18="Single value","",IF(F18="Range of values","Step",IF(F18="Monte Carlo","Standard deviation","ERROR")))</f>
+      <c r="D33" t="str">
+        <f>IF(B34="Single value","",IF(B34="Range of values","Step",IF(B34="Monte Carlo","Standard deviation","ERROR")))</f>
         <v/>
       </c>
-      <c r="I17" t="str">
-        <f>IF(F18="Single value","",IF(F18="Range of values","End",IF(F18="Monte Carlo","","ERROR")))</f>
+      <c r="E33" t="str">
+        <f>IF(B34="Single value","",IF(B34="Range of values","End",IF(B34="Monte Carlo","","ERROR")))</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E18" s="1" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="1">
+      <c r="C34" s="1">
         <v>6</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" t="s">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="G20" t="str">
-        <f>IF(F21="Single value","Value",IF(F21="Range of values","Start",IF(F21="Monte Carlo","Mean","ERROR")))</f>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C36" t="str">
+        <f>IF(B37="Single value","Value",IF(B37="Range of values","Start",IF(B37="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
       </c>
-      <c r="H20" t="str">
-        <f>IF(F21="Single value","",IF(F21="Range of values","Step",IF(F21="Monte Carlo","Standard deviation","ERROR")))</f>
+      <c r="D36" t="str">
+        <f>IF(B37="Single value","",IF(B37="Range of values","Step",IF(B37="Monte Carlo","Standard deviation","ERROR")))</f>
         <v/>
       </c>
-      <c r="I20" t="str">
-        <f>IF(F21="Single value","",IF(F21="Range of values","End",IF(F21="Monte Carlo","","ERROR")))</f>
+      <c r="E36" t="str">
+        <f>IF(B37="Single value","",IF(B37="Range of values","End",IF(B37="Monte Carlo","","ERROR")))</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E21" s="1" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="1">
+      <c r="C37" s="1">
         <v>5</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8294,7 +10012,7 @@
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F15 F18 F21 B25</xm:sqref>
+          <xm:sqref>B31 B34 B37 B25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8593,10 +10311,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8605,12 +10323,12 @@
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -8621,7 +10339,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -8632,12 +10350,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C5" t="str">
         <f>IF(B6="Single value","Value",IF(B6="Range of values","Start",IF(B6="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
@@ -8653,105 +10371,164 @@
       <c r="F5" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>139</v>
+      </c>
+      <c r="N5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1">
-        <v>1593</v>
+      <c r="C6" s="9">
+        <f>$N$6*J6</f>
+        <v>2.6104650300000001E-2</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" t="s">
+        <v>151</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1593</v>
+      </c>
+      <c r="K6" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="N6" s="6">
+        <v>1.6387100000000001E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1">
-        <v>465.5</v>
+      <c r="C8" s="9">
+        <f>$N$6*J8</f>
+        <v>7.6281950500000006E-3</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" t="s">
+        <v>151</v>
+      </c>
+      <c r="J8" s="1">
+        <v>465.5</v>
+      </c>
+      <c r="K8" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="4">
-        <f>93.19</f>
-        <v>93.19</v>
+      <c r="C10" s="9">
+        <f>$N$6*J10</f>
+        <v>1.5271138490000002E-3</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="1"/>
       <c r="F10" t="s">
+        <v>151</v>
+      </c>
+      <c r="J10" s="4">
+        <f>93.19</f>
+        <v>93.19</v>
+      </c>
+      <c r="K10" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>138</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="4">
-        <v>5.625</v>
+      <c r="C12" s="9">
+        <f>$N$12*J12</f>
+        <v>0.142875</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="4">
+        <v>5.625</v>
+      </c>
+      <c r="K12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>2.5399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>142</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="1">
-        <v>5.9089999999999998</v>
+      <c r="C14" s="9">
+        <f>$N$12*J14</f>
+        <v>0.15008859999999999</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="J14" s="1">
+        <v>5.9089999999999998</v>
+      </c>
+      <c r="K14" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="1">
-        <v>0.28399999999999997</v>
+      <c r="C16" s="9">
+        <f>$N$12*J16</f>
+        <v>7.2135999999999988E-3</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="J16" s="1">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="K16" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -8771,7 +10548,7 @@
         <v>9</v>
       </c>
       <c r="C20" s="8">
-        <f>(C6-(2*C10))/(PI()*(C12/2)^2)</f>
+        <f>(J6-(2*J10))/(PI()*(J12/2)^2)</f>
         <v>56.603313253621714</v>
       </c>
       <c r="D20" s="1"/>
@@ -8793,7 +10570,7 @@
         <v>9</v>
       </c>
       <c r="C23" s="8">
-        <f>(C8-C10)/(PI()*(C12/2)^2)</f>
+        <f>(J8-J10)/(PI()*(J12/2)^2)</f>
         <v>14.981999088208545</v>
       </c>
       <c r="D23" s="1"/>
@@ -8810,7 +10587,7 @@
         <v>9</v>
       </c>
       <c r="C25" s="7">
-        <f>C6*0.026157</f>
+        <f>J6*0.026157</f>
         <v>41.668101</v>
       </c>
       <c r="D25" s="4"/>
@@ -8827,7 +10604,7 @@
         <v>9</v>
       </c>
       <c r="C27" s="7">
-        <f>C8*0.010937</f>
+        <f>J8*0.010937</f>
         <v>5.0911735</v>
       </c>
       <c r="D27" s="4"/>
@@ -8840,7 +10617,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>

</xml_diff>

<commit_message>
Made the Monte Carlo stuff cleaner
Moved the monte carlo stuff into functions to make launch control cleaner
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" tabRatio="882" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" tabRatio="882" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
@@ -9761,8 +9761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9999,7 +9999,9 @@
       <c r="C37" s="1">
         <v>5</v>
       </c>
-      <c r="D37" s="1"/>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
       <c r="E37" s="1"/>
     </row>
   </sheetData>
@@ -10313,7 +10315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Basic Monte Carlo output
Monte Carlo now computes a histogram for maximum altitude. Techically useable now, but only barely.
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -21,13 +21,15 @@
     <sheet name="Results 27-Aug-2017 14-35-18" sheetId="15" r:id="rId12"/>
     <sheet name="Results 27-Aug-2017 14-35-43" sheetId="16" r:id="rId13"/>
     <sheet name="Results 17-Sep-2017 13-34-09" sheetId="17" r:id="rId14"/>
+    <sheet name="Results 17-Sep-2017 14-28-17" sheetId="18" r:id="rId15"/>
+    <sheet name="Results 17-Sep-2017 14-30-28" sheetId="19" r:id="rId16"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="154">
   <si>
     <t>Total inert mass</t>
   </si>
@@ -9757,12 +9759,3738 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2:AA24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>-9.8077912979337363</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>53.737018790651931</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0.11868906443783601</v>
+      </c>
+      <c r="K2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2">
+        <v>46964.380599746386</v>
+      </c>
+      <c r="O2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" t="s">
+        <v>57</v>
+      </c>
+      <c r="V2">
+        <v>300</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z2">
+        <v>32.453900860855732</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1.2927625756433149E-4</v>
+      </c>
+      <c r="B3">
+        <v>-9.8077625538079936</v>
+      </c>
+      <c r="C3">
+        <v>-1.267912700009145E-3</v>
+      </c>
+      <c r="D3">
+        <v>-8.1955544419449058E-8</v>
+      </c>
+      <c r="E3">
+        <v>3.7259000016658353E-6</v>
+      </c>
+      <c r="F3">
+        <v>53.736858563643331</v>
+      </c>
+      <c r="G3">
+        <v>-7.5977496586787575E-9</v>
+      </c>
+      <c r="H3">
+        <v>0.12023332196588275</v>
+      </c>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3">
+        <v>1.9100662847745531</v>
+      </c>
+      <c r="P3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" t="s">
+        <v>58</v>
+      </c>
+      <c r="V3">
+        <v>4</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>7.7565754538598888E-4</v>
+      </c>
+      <c r="B4">
+        <v>-9.8076131197978125</v>
+      </c>
+      <c r="C4">
+        <v>-7.6074191152028653E-3</v>
+      </c>
+      <c r="D4">
+        <v>-2.9503849512409596E-6</v>
+      </c>
+      <c r="E4">
+        <v>2.2355232259197035E-5</v>
+      </c>
+      <c r="F4">
+        <v>53.736057428600333</v>
+      </c>
+      <c r="G4">
+        <v>-2.7351488294879236E-7</v>
+      </c>
+      <c r="H4">
+        <v>0.12826125810512462</v>
+      </c>
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4">
+        <v>4.2279193995071358</v>
+      </c>
+      <c r="P4" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q4">
+        <v>2.6105E-2</v>
+      </c>
+      <c r="U4" t="s">
+        <v>59</v>
+      </c>
+      <c r="V4">
+        <v>0.9</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4.0075639844942756E-3</v>
+      </c>
+      <c r="B5">
+        <v>-9.8067021435395496</v>
+      </c>
+      <c r="C5">
+        <v>-3.9303314216520127E-2</v>
+      </c>
+      <c r="D5">
+        <v>-7.8756727076969679E-5</v>
+      </c>
+      <c r="E5">
+        <v>1.1549708301983543E-4</v>
+      </c>
+      <c r="F5">
+        <v>53.732051753385349</v>
+      </c>
+      <c r="G5">
+        <v>-7.3007020691739814E-6</v>
+      </c>
+      <c r="H5">
+        <v>0.17719329330612149</v>
+      </c>
+      <c r="K5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5">
+        <v>277.07370707650551</v>
+      </c>
+      <c r="P5" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q5">
+        <v>18.918327048707731</v>
+      </c>
+      <c r="U5" t="s">
+        <v>53</v>
+      </c>
+      <c r="V5">
+        <v>3</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2.0167096180035708E-2</v>
+      </c>
+      <c r="B6">
+        <v>-9.7933985270463353</v>
+      </c>
+      <c r="C6">
+        <v>-0.19769530261646528</v>
+      </c>
+      <c r="D6">
+        <v>-1.9939277736046404E-3</v>
+      </c>
+      <c r="E6">
+        <v>5.8094923394804159E-4</v>
+      </c>
+      <c r="F6">
+        <v>53.712023377310416</v>
+      </c>
+      <c r="G6">
+        <v>-1.8471367947272326E-4</v>
+      </c>
+      <c r="H6">
+        <v>0.89151398970559792</v>
+      </c>
+      <c r="K6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6">
+        <v>864.56508502112433</v>
+      </c>
+      <c r="P6" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q6">
+        <v>5887436.804562035</v>
+      </c>
+      <c r="U6" t="s">
+        <v>60</v>
+      </c>
+      <c r="V6">
+        <v>300</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z6">
+        <v>1.8241469247509919E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5.0193414275433001E-2</v>
+      </c>
+      <c r="B7">
+        <v>-9.4776570054937466</v>
+      </c>
+      <c r="C7">
+        <v>-0.4890847162890341</v>
+      </c>
+      <c r="D7">
+        <v>-1.2325530476494321E-2</v>
+      </c>
+      <c r="E7">
+        <v>1.437228676623566E-3</v>
+      </c>
+      <c r="F7">
+        <v>53.674808290655484</v>
+      </c>
+      <c r="G7">
+        <v>-1.1305114691530782E-3</v>
+      </c>
+      <c r="H7">
+        <v>17.837316005396374</v>
+      </c>
+      <c r="P7" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q7">
+        <v>853.90017992824039</v>
+      </c>
+      <c r="U7" t="s">
+        <v>61</v>
+      </c>
+      <c r="V7">
+        <v>45</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7.4181163493733826E-2</v>
+      </c>
+      <c r="B8">
+        <v>-6.3831947930205857</v>
+      </c>
+      <c r="C8">
+        <v>-0.69221630572312165</v>
+      </c>
+      <c r="D8">
+        <v>-2.6631639443629708E-2</v>
+      </c>
+      <c r="E8">
+        <v>2.0341526352147719E-3</v>
+      </c>
+      <c r="F8">
+        <v>53.645077500387444</v>
+      </c>
+      <c r="G8">
+        <v>-2.2645975682007743E-3</v>
+      </c>
+      <c r="H8">
+        <v>183.82896630957376</v>
+      </c>
+      <c r="P8" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q8">
+        <v>724.70128514490443</v>
+      </c>
+      <c r="U8" t="s">
+        <v>62</v>
+      </c>
+      <c r="V8">
+        <v>8</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA8">
+        <v>3.0020749999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9.8168912712034651E-2</v>
+      </c>
+      <c r="B9">
+        <v>12.345303705032707</v>
+      </c>
+      <c r="C9">
+        <v>-0.66771155223550616</v>
+      </c>
+      <c r="D9">
+        <v>-4.3842238455975062E-2</v>
+      </c>
+      <c r="E9">
+        <v>1.9621423804388784E-3</v>
+      </c>
+      <c r="F9">
+        <v>53.615346710119397</v>
+      </c>
+      <c r="G9">
+        <v>-2.1071035750547906E-3</v>
+      </c>
+      <c r="H9">
+        <v>1187.8621825097464</v>
+      </c>
+      <c r="O9" t="s">
+        <v>54</v>
+      </c>
+      <c r="U9" t="s">
+        <v>63</v>
+      </c>
+      <c r="V9">
+        <v>45</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA9">
+        <v>8.9602332474964276E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.11929116538065165</v>
+      </c>
+      <c r="B10">
+        <v>32.787872632822051</v>
+      </c>
+      <c r="C10">
+        <v>-0.16331444965731223</v>
+      </c>
+      <c r="D10">
+        <v>-5.3393064528390849E-2</v>
+      </c>
+      <c r="E10">
+        <v>4.7991706511387995E-4</v>
+      </c>
+      <c r="F10">
+        <v>53.589167460938313</v>
+      </c>
+      <c r="G10">
+        <v>-1.2605431750961838E-4</v>
+      </c>
+      <c r="H10">
+        <v>2282.7844039457045</v>
+      </c>
+      <c r="P10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>30</v>
+      </c>
+      <c r="R10" t="s">
+        <v>150</v>
+      </c>
+      <c r="U10" t="s">
+        <v>64</v>
+      </c>
+      <c r="V10">
+        <v>15</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA10">
+        <v>1831.9745409498933</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.14024205540898918</v>
+      </c>
+      <c r="B11">
+        <v>38.142678623492507</v>
+      </c>
+      <c r="C11">
+        <v>0.59598417941665061</v>
+      </c>
+      <c r="D11">
+        <v>-4.9047600796110598E-2</v>
+      </c>
+      <c r="E11">
+        <v>1.7513636598513235E-3</v>
+      </c>
+      <c r="F11">
+        <v>53.563200601284549</v>
+      </c>
+      <c r="G11">
+        <v>1.67871814064406E-3</v>
+      </c>
+      <c r="H11">
+        <v>2568.5006231971997</v>
+      </c>
+      <c r="P11" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q11">
+        <v>7.7915071717360252E-3</v>
+      </c>
+      <c r="U11" t="s">
+        <v>65</v>
+      </c>
+      <c r="V11">
+        <v>2068428</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA11">
+        <v>546.78577951537659</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.16576992529052567</v>
+      </c>
+      <c r="B12">
+        <v>38.960727251071539</v>
+      </c>
+      <c r="C12">
+        <v>1.5839627990373799</v>
+      </c>
+      <c r="D12">
+        <v>-2.1263561117739846E-2</v>
+      </c>
+      <c r="E12">
+        <v>4.6546466331182194E-3</v>
+      </c>
+      <c r="F12">
+        <v>53.531560961461288</v>
+      </c>
+      <c r="G12">
+        <v>1.1857608776918169E-2</v>
+      </c>
+      <c r="H12">
+        <v>2610.7850165843142</v>
+      </c>
+      <c r="P12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q12">
+        <v>2.3647908810884664</v>
+      </c>
+      <c r="U12" t="s">
+        <v>66</v>
+      </c>
+      <c r="V12">
+        <v>3252.5</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA12">
+        <v>66.792845291262523</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.20281596178802641</v>
+      </c>
+      <c r="B13">
+        <v>39.069954535397791</v>
+      </c>
+      <c r="C13">
+        <v>3.0299289531513907</v>
+      </c>
+      <c r="D13">
+        <v>6.4188414534183058E-2</v>
+      </c>
+      <c r="E13">
+        <v>8.9037837262757793E-3</v>
+      </c>
+      <c r="F13">
+        <v>53.485645526405413</v>
+      </c>
+      <c r="G13">
+        <v>4.3387885944673577E-2</v>
+      </c>
+      <c r="H13">
+        <v>2614.4193095130436</v>
+      </c>
+      <c r="P13" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q13">
+        <v>4357255.0535812248</v>
+      </c>
+      <c r="U13" t="s">
+        <v>67</v>
+      </c>
+      <c r="V13">
+        <v>1.4356</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA13">
+        <v>0.14231669665470673</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.27159827498415007</v>
+      </c>
+      <c r="B14">
+        <v>39.145783922735184</v>
+      </c>
+      <c r="C14">
+        <v>5.719866076281459</v>
+      </c>
+      <c r="D14">
+        <v>0.36507408947003211</v>
+      </c>
+      <c r="E14">
+        <v>1.6808520631366213E-2</v>
+      </c>
+      <c r="F14">
+        <v>53.400395655349378</v>
+      </c>
+      <c r="G14">
+        <v>0.1610896289032433</v>
+      </c>
+      <c r="H14">
+        <v>2614.4193207207541</v>
+      </c>
+      <c r="P14" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q14">
+        <v>631.96616757961476</v>
+      </c>
+      <c r="U14" t="s">
+        <v>68</v>
+      </c>
+      <c r="V14">
+        <v>238.91946992864425</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA14">
+        <v>16.321321753211024</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.61550984096476835</v>
+      </c>
+      <c r="B15">
+        <v>39.507629901115472</v>
+      </c>
+      <c r="C15">
+        <v>19.245577403494039</v>
+      </c>
+      <c r="D15">
+        <v>4.6544599608515602</v>
+      </c>
+      <c r="E15">
+        <v>5.6558201191065055E-2</v>
+      </c>
+      <c r="F15">
+        <v>52.974146300069179</v>
+      </c>
+      <c r="G15">
+        <v>1.8601389068137313</v>
+      </c>
+      <c r="H15">
+        <v>2614.4194804611711</v>
+      </c>
+      <c r="P15" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q15">
+        <v>303.5087857798336</v>
+      </c>
+      <c r="U15" t="s">
+        <v>69</v>
+      </c>
+      <c r="V15">
+        <v>1632.6274728336584</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA15">
+        <v>12071.729394727032</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2.3350676708678595</v>
+      </c>
+      <c r="B16">
+        <v>40.885651191846868</v>
+      </c>
+      <c r="C16">
+        <v>88.471053010922063</v>
+      </c>
+      <c r="D16">
+        <v>96.927309799530477</v>
+      </c>
+      <c r="E16">
+        <v>0.26026654212654726</v>
+      </c>
+      <c r="F16">
+        <v>50.842899523668208</v>
+      </c>
+      <c r="G16">
+        <v>36.90900105573791</v>
+      </c>
+      <c r="H16">
+        <v>2614.4229008897387</v>
+      </c>
+      <c r="O16" t="s">
+        <v>53</v>
+      </c>
+      <c r="P16">
+        <v>21.283117929796198</v>
+      </c>
+      <c r="U16" t="s">
+        <v>70</v>
+      </c>
+      <c r="V16">
+        <v>1469.3647255502926</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA16">
+        <v>21.338591027161645</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4.1350676708678593</v>
+      </c>
+      <c r="B17">
+        <v>41.475889309165005</v>
+      </c>
+      <c r="C17">
+        <v>162.73281170778512</v>
+      </c>
+      <c r="D17">
+        <v>322.85095564515456</v>
+      </c>
+      <c r="E17">
+        <v>0.47995905773358716</v>
+      </c>
+      <c r="F17">
+        <v>48.611951467831119</v>
+      </c>
+      <c r="G17">
+        <v>121.32398628143252</v>
+      </c>
+      <c r="H17">
+        <v>2614.4311483631209</v>
+      </c>
+      <c r="U17" t="s">
+        <v>71</v>
+      </c>
+      <c r="V17">
+        <v>92063</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA17">
+        <v>0.14231669665470673</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5.9350676708678591</v>
+      </c>
+      <c r="B18">
+        <v>41.099769709888847</v>
+      </c>
+      <c r="C18">
+        <v>237.21022552752751</v>
+      </c>
+      <c r="D18">
+        <v>682.90287959451564</v>
+      </c>
+      <c r="E18">
+        <v>0.70250007265466463</v>
+      </c>
+      <c r="F18">
+        <v>46.381003411994023</v>
+      </c>
+      <c r="G18">
+        <v>253.19772248768462</v>
+      </c>
+      <c r="H18">
+        <v>2614.4439251058693</v>
+      </c>
+      <c r="U18" t="s">
+        <v>72</v>
+      </c>
+      <c r="V18">
+        <v>1.1724846115020683E-2</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA18">
+        <v>4.4325735113785898</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>7.735067670867859</v>
+      </c>
+      <c r="B19">
+        <v>39.39440721349758</v>
+      </c>
+      <c r="C19">
+        <v>310.00321680181412</v>
+      </c>
+      <c r="D19">
+        <v>1175.8390820170303</v>
+      </c>
+      <c r="E19">
+        <v>0.9233055962783604</v>
+      </c>
+      <c r="F19">
+        <v>44.150055356156926</v>
+      </c>
+      <c r="G19">
+        <v>442.08340268117257</v>
+      </c>
+      <c r="H19">
+        <v>2614.460704923978</v>
+      </c>
+      <c r="U19" t="s">
+        <v>73</v>
+      </c>
+      <c r="V19">
+        <v>1.4473248461150208</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA19">
+        <v>12071.729394727032</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>9.503446508989958</v>
+      </c>
+      <c r="B20">
+        <v>32.694573676337711</v>
+      </c>
+      <c r="C20">
+        <v>372.50406278211403</v>
+      </c>
+      <c r="D20">
+        <v>1781.2366794489831</v>
+      </c>
+      <c r="E20">
+        <v>1.1173213403125017</v>
+      </c>
+      <c r="F20">
+        <v>41.958299061216955</v>
+      </c>
+      <c r="G20">
+        <v>831.0606129055767</v>
+      </c>
+      <c r="H20">
+        <v>2614.4802266868842</v>
+      </c>
+      <c r="U20" t="s">
+        <v>74</v>
+      </c>
+      <c r="V20">
+        <v>2635.8007716814773</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA20">
+        <v>7.4032209766824941</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>11.303446508989959</v>
+      </c>
+      <c r="B21">
+        <v>31.29192208938256</v>
+      </c>
+      <c r="C21">
+        <v>429.87720830998353</v>
+      </c>
+      <c r="D21">
+        <v>2503.7431171989729</v>
+      </c>
+      <c r="E21">
+        <v>1.3005001378925525</v>
+      </c>
+      <c r="F21">
+        <v>39.727351005379859</v>
+      </c>
+      <c r="G21">
+        <v>981.63154213403072</v>
+      </c>
+      <c r="H21">
+        <v>2614.5020279747077</v>
+      </c>
+      <c r="U21" t="s">
+        <v>75</v>
+      </c>
+      <c r="V21">
+        <v>592.58110874133922</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA21">
+        <v>2.0105798841732372</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>13.103446508989959</v>
+      </c>
+      <c r="B22">
+        <v>30.717596443922417</v>
+      </c>
+      <c r="C22">
+        <v>485.6101317711437</v>
+      </c>
+      <c r="D22">
+        <v>3327.8379963220764</v>
+      </c>
+      <c r="E22">
+        <v>1.4837979384511213</v>
+      </c>
+      <c r="F22">
+        <v>37.49640294954277</v>
+      </c>
+      <c r="G22">
+        <v>1094.8859264552373</v>
+      </c>
+      <c r="H22">
+        <v>2614.5250132930091</v>
+      </c>
+      <c r="U22" t="s">
+        <v>76</v>
+      </c>
+      <c r="V22">
+        <v>8.8045295423009077E-4</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA22">
+        <v>9.4138008608557318</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>14.90344650898996</v>
+      </c>
+      <c r="B23">
+        <v>30.78616506191095</v>
+      </c>
+      <c r="C23">
+        <v>540.86773333256019</v>
+      </c>
+      <c r="D23">
+        <v>4251.6323108320721</v>
+      </c>
+      <c r="E23">
+        <v>1.6715769334284727</v>
+      </c>
+      <c r="F23">
+        <v>35.26545489370568</v>
+      </c>
+      <c r="G23">
+        <v>1182.9063174766882</v>
+      </c>
+      <c r="H23">
+        <v>2614.5485453249394</v>
+      </c>
+      <c r="U23" t="s">
+        <v>77</v>
+      </c>
+      <c r="V23">
+        <v>1.3647048084662576</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z23">
+        <v>53.737018790651931</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>16.703446508989959</v>
+      </c>
+      <c r="B24">
+        <v>32.11927527460405</v>
+      </c>
+      <c r="C24">
+        <v>597.2087865858515</v>
+      </c>
+      <c r="D24">
+        <v>5275.5408889114688</v>
+      </c>
+      <c r="E24">
+        <v>1.8697393776984526</v>
+      </c>
+      <c r="F24">
+        <v>33.034506837868584</v>
+      </c>
+      <c r="G24">
+        <v>1229.4591348585516</v>
+      </c>
+      <c r="H24">
+        <v>2614.5720656243334</v>
+      </c>
+      <c r="U24" t="s">
+        <v>78</v>
+      </c>
+      <c r="V24">
+        <v>3.3481749037418129E-2</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z24">
+        <v>0.39606063769020622</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>16.910570229076576</v>
+      </c>
+      <c r="B25">
+        <v>32.389892579251153</v>
+      </c>
+      <c r="C25">
+        <v>603.89063214461294</v>
+      </c>
+      <c r="D25">
+        <v>5399.9280999914481</v>
+      </c>
+      <c r="E25">
+        <v>1.893676874471854</v>
+      </c>
+      <c r="F25">
+        <v>32.777794470843588</v>
+      </c>
+      <c r="G25">
+        <v>1231.355343927984</v>
+      </c>
+      <c r="H25">
+        <v>2614.5747495823557</v>
+      </c>
+      <c r="U25" t="s">
+        <v>79</v>
+      </c>
+      <c r="V25">
+        <v>1.3181790959613437</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>17.056344586235362</v>
+      </c>
+      <c r="B26">
+        <v>18.605894766498089</v>
+      </c>
+      <c r="C26">
+        <v>608.42542046287576</v>
+      </c>
+      <c r="D26">
+        <v>5488.3047523584919</v>
+      </c>
+      <c r="E26">
+        <v>1.9100662847745531</v>
+      </c>
+      <c r="F26">
+        <v>32.597119460457876</v>
+      </c>
+      <c r="G26">
+        <v>1232.5342841481561</v>
+      </c>
+      <c r="H26">
+        <v>2158.8106004274941</v>
+      </c>
+      <c r="U26" t="s">
+        <v>80</v>
+      </c>
+      <c r="V26">
+        <v>1.2394155865761627</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>17.202118943394147</v>
+      </c>
+      <c r="B27">
+        <v>-46.870015201803916</v>
+      </c>
+      <c r="C27">
+        <v>602.70752823196938</v>
+      </c>
+      <c r="D27">
+        <v>5576.6521215743205</v>
+      </c>
+      <c r="E27">
+        <v>1.8942712547979834</v>
+      </c>
+      <c r="F27">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G27">
+        <v>1202.7420592611506</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="U27" t="s">
+        <v>81</v>
+      </c>
+      <c r="V27">
+        <v>0.13771284295290698</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>17.373460836350826</v>
+      </c>
+      <c r="B28">
+        <v>-45.733303249099436</v>
+      </c>
+      <c r="C28">
+        <v>594.77556814531465</v>
+      </c>
+      <c r="D28">
+        <v>5679.2387915255722</v>
+      </c>
+      <c r="E28">
+        <v>1.8718207166426761</v>
+      </c>
+      <c r="F28">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G28">
+        <v>1165.8513222407296</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="U28" t="s">
+        <v>82</v>
+      </c>
+      <c r="V28">
+        <v>4.5373593584471848E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>18.037531039975594</v>
+      </c>
+      <c r="B29">
+        <v>-41.69138110803349</v>
+      </c>
+      <c r="C29">
+        <v>565.78312242040852</v>
+      </c>
+      <c r="D29">
+        <v>6064.4370110113141</v>
+      </c>
+      <c r="E29">
+        <v>1.7895178955290192</v>
+      </c>
+      <c r="F29">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G29">
+        <v>1034.6751817872778</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="U29" t="s">
+        <v>83</v>
+      </c>
+      <c r="V29">
+        <v>1.1017027436232558</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>19.452137410531339</v>
+      </c>
+      <c r="B30">
+        <v>-34.595837642179312</v>
+      </c>
+      <c r="C30">
+        <v>512.03882601297448</v>
+      </c>
+      <c r="D30">
+        <v>6825.5995756684415</v>
+      </c>
+      <c r="E30">
+        <v>1.6358813547761384</v>
+      </c>
+      <c r="F30">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G30">
+        <v>804.39711759255351</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="U30" t="s">
+        <v>84</v>
+      </c>
+      <c r="V30">
+        <v>1.5202163514902139E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>21.25213741053134</v>
+      </c>
+      <c r="B31">
+        <v>-28.261666814553486</v>
+      </c>
+      <c r="C31">
+        <v>455.82766095248297</v>
+      </c>
+      <c r="D31">
+        <v>7694.9849689429857</v>
+      </c>
+      <c r="E31">
+        <v>1.4734737590132565</v>
+      </c>
+      <c r="F31">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G31">
+        <v>598.8285655170605</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="U31" t="s">
+        <v>85</v>
+      </c>
+      <c r="V31">
+        <v>3.5218118169203631E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>23.052137410531341</v>
+      </c>
+      <c r="B32">
+        <v>-23.884588947937846</v>
+      </c>
+      <c r="C32">
+        <v>409.13128255754532</v>
+      </c>
+      <c r="D32">
+        <v>8472.2675877965321</v>
+      </c>
+      <c r="E32">
+        <v>1.3367835559465349</v>
+      </c>
+      <c r="F32">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G32">
+        <v>456.77531437367065</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="U32" t="s">
+        <v>86</v>
+      </c>
+      <c r="V32">
+        <v>5.4588192338650305</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>24.852137410531341</v>
+      </c>
+      <c r="B33">
+        <v>-20.727766842799369</v>
+      </c>
+      <c r="C33">
+        <v>369.12358717746218</v>
+      </c>
+      <c r="D33">
+        <v>9171.8447226932258</v>
+      </c>
+      <c r="E33">
+        <v>1.2180033514885484</v>
+      </c>
+      <c r="F33">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G33">
+        <v>354.32412273814867</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="U33" t="s">
+        <v>87</v>
+      </c>
+      <c r="V33">
+        <v>6.6963498074836258E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>26.652137410531342</v>
+      </c>
+      <c r="B34">
+        <v>-18.281792048072234</v>
+      </c>
+      <c r="C34">
+        <v>334.08386769182437</v>
+      </c>
+      <c r="D34">
+        <v>9804.0705657555609</v>
+      </c>
+      <c r="E34">
+        <v>1.1124293896336017</v>
+      </c>
+      <c r="F34">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G34">
+        <v>274.94269924192224</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="U34" t="s">
+        <v>88</v>
+      </c>
+      <c r="V34">
+        <v>2.6363581919226875</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>28.452137410531343</v>
+      </c>
+      <c r="B35">
+        <v>-15.882874695346633</v>
+      </c>
+      <c r="C35">
+        <v>303.15823178571509</v>
+      </c>
+      <c r="D35">
+        <v>10376.968961663251</v>
+      </c>
+      <c r="E35">
+        <v>1.0179340621748745</v>
+      </c>
+      <c r="F35">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G35">
+        <v>197.08847330317909</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="U35" t="s">
+        <v>89</v>
+      </c>
+      <c r="V35">
+        <v>17.171897917299866</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>30.252137410531343</v>
+      </c>
+      <c r="B36">
+        <v>-13.620681138868854</v>
+      </c>
+      <c r="C36">
+        <v>276.76593600063137</v>
+      </c>
+      <c r="D36">
+        <v>10898.29171636667</v>
+      </c>
+      <c r="E36">
+        <v>0.93653245577495126</v>
+      </c>
+      <c r="F36">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G36">
+        <v>123.67146789318255</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="U36" t="s">
+        <v>90</v>
+      </c>
+      <c r="V36">
+        <v>10175.742307026649</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>32.052137410531344</v>
+      </c>
+      <c r="B37">
+        <v>-12.545255757248325</v>
+      </c>
+      <c r="C37">
+        <v>253.40503705455333</v>
+      </c>
+      <c r="D37">
+        <v>11375.173560044823</v>
+      </c>
+      <c r="E37">
+        <v>0.85879014375948848</v>
+      </c>
+      <c r="F37">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G37">
+        <v>88.769719174822029</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="U37" t="s">
+        <v>91</v>
+      </c>
+      <c r="V37">
+        <v>216.78369778735134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>33.852137410531341</v>
+      </c>
+      <c r="B38">
+        <v>-11.913389325677002</v>
+      </c>
+      <c r="C38">
+        <v>231.42274302019197</v>
+      </c>
+      <c r="D38">
+        <v>11811.347655406194</v>
+      </c>
+      <c r="E38">
+        <v>0.78429210822964057</v>
+      </c>
+      <c r="F38">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G38">
+        <v>68.263188647303622</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="U38" t="s">
+        <v>92</v>
+      </c>
+      <c r="V38">
+        <v>3.9620382940354082E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>35.652137410531338</v>
+      </c>
+      <c r="B39">
+        <v>-11.424461259597875</v>
+      </c>
+      <c r="C39">
+        <v>210.44098941475278</v>
+      </c>
+      <c r="D39">
+        <v>12208.892952366932</v>
+      </c>
+      <c r="E39">
+        <v>0.71318490608171259</v>
+      </c>
+      <c r="F39">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G39">
+        <v>52.395565662681676</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="U39" t="s">
+        <v>93</v>
+      </c>
+      <c r="V39">
+        <v>2417.7841094874643</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>37.452137410531336</v>
+      </c>
+      <c r="B40">
+        <v>-11.042372606652352</v>
+      </c>
+      <c r="C40">
+        <v>190.23324042993457</v>
+      </c>
+      <c r="D40">
+        <v>12569.397047024524</v>
+      </c>
+      <c r="E40">
+        <v>0.64470080703836308</v>
+      </c>
+      <c r="F40">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G40">
+        <v>39.995298399929744</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="U40" t="s">
+        <v>94</v>
+      </c>
+      <c r="V40">
+        <v>0.26413588626902723</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39.252137410531333</v>
+      </c>
+      <c r="B41">
+        <v>-10.746204273335103</v>
+      </c>
+      <c r="C41">
+        <v>170.63503794159354</v>
+      </c>
+      <c r="D41">
+        <v>12894.098364664609</v>
+      </c>
+      <c r="E41">
+        <v>0.57828246220977697</v>
+      </c>
+      <c r="F41">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G41">
+        <v>30.383480672326893</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="U41" t="s">
+        <v>95</v>
+      </c>
+      <c r="V41">
+        <v>409.41144253987727</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41.05213741053133</v>
+      </c>
+      <c r="B42">
+        <v>-10.513747345961264</v>
+      </c>
+      <c r="C42">
+        <v>151.51007090267919</v>
+      </c>
+      <c r="D42">
+        <v>13183.96647457576</v>
+      </c>
+      <c r="E42">
+        <v>0.51346791320296747</v>
+      </c>
+      <c r="F42">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G42">
+        <v>22.839346596917164</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="U42" t="s">
+        <v>96</v>
+      </c>
+      <c r="V42">
+        <v>22.831531676802577</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42.852137410531327</v>
+      </c>
+      <c r="B43">
+        <v>-10.328963280082133</v>
+      </c>
+      <c r="C43">
+        <v>132.75779912235802</v>
+      </c>
+      <c r="D43">
+        <v>13439.757704012083</v>
+      </c>
+      <c r="E43">
+        <v>0.44991642912346169</v>
+      </c>
+      <c r="F43">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G43">
+        <v>16.842382842210025</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="U43" t="s">
+        <v>97</v>
+      </c>
+      <c r="V43">
+        <v>5.8330119607457478</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44.652137410531324</v>
+      </c>
+      <c r="B44">
+        <v>-10.182331946742487</v>
+      </c>
+      <c r="C44">
+        <v>114.30269799426569</v>
+      </c>
+      <c r="D44">
+        <v>13662.07276396077</v>
+      </c>
+      <c r="E44">
+        <v>0.3873720569392643</v>
+      </c>
+      <c r="F44">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G44">
+        <v>12.083624086910042</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="U44" t="s">
+        <v>98</v>
+      </c>
+      <c r="V44">
+        <v>2.4597556798014728</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>46.452137410531321</v>
+      </c>
+      <c r="B45">
+        <v>-10.065623989412309</v>
+      </c>
+      <c r="C45">
+        <v>96.083941527841247</v>
+      </c>
+      <c r="D45">
+        <v>13851.389235105291</v>
+      </c>
+      <c r="E45">
+        <v>0.32562865725478429</v>
+      </c>
+      <c r="F45">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G45">
+        <v>8.2959956100435139</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>48.252137410531319</v>
+      </c>
+      <c r="B46">
+        <v>-9.9751660909906015</v>
+      </c>
+      <c r="C46">
+        <v>78.050885422714799</v>
+      </c>
+      <c r="D46">
+        <v>14008.086052469687</v>
+      </c>
+      <c r="E46">
+        <v>0.26451459644150027</v>
+      </c>
+      <c r="F46">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G46">
+        <v>5.3602839425840436</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>50.052137410531316</v>
+      </c>
+      <c r="B47">
+        <v>-9.9070354363267334</v>
+      </c>
+      <c r="C47">
+        <v>60.160013731704609</v>
+      </c>
+      <c r="D47">
+        <v>14132.457583714615</v>
+      </c>
+      <c r="E47">
+        <v>0.20388239887315632</v>
+      </c>
+      <c r="F47">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G47">
+        <v>3.1491784305376442</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>51.852137410531313</v>
+      </c>
+      <c r="B48">
+        <v>-9.858111201092731</v>
+      </c>
+      <c r="C48">
+        <v>42.374021655029509</v>
+      </c>
+      <c r="D48">
+        <v>14224.725010828279</v>
+      </c>
+      <c r="E48">
+        <v>0.143605638513635</v>
+      </c>
+      <c r="F48">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G48">
+        <v>1.5613961505601874</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>53.65213741053131</v>
+      </c>
+      <c r="B49">
+        <v>-9.8264607938878239</v>
+      </c>
+      <c r="C49">
+        <v>24.660403301048571</v>
+      </c>
+      <c r="D49">
+        <v>14285.047459530417</v>
+      </c>
+      <c r="E49">
+        <v>8.3574152835467194E-2</v>
+      </c>
+      <c r="F49">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G49">
+        <v>0.53421697292637893</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>55.452137410531307</v>
+      </c>
+      <c r="B50">
+        <v>-9.811334504012958</v>
+      </c>
+      <c r="C50">
+        <v>6.9888533117958538</v>
+      </c>
+      <c r="D50">
+        <v>14313.527701478539</v>
+      </c>
+      <c r="E50">
+        <v>2.3685236923917299E-2</v>
+      </c>
+      <c r="F50">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G50">
+        <v>4.3309860934955945E-2</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>56.674231989357395</v>
+      </c>
+      <c r="B51">
+        <v>-9.8093313640016451</v>
+      </c>
+      <c r="C51">
+        <v>-4.9999999999999503</v>
+      </c>
+      <c r="D51">
+        <v>14314.742748730931</v>
+      </c>
+      <c r="E51">
+        <v>1.6945009336467896E-2</v>
+      </c>
+      <c r="F51">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G51">
+        <v>-2.1699846402632925E-2</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2:AA24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>-9.8077912979337363</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>53.737018790651931</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0.11868906443783601</v>
+      </c>
+      <c r="K2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2">
+        <v>46964.380599746386</v>
+      </c>
+      <c r="O2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" t="s">
+        <v>57</v>
+      </c>
+      <c r="V2">
+        <v>300</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z2">
+        <v>32.453900860855732</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1.2927625756433149E-4</v>
+      </c>
+      <c r="B3">
+        <v>-9.8077625538079936</v>
+      </c>
+      <c r="C3">
+        <v>-1.267912700009145E-3</v>
+      </c>
+      <c r="D3">
+        <v>-8.1955544419449058E-8</v>
+      </c>
+      <c r="E3">
+        <v>3.7259000016658353E-6</v>
+      </c>
+      <c r="F3">
+        <v>53.736858563643331</v>
+      </c>
+      <c r="G3">
+        <v>-7.5977496586787575E-9</v>
+      </c>
+      <c r="H3">
+        <v>0.12023332196588275</v>
+      </c>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3">
+        <v>1.9100662847745531</v>
+      </c>
+      <c r="P3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" t="s">
+        <v>58</v>
+      </c>
+      <c r="V3">
+        <v>4</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>7.7565754538598888E-4</v>
+      </c>
+      <c r="B4">
+        <v>-9.8076131197978125</v>
+      </c>
+      <c r="C4">
+        <v>-7.6074191152028653E-3</v>
+      </c>
+      <c r="D4">
+        <v>-2.9503849512409596E-6</v>
+      </c>
+      <c r="E4">
+        <v>2.2355232259197035E-5</v>
+      </c>
+      <c r="F4">
+        <v>53.736057428600333</v>
+      </c>
+      <c r="G4">
+        <v>-2.7351488294879236E-7</v>
+      </c>
+      <c r="H4">
+        <v>0.12826125810512462</v>
+      </c>
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4">
+        <v>4.2279193995071358</v>
+      </c>
+      <c r="P4" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q4">
+        <v>2.6105E-2</v>
+      </c>
+      <c r="U4" t="s">
+        <v>59</v>
+      </c>
+      <c r="V4">
+        <v>0.9</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4.0075639844942756E-3</v>
+      </c>
+      <c r="B5">
+        <v>-9.8067021435395496</v>
+      </c>
+      <c r="C5">
+        <v>-3.9303314216520127E-2</v>
+      </c>
+      <c r="D5">
+        <v>-7.8756727076969679E-5</v>
+      </c>
+      <c r="E5">
+        <v>1.1549708301983543E-4</v>
+      </c>
+      <c r="F5">
+        <v>53.732051753385349</v>
+      </c>
+      <c r="G5">
+        <v>-7.3007020691739814E-6</v>
+      </c>
+      <c r="H5">
+        <v>0.17719329330612149</v>
+      </c>
+      <c r="K5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5">
+        <v>277.07370707650551</v>
+      </c>
+      <c r="P5" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q5">
+        <v>18.918327048707731</v>
+      </c>
+      <c r="U5" t="s">
+        <v>53</v>
+      </c>
+      <c r="V5">
+        <v>3</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2.0167096180035708E-2</v>
+      </c>
+      <c r="B6">
+        <v>-9.7933985270463353</v>
+      </c>
+      <c r="C6">
+        <v>-0.19769530261646528</v>
+      </c>
+      <c r="D6">
+        <v>-1.9939277736046404E-3</v>
+      </c>
+      <c r="E6">
+        <v>5.8094923394804159E-4</v>
+      </c>
+      <c r="F6">
+        <v>53.712023377310416</v>
+      </c>
+      <c r="G6">
+        <v>-1.8471367947272326E-4</v>
+      </c>
+      <c r="H6">
+        <v>0.89151398970559792</v>
+      </c>
+      <c r="K6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6">
+        <v>864.56508502112433</v>
+      </c>
+      <c r="P6" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q6">
+        <v>5887436.804562035</v>
+      </c>
+      <c r="U6" t="s">
+        <v>60</v>
+      </c>
+      <c r="V6">
+        <v>300</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z6">
+        <v>1.8241469247509919E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5.0193414275433001E-2</v>
+      </c>
+      <c r="B7">
+        <v>-9.4776570054937466</v>
+      </c>
+      <c r="C7">
+        <v>-0.4890847162890341</v>
+      </c>
+      <c r="D7">
+        <v>-1.2325530476494321E-2</v>
+      </c>
+      <c r="E7">
+        <v>1.437228676623566E-3</v>
+      </c>
+      <c r="F7">
+        <v>53.674808290655484</v>
+      </c>
+      <c r="G7">
+        <v>-1.1305114691530782E-3</v>
+      </c>
+      <c r="H7">
+        <v>17.837316005396374</v>
+      </c>
+      <c r="P7" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q7">
+        <v>853.90017992824039</v>
+      </c>
+      <c r="U7" t="s">
+        <v>61</v>
+      </c>
+      <c r="V7">
+        <v>45</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7.4181163493733826E-2</v>
+      </c>
+      <c r="B8">
+        <v>-6.3831947930205857</v>
+      </c>
+      <c r="C8">
+        <v>-0.69221630572312165</v>
+      </c>
+      <c r="D8">
+        <v>-2.6631639443629708E-2</v>
+      </c>
+      <c r="E8">
+        <v>2.0341526352147719E-3</v>
+      </c>
+      <c r="F8">
+        <v>53.645077500387444</v>
+      </c>
+      <c r="G8">
+        <v>-2.2645975682007743E-3</v>
+      </c>
+      <c r="H8">
+        <v>183.82896630957376</v>
+      </c>
+      <c r="P8" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q8">
+        <v>724.70128514490443</v>
+      </c>
+      <c r="U8" t="s">
+        <v>62</v>
+      </c>
+      <c r="V8">
+        <v>8</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA8">
+        <v>3.0020749999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9.8168912712034651E-2</v>
+      </c>
+      <c r="B9">
+        <v>12.345303705032707</v>
+      </c>
+      <c r="C9">
+        <v>-0.66771155223550616</v>
+      </c>
+      <c r="D9">
+        <v>-4.3842238455975062E-2</v>
+      </c>
+      <c r="E9">
+        <v>1.9621423804388784E-3</v>
+      </c>
+      <c r="F9">
+        <v>53.615346710119397</v>
+      </c>
+      <c r="G9">
+        <v>-2.1071035750547906E-3</v>
+      </c>
+      <c r="H9">
+        <v>1187.8621825097464</v>
+      </c>
+      <c r="O9" t="s">
+        <v>54</v>
+      </c>
+      <c r="U9" t="s">
+        <v>63</v>
+      </c>
+      <c r="V9">
+        <v>45</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA9">
+        <v>8.9602332474964276E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.11929116538065165</v>
+      </c>
+      <c r="B10">
+        <v>32.787872632822051</v>
+      </c>
+      <c r="C10">
+        <v>-0.16331444965731223</v>
+      </c>
+      <c r="D10">
+        <v>-5.3393064528390849E-2</v>
+      </c>
+      <c r="E10">
+        <v>4.7991706511387995E-4</v>
+      </c>
+      <c r="F10">
+        <v>53.589167460938313</v>
+      </c>
+      <c r="G10">
+        <v>-1.2605431750961838E-4</v>
+      </c>
+      <c r="H10">
+        <v>2282.7844039457045</v>
+      </c>
+      <c r="P10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>30</v>
+      </c>
+      <c r="R10" t="s">
+        <v>150</v>
+      </c>
+      <c r="U10" t="s">
+        <v>64</v>
+      </c>
+      <c r="V10">
+        <v>15</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA10">
+        <v>1831.9745409498933</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.14024205540898918</v>
+      </c>
+      <c r="B11">
+        <v>38.142678623492507</v>
+      </c>
+      <c r="C11">
+        <v>0.59598417941665061</v>
+      </c>
+      <c r="D11">
+        <v>-4.9047600796110598E-2</v>
+      </c>
+      <c r="E11">
+        <v>1.7513636598513235E-3</v>
+      </c>
+      <c r="F11">
+        <v>53.563200601284549</v>
+      </c>
+      <c r="G11">
+        <v>1.67871814064406E-3</v>
+      </c>
+      <c r="H11">
+        <v>2568.5006231971997</v>
+      </c>
+      <c r="P11" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q11">
+        <v>7.7915071717360252E-3</v>
+      </c>
+      <c r="U11" t="s">
+        <v>65</v>
+      </c>
+      <c r="V11">
+        <v>2068428</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA11">
+        <v>546.78577951537659</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.16576992529052567</v>
+      </c>
+      <c r="B12">
+        <v>38.960727251071539</v>
+      </c>
+      <c r="C12">
+        <v>1.5839627990373799</v>
+      </c>
+      <c r="D12">
+        <v>-2.1263561117739846E-2</v>
+      </c>
+      <c r="E12">
+        <v>4.6546466331182194E-3</v>
+      </c>
+      <c r="F12">
+        <v>53.531560961461288</v>
+      </c>
+      <c r="G12">
+        <v>1.1857608776918169E-2</v>
+      </c>
+      <c r="H12">
+        <v>2610.7850165843142</v>
+      </c>
+      <c r="P12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q12">
+        <v>2.3647908810884664</v>
+      </c>
+      <c r="U12" t="s">
+        <v>66</v>
+      </c>
+      <c r="V12">
+        <v>3252.5</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA12">
+        <v>66.792845291262523</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.20281596178802641</v>
+      </c>
+      <c r="B13">
+        <v>39.069954535397791</v>
+      </c>
+      <c r="C13">
+        <v>3.0299289531513907</v>
+      </c>
+      <c r="D13">
+        <v>6.4188414534183058E-2</v>
+      </c>
+      <c r="E13">
+        <v>8.9037837262757793E-3</v>
+      </c>
+      <c r="F13">
+        <v>53.485645526405413</v>
+      </c>
+      <c r="G13">
+        <v>4.3387885944673577E-2</v>
+      </c>
+      <c r="H13">
+        <v>2614.4193095130436</v>
+      </c>
+      <c r="P13" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q13">
+        <v>4357255.0535812248</v>
+      </c>
+      <c r="U13" t="s">
+        <v>67</v>
+      </c>
+      <c r="V13">
+        <v>1.4356</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA13">
+        <v>0.14231669665470673</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.27159827498415007</v>
+      </c>
+      <c r="B14">
+        <v>39.145783922735184</v>
+      </c>
+      <c r="C14">
+        <v>5.719866076281459</v>
+      </c>
+      <c r="D14">
+        <v>0.36507408947003211</v>
+      </c>
+      <c r="E14">
+        <v>1.6808520631366213E-2</v>
+      </c>
+      <c r="F14">
+        <v>53.400395655349378</v>
+      </c>
+      <c r="G14">
+        <v>0.1610896289032433</v>
+      </c>
+      <c r="H14">
+        <v>2614.4193207207541</v>
+      </c>
+      <c r="P14" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q14">
+        <v>631.96616757961476</v>
+      </c>
+      <c r="U14" t="s">
+        <v>68</v>
+      </c>
+      <c r="V14">
+        <v>238.91946992864425</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA14">
+        <v>16.321321753211024</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.61550984096476835</v>
+      </c>
+      <c r="B15">
+        <v>39.507629901115472</v>
+      </c>
+      <c r="C15">
+        <v>19.245577403494039</v>
+      </c>
+      <c r="D15">
+        <v>4.6544599608515602</v>
+      </c>
+      <c r="E15">
+        <v>5.6558201191065055E-2</v>
+      </c>
+      <c r="F15">
+        <v>52.974146300069179</v>
+      </c>
+      <c r="G15">
+        <v>1.8601389068137313</v>
+      </c>
+      <c r="H15">
+        <v>2614.4194804611711</v>
+      </c>
+      <c r="P15" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q15">
+        <v>303.5087857798336</v>
+      </c>
+      <c r="U15" t="s">
+        <v>69</v>
+      </c>
+      <c r="V15">
+        <v>1632.6274728336584</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA15">
+        <v>12071.729394727032</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2.3350676708678595</v>
+      </c>
+      <c r="B16">
+        <v>40.885651191846868</v>
+      </c>
+      <c r="C16">
+        <v>88.471053010922063</v>
+      </c>
+      <c r="D16">
+        <v>96.927309799530477</v>
+      </c>
+      <c r="E16">
+        <v>0.26026654212654726</v>
+      </c>
+      <c r="F16">
+        <v>50.842899523668208</v>
+      </c>
+      <c r="G16">
+        <v>36.90900105573791</v>
+      </c>
+      <c r="H16">
+        <v>2614.4229008897387</v>
+      </c>
+      <c r="O16" t="s">
+        <v>53</v>
+      </c>
+      <c r="P16">
+        <v>21.283117929796198</v>
+      </c>
+      <c r="U16" t="s">
+        <v>70</v>
+      </c>
+      <c r="V16">
+        <v>1469.3647255502926</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA16">
+        <v>21.338591027161645</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4.1350676708678593</v>
+      </c>
+      <c r="B17">
+        <v>41.475889309165005</v>
+      </c>
+      <c r="C17">
+        <v>162.73281170778512</v>
+      </c>
+      <c r="D17">
+        <v>322.85095564515456</v>
+      </c>
+      <c r="E17">
+        <v>0.47995905773358716</v>
+      </c>
+      <c r="F17">
+        <v>48.611951467831119</v>
+      </c>
+      <c r="G17">
+        <v>121.32398628143252</v>
+      </c>
+      <c r="H17">
+        <v>2614.4311483631209</v>
+      </c>
+      <c r="U17" t="s">
+        <v>71</v>
+      </c>
+      <c r="V17">
+        <v>92063</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA17">
+        <v>0.14231669665470673</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5.9350676708678591</v>
+      </c>
+      <c r="B18">
+        <v>41.099769709888847</v>
+      </c>
+      <c r="C18">
+        <v>237.21022552752751</v>
+      </c>
+      <c r="D18">
+        <v>682.90287959451564</v>
+      </c>
+      <c r="E18">
+        <v>0.70250007265466463</v>
+      </c>
+      <c r="F18">
+        <v>46.381003411994023</v>
+      </c>
+      <c r="G18">
+        <v>253.19772248768462</v>
+      </c>
+      <c r="H18">
+        <v>2614.4439251058693</v>
+      </c>
+      <c r="U18" t="s">
+        <v>72</v>
+      </c>
+      <c r="V18">
+        <v>1.1724846115020683E-2</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA18">
+        <v>4.4325735113785898</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>7.735067670867859</v>
+      </c>
+      <c r="B19">
+        <v>39.39440721349758</v>
+      </c>
+      <c r="C19">
+        <v>310.00321680181412</v>
+      </c>
+      <c r="D19">
+        <v>1175.8390820170303</v>
+      </c>
+      <c r="E19">
+        <v>0.9233055962783604</v>
+      </c>
+      <c r="F19">
+        <v>44.150055356156926</v>
+      </c>
+      <c r="G19">
+        <v>442.08340268117257</v>
+      </c>
+      <c r="H19">
+        <v>2614.460704923978</v>
+      </c>
+      <c r="U19" t="s">
+        <v>73</v>
+      </c>
+      <c r="V19">
+        <v>1.4473248461150208</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA19">
+        <v>12071.729394727032</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>9.503446508989958</v>
+      </c>
+      <c r="B20">
+        <v>32.694573676337711</v>
+      </c>
+      <c r="C20">
+        <v>372.50406278211403</v>
+      </c>
+      <c r="D20">
+        <v>1781.2366794489831</v>
+      </c>
+      <c r="E20">
+        <v>1.1173213403125017</v>
+      </c>
+      <c r="F20">
+        <v>41.958299061216955</v>
+      </c>
+      <c r="G20">
+        <v>831.0606129055767</v>
+      </c>
+      <c r="H20">
+        <v>2614.4802266868842</v>
+      </c>
+      <c r="U20" t="s">
+        <v>74</v>
+      </c>
+      <c r="V20">
+        <v>2635.8007716814773</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA20">
+        <v>7.4032209766824941</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>11.303446508989959</v>
+      </c>
+      <c r="B21">
+        <v>31.29192208938256</v>
+      </c>
+      <c r="C21">
+        <v>429.87720830998353</v>
+      </c>
+      <c r="D21">
+        <v>2503.7431171989729</v>
+      </c>
+      <c r="E21">
+        <v>1.3005001378925525</v>
+      </c>
+      <c r="F21">
+        <v>39.727351005379859</v>
+      </c>
+      <c r="G21">
+        <v>981.63154213403072</v>
+      </c>
+      <c r="H21">
+        <v>2614.5020279747077</v>
+      </c>
+      <c r="U21" t="s">
+        <v>75</v>
+      </c>
+      <c r="V21">
+        <v>592.58110874133922</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA21">
+        <v>2.0105798841732372</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>13.103446508989959</v>
+      </c>
+      <c r="B22">
+        <v>30.717596443922417</v>
+      </c>
+      <c r="C22">
+        <v>485.6101317711437</v>
+      </c>
+      <c r="D22">
+        <v>3327.8379963220764</v>
+      </c>
+      <c r="E22">
+        <v>1.4837979384511213</v>
+      </c>
+      <c r="F22">
+        <v>37.49640294954277</v>
+      </c>
+      <c r="G22">
+        <v>1094.8859264552373</v>
+      </c>
+      <c r="H22">
+        <v>2614.5250132930091</v>
+      </c>
+      <c r="U22" t="s">
+        <v>76</v>
+      </c>
+      <c r="V22">
+        <v>8.8045295423009077E-4</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA22">
+        <v>9.4138008608557318</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>14.90344650898996</v>
+      </c>
+      <c r="B23">
+        <v>30.78616506191095</v>
+      </c>
+      <c r="C23">
+        <v>540.86773333256019</v>
+      </c>
+      <c r="D23">
+        <v>4251.6323108320721</v>
+      </c>
+      <c r="E23">
+        <v>1.6715769334284727</v>
+      </c>
+      <c r="F23">
+        <v>35.26545489370568</v>
+      </c>
+      <c r="G23">
+        <v>1182.9063174766882</v>
+      </c>
+      <c r="H23">
+        <v>2614.5485453249394</v>
+      </c>
+      <c r="U23" t="s">
+        <v>77</v>
+      </c>
+      <c r="V23">
+        <v>1.3647048084662576</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z23">
+        <v>53.737018790651931</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>16.703446508989959</v>
+      </c>
+      <c r="B24">
+        <v>32.11927527460405</v>
+      </c>
+      <c r="C24">
+        <v>597.2087865858515</v>
+      </c>
+      <c r="D24">
+        <v>5275.5408889114688</v>
+      </c>
+      <c r="E24">
+        <v>1.8697393776984526</v>
+      </c>
+      <c r="F24">
+        <v>33.034506837868584</v>
+      </c>
+      <c r="G24">
+        <v>1229.4591348585516</v>
+      </c>
+      <c r="H24">
+        <v>2614.5720656243334</v>
+      </c>
+      <c r="U24" t="s">
+        <v>78</v>
+      </c>
+      <c r="V24">
+        <v>3.3481749037418129E-2</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z24">
+        <v>0.39606063769020622</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>16.910570229076576</v>
+      </c>
+      <c r="B25">
+        <v>32.389892579251153</v>
+      </c>
+      <c r="C25">
+        <v>603.89063214461294</v>
+      </c>
+      <c r="D25">
+        <v>5399.9280999914481</v>
+      </c>
+      <c r="E25">
+        <v>1.893676874471854</v>
+      </c>
+      <c r="F25">
+        <v>32.777794470843588</v>
+      </c>
+      <c r="G25">
+        <v>1231.355343927984</v>
+      </c>
+      <c r="H25">
+        <v>2614.5747495823557</v>
+      </c>
+      <c r="U25" t="s">
+        <v>79</v>
+      </c>
+      <c r="V25">
+        <v>1.3181790959613437</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>17.056344586235362</v>
+      </c>
+      <c r="B26">
+        <v>18.605894766498089</v>
+      </c>
+      <c r="C26">
+        <v>608.42542046287576</v>
+      </c>
+      <c r="D26">
+        <v>5488.3047523584919</v>
+      </c>
+      <c r="E26">
+        <v>1.9100662847745531</v>
+      </c>
+      <c r="F26">
+        <v>32.597119460457876</v>
+      </c>
+      <c r="G26">
+        <v>1232.5342841481561</v>
+      </c>
+      <c r="H26">
+        <v>2158.8106004274941</v>
+      </c>
+      <c r="U26" t="s">
+        <v>80</v>
+      </c>
+      <c r="V26">
+        <v>1.2394155865761627</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>17.202118943394147</v>
+      </c>
+      <c r="B27">
+        <v>-46.870015201803916</v>
+      </c>
+      <c r="C27">
+        <v>602.70752823196938</v>
+      </c>
+      <c r="D27">
+        <v>5576.6521215743205</v>
+      </c>
+      <c r="E27">
+        <v>1.8942712547979834</v>
+      </c>
+      <c r="F27">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G27">
+        <v>1202.7420592611506</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="U27" t="s">
+        <v>81</v>
+      </c>
+      <c r="V27">
+        <v>0.13771284295290698</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>17.373460836350826</v>
+      </c>
+      <c r="B28">
+        <v>-45.733303249099436</v>
+      </c>
+      <c r="C28">
+        <v>594.77556814531465</v>
+      </c>
+      <c r="D28">
+        <v>5679.2387915255722</v>
+      </c>
+      <c r="E28">
+        <v>1.8718207166426761</v>
+      </c>
+      <c r="F28">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G28">
+        <v>1165.8513222407296</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="U28" t="s">
+        <v>82</v>
+      </c>
+      <c r="V28">
+        <v>4.5373593584471848E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>18.037531039975594</v>
+      </c>
+      <c r="B29">
+        <v>-41.69138110803349</v>
+      </c>
+      <c r="C29">
+        <v>565.78312242040852</v>
+      </c>
+      <c r="D29">
+        <v>6064.4370110113141</v>
+      </c>
+      <c r="E29">
+        <v>1.7895178955290192</v>
+      </c>
+      <c r="F29">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G29">
+        <v>1034.6751817872778</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="U29" t="s">
+        <v>83</v>
+      </c>
+      <c r="V29">
+        <v>1.1017027436232558</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>19.452137410531339</v>
+      </c>
+      <c r="B30">
+        <v>-34.595837642179312</v>
+      </c>
+      <c r="C30">
+        <v>512.03882601297448</v>
+      </c>
+      <c r="D30">
+        <v>6825.5995756684415</v>
+      </c>
+      <c r="E30">
+        <v>1.6358813547761384</v>
+      </c>
+      <c r="F30">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G30">
+        <v>804.39711759255351</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="U30" t="s">
+        <v>84</v>
+      </c>
+      <c r="V30">
+        <v>1.5202163514902139E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>21.25213741053134</v>
+      </c>
+      <c r="B31">
+        <v>-28.261666814553486</v>
+      </c>
+      <c r="C31">
+        <v>455.82766095248297</v>
+      </c>
+      <c r="D31">
+        <v>7694.9849689429857</v>
+      </c>
+      <c r="E31">
+        <v>1.4734737590132565</v>
+      </c>
+      <c r="F31">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G31">
+        <v>598.8285655170605</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="U31" t="s">
+        <v>85</v>
+      </c>
+      <c r="V31">
+        <v>3.5218118169203631E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>23.052137410531341</v>
+      </c>
+      <c r="B32">
+        <v>-23.884588947937846</v>
+      </c>
+      <c r="C32">
+        <v>409.13128255754532</v>
+      </c>
+      <c r="D32">
+        <v>8472.2675877965321</v>
+      </c>
+      <c r="E32">
+        <v>1.3367835559465349</v>
+      </c>
+      <c r="F32">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G32">
+        <v>456.77531437367065</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="U32" t="s">
+        <v>86</v>
+      </c>
+      <c r="V32">
+        <v>5.4588192338650305</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>24.852137410531341</v>
+      </c>
+      <c r="B33">
+        <v>-20.727766842799369</v>
+      </c>
+      <c r="C33">
+        <v>369.12358717746218</v>
+      </c>
+      <c r="D33">
+        <v>9171.8447226932258</v>
+      </c>
+      <c r="E33">
+        <v>1.2180033514885484</v>
+      </c>
+      <c r="F33">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G33">
+        <v>354.32412273814867</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="U33" t="s">
+        <v>87</v>
+      </c>
+      <c r="V33">
+        <v>6.6963498074836258E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>26.652137410531342</v>
+      </c>
+      <c r="B34">
+        <v>-18.281792048072234</v>
+      </c>
+      <c r="C34">
+        <v>334.08386769182437</v>
+      </c>
+      <c r="D34">
+        <v>9804.0705657555609</v>
+      </c>
+      <c r="E34">
+        <v>1.1124293896336017</v>
+      </c>
+      <c r="F34">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G34">
+        <v>274.94269924192224</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="U34" t="s">
+        <v>88</v>
+      </c>
+      <c r="V34">
+        <v>2.6363581919226875</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>28.452137410531343</v>
+      </c>
+      <c r="B35">
+        <v>-15.882874695346633</v>
+      </c>
+      <c r="C35">
+        <v>303.15823178571509</v>
+      </c>
+      <c r="D35">
+        <v>10376.968961663251</v>
+      </c>
+      <c r="E35">
+        <v>1.0179340621748745</v>
+      </c>
+      <c r="F35">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G35">
+        <v>197.08847330317909</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="U35" t="s">
+        <v>89</v>
+      </c>
+      <c r="V35">
+        <v>17.171897917299866</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>30.252137410531343</v>
+      </c>
+      <c r="B36">
+        <v>-13.620681138868854</v>
+      </c>
+      <c r="C36">
+        <v>276.76593600063137</v>
+      </c>
+      <c r="D36">
+        <v>10898.29171636667</v>
+      </c>
+      <c r="E36">
+        <v>0.93653245577495126</v>
+      </c>
+      <c r="F36">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G36">
+        <v>123.67146789318255</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="U36" t="s">
+        <v>90</v>
+      </c>
+      <c r="V36">
+        <v>10175.742307026649</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>32.052137410531344</v>
+      </c>
+      <c r="B37">
+        <v>-12.545255757248325</v>
+      </c>
+      <c r="C37">
+        <v>253.40503705455333</v>
+      </c>
+      <c r="D37">
+        <v>11375.173560044823</v>
+      </c>
+      <c r="E37">
+        <v>0.85879014375948848</v>
+      </c>
+      <c r="F37">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G37">
+        <v>88.769719174822029</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="U37" t="s">
+        <v>91</v>
+      </c>
+      <c r="V37">
+        <v>216.78369778735134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>33.852137410531341</v>
+      </c>
+      <c r="B38">
+        <v>-11.913389325677002</v>
+      </c>
+      <c r="C38">
+        <v>231.42274302019197</v>
+      </c>
+      <c r="D38">
+        <v>11811.347655406194</v>
+      </c>
+      <c r="E38">
+        <v>0.78429210822964057</v>
+      </c>
+      <c r="F38">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G38">
+        <v>68.263188647303622</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="U38" t="s">
+        <v>92</v>
+      </c>
+      <c r="V38">
+        <v>3.9620382940354082E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>35.652137410531338</v>
+      </c>
+      <c r="B39">
+        <v>-11.424461259597875</v>
+      </c>
+      <c r="C39">
+        <v>210.44098941475278</v>
+      </c>
+      <c r="D39">
+        <v>12208.892952366932</v>
+      </c>
+      <c r="E39">
+        <v>0.71318490608171259</v>
+      </c>
+      <c r="F39">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G39">
+        <v>52.395565662681676</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="U39" t="s">
+        <v>93</v>
+      </c>
+      <c r="V39">
+        <v>2417.7841094874643</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>37.452137410531336</v>
+      </c>
+      <c r="B40">
+        <v>-11.042372606652352</v>
+      </c>
+      <c r="C40">
+        <v>190.23324042993457</v>
+      </c>
+      <c r="D40">
+        <v>12569.397047024524</v>
+      </c>
+      <c r="E40">
+        <v>0.64470080703836308</v>
+      </c>
+      <c r="F40">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G40">
+        <v>39.995298399929744</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="U40" t="s">
+        <v>94</v>
+      </c>
+      <c r="V40">
+        <v>0.26413588626902723</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39.252137410531333</v>
+      </c>
+      <c r="B41">
+        <v>-10.746204273335103</v>
+      </c>
+      <c r="C41">
+        <v>170.63503794159354</v>
+      </c>
+      <c r="D41">
+        <v>12894.098364664609</v>
+      </c>
+      <c r="E41">
+        <v>0.57828246220977697</v>
+      </c>
+      <c r="F41">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G41">
+        <v>30.383480672326893</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="U41" t="s">
+        <v>95</v>
+      </c>
+      <c r="V41">
+        <v>409.41144253987727</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41.05213741053133</v>
+      </c>
+      <c r="B42">
+        <v>-10.513747345961264</v>
+      </c>
+      <c r="C42">
+        <v>151.51007090267919</v>
+      </c>
+      <c r="D42">
+        <v>13183.96647457576</v>
+      </c>
+      <c r="E42">
+        <v>0.51346791320296747</v>
+      </c>
+      <c r="F42">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G42">
+        <v>22.839346596917164</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="U42" t="s">
+        <v>96</v>
+      </c>
+      <c r="V42">
+        <v>22.831531676802577</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42.852137410531327</v>
+      </c>
+      <c r="B43">
+        <v>-10.328963280082133</v>
+      </c>
+      <c r="C43">
+        <v>132.75779912235802</v>
+      </c>
+      <c r="D43">
+        <v>13439.757704012083</v>
+      </c>
+      <c r="E43">
+        <v>0.44991642912346169</v>
+      </c>
+      <c r="F43">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G43">
+        <v>16.842382842210025</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="U43" t="s">
+        <v>97</v>
+      </c>
+      <c r="V43">
+        <v>5.8330119607457478</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44.652137410531324</v>
+      </c>
+      <c r="B44">
+        <v>-10.182331946742487</v>
+      </c>
+      <c r="C44">
+        <v>114.30269799426569</v>
+      </c>
+      <c r="D44">
+        <v>13662.07276396077</v>
+      </c>
+      <c r="E44">
+        <v>0.3873720569392643</v>
+      </c>
+      <c r="F44">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G44">
+        <v>12.083624086910042</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="U44" t="s">
+        <v>98</v>
+      </c>
+      <c r="V44">
+        <v>2.4597556798014728</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>46.452137410531321</v>
+      </c>
+      <c r="B45">
+        <v>-10.065623989412309</v>
+      </c>
+      <c r="C45">
+        <v>96.083941527841247</v>
+      </c>
+      <c r="D45">
+        <v>13851.389235105291</v>
+      </c>
+      <c r="E45">
+        <v>0.32562865725478429</v>
+      </c>
+      <c r="F45">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G45">
+        <v>8.2959956100435139</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>48.252137410531319</v>
+      </c>
+      <c r="B46">
+        <v>-9.9751660909906015</v>
+      </c>
+      <c r="C46">
+        <v>78.050885422714799</v>
+      </c>
+      <c r="D46">
+        <v>14008.086052469687</v>
+      </c>
+      <c r="E46">
+        <v>0.26451459644150027</v>
+      </c>
+      <c r="F46">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G46">
+        <v>5.3602839425840436</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>50.052137410531316</v>
+      </c>
+      <c r="B47">
+        <v>-9.9070354363267334</v>
+      </c>
+      <c r="C47">
+        <v>60.160013731704609</v>
+      </c>
+      <c r="D47">
+        <v>14132.457583714615</v>
+      </c>
+      <c r="E47">
+        <v>0.20388239887315632</v>
+      </c>
+      <c r="F47">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G47">
+        <v>3.1491784305376442</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>51.852137410531313</v>
+      </c>
+      <c r="B48">
+        <v>-9.858111201092731</v>
+      </c>
+      <c r="C48">
+        <v>42.374021655029509</v>
+      </c>
+      <c r="D48">
+        <v>14224.725010828279</v>
+      </c>
+      <c r="E48">
+        <v>0.143605638513635</v>
+      </c>
+      <c r="F48">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G48">
+        <v>1.5613961505601874</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>53.65213741053131</v>
+      </c>
+      <c r="B49">
+        <v>-9.8264607938878239</v>
+      </c>
+      <c r="C49">
+        <v>24.660403301048571</v>
+      </c>
+      <c r="D49">
+        <v>14285.047459530417</v>
+      </c>
+      <c r="E49">
+        <v>8.3574152835467194E-2</v>
+      </c>
+      <c r="F49">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G49">
+        <v>0.53421697292637893</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>55.452137410531307</v>
+      </c>
+      <c r="B50">
+        <v>-9.811334504012958</v>
+      </c>
+      <c r="C50">
+        <v>6.9888533117958538</v>
+      </c>
+      <c r="D50">
+        <v>14313.527701478539</v>
+      </c>
+      <c r="E50">
+        <v>2.3685236923917299E-2</v>
+      </c>
+      <c r="F50">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G50">
+        <v>4.3309860934955945E-2</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>56.674231989357395</v>
+      </c>
+      <c r="B51">
+        <v>-9.8093313640016451</v>
+      </c>
+      <c r="C51">
+        <v>-4.9999999999999503</v>
+      </c>
+      <c r="D51">
+        <v>14314.742748730931</v>
+      </c>
+      <c r="E51">
+        <v>1.6945009336467896E-2</v>
+      </c>
+      <c r="F51">
+        <v>32.453900860855732</v>
+      </c>
+      <c r="G51">
+        <v>-2.1699846402632925E-2</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9911,6 +13639,9 @@
         <v>3</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+    </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C30" t="str">
         <f>IF(B31="Single value","Value",IF(B31="Range of values","Start",IF(B31="Monte Carlo","Mean","ERROR")))</f>
@@ -9999,9 +13730,7 @@
       <c r="C37" s="1">
         <v>5</v>
       </c>
-      <c r="D37" s="1">
-        <v>1</v>
-      </c>
+      <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
   </sheetData>
@@ -10316,7 +14045,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Overwrote someone's stuff again, fixed
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" tabRatio="882" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" tabRatio="882"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
@@ -21,15 +21,13 @@
     <sheet name="Results 27-Aug-2017 14-35-18" sheetId="15" r:id="rId12"/>
     <sheet name="Results 27-Aug-2017 14-35-43" sheetId="16" r:id="rId13"/>
     <sheet name="Results 17-Sep-2017 13-34-09" sheetId="17" r:id="rId14"/>
-    <sheet name="Results 17-Sep-2017 14-28-17" sheetId="18" r:id="rId15"/>
-    <sheet name="Results 17-Sep-2017 14-30-28" sheetId="19" r:id="rId16"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="174">
   <si>
     <t>Total inert mass</t>
   </si>
@@ -491,16 +489,77 @@
   </si>
   <si>
     <t>in to m</t>
+  </si>
+  <si>
+    <t>Las Cruces US Climate Data</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Launch Angle</t>
+  </si>
+  <si>
+    <t>Degrees</t>
+  </si>
+  <si>
+    <t>Launch Altitude</t>
+  </si>
+  <si>
+    <t>ft</t>
+  </si>
+  <si>
+    <t>Tank</t>
+  </si>
+  <si>
+    <t>Tank Mass Calculation</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>End Cap</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>lbm</t>
+  </si>
+  <si>
+    <t>Subtotal Mass</t>
+  </si>
+  <si>
+    <t>Ox Cylinder</t>
+  </si>
+  <si>
+    <t>Fuel Cylinder</t>
+  </si>
+  <si>
+    <t>lbm/in</t>
+  </si>
+  <si>
+    <t>Interpropellant Bulkhead</t>
+  </si>
+  <si>
+    <t>Total Mass</t>
+  </si>
+  <si>
+    <t>DO NOT INPUT, CALCULATED FROM LAUNCH ALTITUDE. Need to implement temperature compensation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,8 +582,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -541,6 +608,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -562,11 +635,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -577,9 +651,15 @@
     <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -879,10 +959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F7"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,7 +971,12 @@
     <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G1" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3" t="str">
         <f>IF(B4="Single value","Value",IF(B4="Range of values","Start",IF(B4="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
@@ -905,7 +990,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -921,7 +1006,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C6" t="str">
         <f>IF(B7="Single value","Value",IF(B7="Range of values","Start",IF(B7="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
@@ -935,32 +1020,79 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1">
-        <v>86000</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="C7" s="11">
+        <f>101325*(1-(0.0000225577)*(C13*0.3048))^5.25588</f>
+        <v>85592.941945501399</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
       <c r="F7" t="s">
         <v>25</v>
       </c>
+      <c r="G7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1">
+        <v>4595</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" t="s">
+        <v>159</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Validation!$A$2:$A$4</xm:f>
+            <xm:f>Validation!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>B4 B7</xm:sqref>
+          <xm:sqref>B4 B7 B10 B13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -9759,3738 +9891,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA51"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2:AA24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H1" t="s">
-        <v>131</v>
-      </c>
-      <c r="K1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" t="s">
-        <v>46</v>
-      </c>
-      <c r="U1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>-9.8077912979337363</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>53.737018790651931</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0.11868906443783601</v>
-      </c>
-      <c r="K2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2">
-        <v>46964.380599746386</v>
-      </c>
-      <c r="O2" t="s">
-        <v>47</v>
-      </c>
-      <c r="U2" t="s">
-        <v>57</v>
-      </c>
-      <c r="V2">
-        <v>300</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z2">
-        <v>32.453900860855732</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1.2927625756433149E-4</v>
-      </c>
-      <c r="B3">
-        <v>-9.8077625538079936</v>
-      </c>
-      <c r="C3">
-        <v>-1.267912700009145E-3</v>
-      </c>
-      <c r="D3">
-        <v>-8.1955544419449058E-8</v>
-      </c>
-      <c r="E3">
-        <v>3.7259000016658353E-6</v>
-      </c>
-      <c r="F3">
-        <v>53.736858563643331</v>
-      </c>
-      <c r="G3">
-        <v>-7.5977496586787575E-9</v>
-      </c>
-      <c r="H3">
-        <v>0.12023332196588275</v>
-      </c>
-      <c r="K3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3">
-        <v>1.9100662847745531</v>
-      </c>
-      <c r="P3" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>28</v>
-      </c>
-      <c r="R3" t="s">
-        <v>29</v>
-      </c>
-      <c r="U3" t="s">
-        <v>58</v>
-      </c>
-      <c r="V3">
-        <v>4</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>7.7565754538598888E-4</v>
-      </c>
-      <c r="B4">
-        <v>-9.8076131197978125</v>
-      </c>
-      <c r="C4">
-        <v>-7.6074191152028653E-3</v>
-      </c>
-      <c r="D4">
-        <v>-2.9503849512409596E-6</v>
-      </c>
-      <c r="E4">
-        <v>2.2355232259197035E-5</v>
-      </c>
-      <c r="F4">
-        <v>53.736057428600333</v>
-      </c>
-      <c r="G4">
-        <v>-2.7351488294879236E-7</v>
-      </c>
-      <c r="H4">
-        <v>0.12826125810512462</v>
-      </c>
-      <c r="K4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4">
-        <v>4.2279193995071358</v>
-      </c>
-      <c r="P4" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q4">
-        <v>2.6105E-2</v>
-      </c>
-      <c r="U4" t="s">
-        <v>59</v>
-      </c>
-      <c r="V4">
-        <v>0.9</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>102</v>
-      </c>
-      <c r="Z4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4.0075639844942756E-3</v>
-      </c>
-      <c r="B5">
-        <v>-9.8067021435395496</v>
-      </c>
-      <c r="C5">
-        <v>-3.9303314216520127E-2</v>
-      </c>
-      <c r="D5">
-        <v>-7.8756727076969679E-5</v>
-      </c>
-      <c r="E5">
-        <v>1.1549708301983543E-4</v>
-      </c>
-      <c r="F5">
-        <v>53.732051753385349</v>
-      </c>
-      <c r="G5">
-        <v>-7.3007020691739814E-6</v>
-      </c>
-      <c r="H5">
-        <v>0.17719329330612149</v>
-      </c>
-      <c r="K5" t="s">
-        <v>44</v>
-      </c>
-      <c r="L5">
-        <v>277.07370707650551</v>
-      </c>
-      <c r="P5" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q5">
-        <v>18.918327048707731</v>
-      </c>
-      <c r="U5" t="s">
-        <v>53</v>
-      </c>
-      <c r="V5">
-        <v>3</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2.0167096180035708E-2</v>
-      </c>
-      <c r="B6">
-        <v>-9.7933985270463353</v>
-      </c>
-      <c r="C6">
-        <v>-0.19769530261646528</v>
-      </c>
-      <c r="D6">
-        <v>-1.9939277736046404E-3</v>
-      </c>
-      <c r="E6">
-        <v>5.8094923394804159E-4</v>
-      </c>
-      <c r="F6">
-        <v>53.712023377310416</v>
-      </c>
-      <c r="G6">
-        <v>-1.8471367947272326E-4</v>
-      </c>
-      <c r="H6">
-        <v>0.89151398970559792</v>
-      </c>
-      <c r="K6" t="s">
-        <v>45</v>
-      </c>
-      <c r="L6">
-        <v>864.56508502112433</v>
-      </c>
-      <c r="P6" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q6">
-        <v>5887436.804562035</v>
-      </c>
-      <c r="U6" t="s">
-        <v>60</v>
-      </c>
-      <c r="V6">
-        <v>300</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>104</v>
-      </c>
-      <c r="Z6">
-        <v>1.8241469247509919E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5.0193414275433001E-2</v>
-      </c>
-      <c r="B7">
-        <v>-9.4776570054937466</v>
-      </c>
-      <c r="C7">
-        <v>-0.4890847162890341</v>
-      </c>
-      <c r="D7">
-        <v>-1.2325530476494321E-2</v>
-      </c>
-      <c r="E7">
-        <v>1.437228676623566E-3</v>
-      </c>
-      <c r="F7">
-        <v>53.674808290655484</v>
-      </c>
-      <c r="G7">
-        <v>-1.1305114691530782E-3</v>
-      </c>
-      <c r="H7">
-        <v>17.837316005396374</v>
-      </c>
-      <c r="P7" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q7">
-        <v>853.90017992824039</v>
-      </c>
-      <c r="U7" t="s">
-        <v>61</v>
-      </c>
-      <c r="V7">
-        <v>45</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7.4181163493733826E-2</v>
-      </c>
-      <c r="B8">
-        <v>-6.3831947930205857</v>
-      </c>
-      <c r="C8">
-        <v>-0.69221630572312165</v>
-      </c>
-      <c r="D8">
-        <v>-2.6631639443629708E-2</v>
-      </c>
-      <c r="E8">
-        <v>2.0341526352147719E-3</v>
-      </c>
-      <c r="F8">
-        <v>53.645077500387444</v>
-      </c>
-      <c r="G8">
-        <v>-2.2645975682007743E-3</v>
-      </c>
-      <c r="H8">
-        <v>183.82896630957376</v>
-      </c>
-      <c r="P8" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q8">
-        <v>724.70128514490443</v>
-      </c>
-      <c r="U8" t="s">
-        <v>62</v>
-      </c>
-      <c r="V8">
-        <v>8</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA8">
-        <v>3.0020749999999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>9.8168912712034651E-2</v>
-      </c>
-      <c r="B9">
-        <v>12.345303705032707</v>
-      </c>
-      <c r="C9">
-        <v>-0.66771155223550616</v>
-      </c>
-      <c r="D9">
-        <v>-4.3842238455975062E-2</v>
-      </c>
-      <c r="E9">
-        <v>1.9621423804388784E-3</v>
-      </c>
-      <c r="F9">
-        <v>53.615346710119397</v>
-      </c>
-      <c r="G9">
-        <v>-2.1071035750547906E-3</v>
-      </c>
-      <c r="H9">
-        <v>1187.8621825097464</v>
-      </c>
-      <c r="O9" t="s">
-        <v>54</v>
-      </c>
-      <c r="U9" t="s">
-        <v>63</v>
-      </c>
-      <c r="V9">
-        <v>45</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>107</v>
-      </c>
-      <c r="AA9">
-        <v>8.9602332474964276E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>0.11929116538065165</v>
-      </c>
-      <c r="B10">
-        <v>32.787872632822051</v>
-      </c>
-      <c r="C10">
-        <v>-0.16331444965731223</v>
-      </c>
-      <c r="D10">
-        <v>-5.3393064528390849E-2</v>
-      </c>
-      <c r="E10">
-        <v>4.7991706511387995E-4</v>
-      </c>
-      <c r="F10">
-        <v>53.589167460938313</v>
-      </c>
-      <c r="G10">
-        <v>-1.2605431750961838E-4</v>
-      </c>
-      <c r="H10">
-        <v>2282.7844039457045</v>
-      </c>
-      <c r="P10" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>30</v>
-      </c>
-      <c r="R10" t="s">
-        <v>150</v>
-      </c>
-      <c r="U10" t="s">
-        <v>64</v>
-      </c>
-      <c r="V10">
-        <v>15</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA10">
-        <v>1831.9745409498933</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0.14024205540898918</v>
-      </c>
-      <c r="B11">
-        <v>38.142678623492507</v>
-      </c>
-      <c r="C11">
-        <v>0.59598417941665061</v>
-      </c>
-      <c r="D11">
-        <v>-4.9047600796110598E-2</v>
-      </c>
-      <c r="E11">
-        <v>1.7513636598513235E-3</v>
-      </c>
-      <c r="F11">
-        <v>53.563200601284549</v>
-      </c>
-      <c r="G11">
-        <v>1.67871814064406E-3</v>
-      </c>
-      <c r="H11">
-        <v>2568.5006231971997</v>
-      </c>
-      <c r="P11" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q11">
-        <v>7.7915071717360252E-3</v>
-      </c>
-      <c r="U11" t="s">
-        <v>65</v>
-      </c>
-      <c r="V11">
-        <v>2068428</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>109</v>
-      </c>
-      <c r="AA11">
-        <v>546.78577951537659</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>0.16576992529052567</v>
-      </c>
-      <c r="B12">
-        <v>38.960727251071539</v>
-      </c>
-      <c r="C12">
-        <v>1.5839627990373799</v>
-      </c>
-      <c r="D12">
-        <v>-2.1263561117739846E-2</v>
-      </c>
-      <c r="E12">
-        <v>4.6546466331182194E-3</v>
-      </c>
-      <c r="F12">
-        <v>53.531560961461288</v>
-      </c>
-      <c r="G12">
-        <v>1.1857608776918169E-2</v>
-      </c>
-      <c r="H12">
-        <v>2610.7850165843142</v>
-      </c>
-      <c r="P12" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q12">
-        <v>2.3647908810884664</v>
-      </c>
-      <c r="U12" t="s">
-        <v>66</v>
-      </c>
-      <c r="V12">
-        <v>3252.5</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA12">
-        <v>66.792845291262523</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>0.20281596178802641</v>
-      </c>
-      <c r="B13">
-        <v>39.069954535397791</v>
-      </c>
-      <c r="C13">
-        <v>3.0299289531513907</v>
-      </c>
-      <c r="D13">
-        <v>6.4188414534183058E-2</v>
-      </c>
-      <c r="E13">
-        <v>8.9037837262757793E-3</v>
-      </c>
-      <c r="F13">
-        <v>53.485645526405413</v>
-      </c>
-      <c r="G13">
-        <v>4.3387885944673577E-2</v>
-      </c>
-      <c r="H13">
-        <v>2614.4193095130436</v>
-      </c>
-      <c r="P13" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q13">
-        <v>4357255.0535812248</v>
-      </c>
-      <c r="U13" t="s">
-        <v>67</v>
-      </c>
-      <c r="V13">
-        <v>1.4356</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA13">
-        <v>0.14231669665470673</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>0.27159827498415007</v>
-      </c>
-      <c r="B14">
-        <v>39.145783922735184</v>
-      </c>
-      <c r="C14">
-        <v>5.719866076281459</v>
-      </c>
-      <c r="D14">
-        <v>0.36507408947003211</v>
-      </c>
-      <c r="E14">
-        <v>1.6808520631366213E-2</v>
-      </c>
-      <c r="F14">
-        <v>53.400395655349378</v>
-      </c>
-      <c r="G14">
-        <v>0.1610896289032433</v>
-      </c>
-      <c r="H14">
-        <v>2614.4193207207541</v>
-      </c>
-      <c r="P14" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q14">
-        <v>631.96616757961476</v>
-      </c>
-      <c r="U14" t="s">
-        <v>68</v>
-      </c>
-      <c r="V14">
-        <v>238.91946992864425</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA14">
-        <v>16.321321753211024</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>0.61550984096476835</v>
-      </c>
-      <c r="B15">
-        <v>39.507629901115472</v>
-      </c>
-      <c r="C15">
-        <v>19.245577403494039</v>
-      </c>
-      <c r="D15">
-        <v>4.6544599608515602</v>
-      </c>
-      <c r="E15">
-        <v>5.6558201191065055E-2</v>
-      </c>
-      <c r="F15">
-        <v>52.974146300069179</v>
-      </c>
-      <c r="G15">
-        <v>1.8601389068137313</v>
-      </c>
-      <c r="H15">
-        <v>2614.4194804611711</v>
-      </c>
-      <c r="P15" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q15">
-        <v>303.5087857798336</v>
-      </c>
-      <c r="U15" t="s">
-        <v>69</v>
-      </c>
-      <c r="V15">
-        <v>1632.6274728336584</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>113</v>
-      </c>
-      <c r="AA15">
-        <v>12071.729394727032</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2.3350676708678595</v>
-      </c>
-      <c r="B16">
-        <v>40.885651191846868</v>
-      </c>
-      <c r="C16">
-        <v>88.471053010922063</v>
-      </c>
-      <c r="D16">
-        <v>96.927309799530477</v>
-      </c>
-      <c r="E16">
-        <v>0.26026654212654726</v>
-      </c>
-      <c r="F16">
-        <v>50.842899523668208</v>
-      </c>
-      <c r="G16">
-        <v>36.90900105573791</v>
-      </c>
-      <c r="H16">
-        <v>2614.4229008897387</v>
-      </c>
-      <c r="O16" t="s">
-        <v>53</v>
-      </c>
-      <c r="P16">
-        <v>21.283117929796198</v>
-      </c>
-      <c r="U16" t="s">
-        <v>70</v>
-      </c>
-      <c r="V16">
-        <v>1469.3647255502926</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>114</v>
-      </c>
-      <c r="AA16">
-        <v>21.338591027161645</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>4.1350676708678593</v>
-      </c>
-      <c r="B17">
-        <v>41.475889309165005</v>
-      </c>
-      <c r="C17">
-        <v>162.73281170778512</v>
-      </c>
-      <c r="D17">
-        <v>322.85095564515456</v>
-      </c>
-      <c r="E17">
-        <v>0.47995905773358716</v>
-      </c>
-      <c r="F17">
-        <v>48.611951467831119</v>
-      </c>
-      <c r="G17">
-        <v>121.32398628143252</v>
-      </c>
-      <c r="H17">
-        <v>2614.4311483631209</v>
-      </c>
-      <c r="U17" t="s">
-        <v>71</v>
-      </c>
-      <c r="V17">
-        <v>92063</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA17">
-        <v>0.14231669665470673</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>5.9350676708678591</v>
-      </c>
-      <c r="B18">
-        <v>41.099769709888847</v>
-      </c>
-      <c r="C18">
-        <v>237.21022552752751</v>
-      </c>
-      <c r="D18">
-        <v>682.90287959451564</v>
-      </c>
-      <c r="E18">
-        <v>0.70250007265466463</v>
-      </c>
-      <c r="F18">
-        <v>46.381003411994023</v>
-      </c>
-      <c r="G18">
-        <v>253.19772248768462</v>
-      </c>
-      <c r="H18">
-        <v>2614.4439251058693</v>
-      </c>
-      <c r="U18" t="s">
-        <v>72</v>
-      </c>
-      <c r="V18">
-        <v>1.1724846115020683E-2</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA18">
-        <v>4.4325735113785898</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>7.735067670867859</v>
-      </c>
-      <c r="B19">
-        <v>39.39440721349758</v>
-      </c>
-      <c r="C19">
-        <v>310.00321680181412</v>
-      </c>
-      <c r="D19">
-        <v>1175.8390820170303</v>
-      </c>
-      <c r="E19">
-        <v>0.9233055962783604</v>
-      </c>
-      <c r="F19">
-        <v>44.150055356156926</v>
-      </c>
-      <c r="G19">
-        <v>442.08340268117257</v>
-      </c>
-      <c r="H19">
-        <v>2614.460704923978</v>
-      </c>
-      <c r="U19" t="s">
-        <v>73</v>
-      </c>
-      <c r="V19">
-        <v>1.4473248461150208</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA19">
-        <v>12071.729394727032</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>9.503446508989958</v>
-      </c>
-      <c r="B20">
-        <v>32.694573676337711</v>
-      </c>
-      <c r="C20">
-        <v>372.50406278211403</v>
-      </c>
-      <c r="D20">
-        <v>1781.2366794489831</v>
-      </c>
-      <c r="E20">
-        <v>1.1173213403125017</v>
-      </c>
-      <c r="F20">
-        <v>41.958299061216955</v>
-      </c>
-      <c r="G20">
-        <v>831.0606129055767</v>
-      </c>
-      <c r="H20">
-        <v>2614.4802266868842</v>
-      </c>
-      <c r="U20" t="s">
-        <v>74</v>
-      </c>
-      <c r="V20">
-        <v>2635.8007716814773</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>118</v>
-      </c>
-      <c r="AA20">
-        <v>7.4032209766824941</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>11.303446508989959</v>
-      </c>
-      <c r="B21">
-        <v>31.29192208938256</v>
-      </c>
-      <c r="C21">
-        <v>429.87720830998353</v>
-      </c>
-      <c r="D21">
-        <v>2503.7431171989729</v>
-      </c>
-      <c r="E21">
-        <v>1.3005001378925525</v>
-      </c>
-      <c r="F21">
-        <v>39.727351005379859</v>
-      </c>
-      <c r="G21">
-        <v>981.63154213403072</v>
-      </c>
-      <c r="H21">
-        <v>2614.5020279747077</v>
-      </c>
-      <c r="U21" t="s">
-        <v>75</v>
-      </c>
-      <c r="V21">
-        <v>592.58110874133922</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>119</v>
-      </c>
-      <c r="AA21">
-        <v>2.0105798841732372</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>13.103446508989959</v>
-      </c>
-      <c r="B22">
-        <v>30.717596443922417</v>
-      </c>
-      <c r="C22">
-        <v>485.6101317711437</v>
-      </c>
-      <c r="D22">
-        <v>3327.8379963220764</v>
-      </c>
-      <c r="E22">
-        <v>1.4837979384511213</v>
-      </c>
-      <c r="F22">
-        <v>37.49640294954277</v>
-      </c>
-      <c r="G22">
-        <v>1094.8859264552373</v>
-      </c>
-      <c r="H22">
-        <v>2614.5250132930091</v>
-      </c>
-      <c r="U22" t="s">
-        <v>76</v>
-      </c>
-      <c r="V22">
-        <v>8.8045295423009077E-4</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA22">
-        <v>9.4138008608557318</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>14.90344650898996</v>
-      </c>
-      <c r="B23">
-        <v>30.78616506191095</v>
-      </c>
-      <c r="C23">
-        <v>540.86773333256019</v>
-      </c>
-      <c r="D23">
-        <v>4251.6323108320721</v>
-      </c>
-      <c r="E23">
-        <v>1.6715769334284727</v>
-      </c>
-      <c r="F23">
-        <v>35.26545489370568</v>
-      </c>
-      <c r="G23">
-        <v>1182.9063174766882</v>
-      </c>
-      <c r="H23">
-        <v>2614.5485453249394</v>
-      </c>
-      <c r="U23" t="s">
-        <v>77</v>
-      </c>
-      <c r="V23">
-        <v>1.3647048084662576</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z23">
-        <v>53.737018790651931</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>16.703446508989959</v>
-      </c>
-      <c r="B24">
-        <v>32.11927527460405</v>
-      </c>
-      <c r="C24">
-        <v>597.2087865858515</v>
-      </c>
-      <c r="D24">
-        <v>5275.5408889114688</v>
-      </c>
-      <c r="E24">
-        <v>1.8697393776984526</v>
-      </c>
-      <c r="F24">
-        <v>33.034506837868584</v>
-      </c>
-      <c r="G24">
-        <v>1229.4591348585516</v>
-      </c>
-      <c r="H24">
-        <v>2614.5720656243334</v>
-      </c>
-      <c r="U24" t="s">
-        <v>78</v>
-      </c>
-      <c r="V24">
-        <v>3.3481749037418129E-2</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>121</v>
-      </c>
-      <c r="Z24">
-        <v>0.39606063769020622</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>16.910570229076576</v>
-      </c>
-      <c r="B25">
-        <v>32.389892579251153</v>
-      </c>
-      <c r="C25">
-        <v>603.89063214461294</v>
-      </c>
-      <c r="D25">
-        <v>5399.9280999914481</v>
-      </c>
-      <c r="E25">
-        <v>1.893676874471854</v>
-      </c>
-      <c r="F25">
-        <v>32.777794470843588</v>
-      </c>
-      <c r="G25">
-        <v>1231.355343927984</v>
-      </c>
-      <c r="H25">
-        <v>2614.5747495823557</v>
-      </c>
-      <c r="U25" t="s">
-        <v>79</v>
-      </c>
-      <c r="V25">
-        <v>1.3181790959613437</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>17.056344586235362</v>
-      </c>
-      <c r="B26">
-        <v>18.605894766498089</v>
-      </c>
-      <c r="C26">
-        <v>608.42542046287576</v>
-      </c>
-      <c r="D26">
-        <v>5488.3047523584919</v>
-      </c>
-      <c r="E26">
-        <v>1.9100662847745531</v>
-      </c>
-      <c r="F26">
-        <v>32.597119460457876</v>
-      </c>
-      <c r="G26">
-        <v>1232.5342841481561</v>
-      </c>
-      <c r="H26">
-        <v>2158.8106004274941</v>
-      </c>
-      <c r="U26" t="s">
-        <v>80</v>
-      </c>
-      <c r="V26">
-        <v>1.2394155865761627</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>17.202118943394147</v>
-      </c>
-      <c r="B27">
-        <v>-46.870015201803916</v>
-      </c>
-      <c r="C27">
-        <v>602.70752823196938</v>
-      </c>
-      <c r="D27">
-        <v>5576.6521215743205</v>
-      </c>
-      <c r="E27">
-        <v>1.8942712547979834</v>
-      </c>
-      <c r="F27">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G27">
-        <v>1202.7420592611506</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="U27" t="s">
-        <v>81</v>
-      </c>
-      <c r="V27">
-        <v>0.13771284295290698</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>17.373460836350826</v>
-      </c>
-      <c r="B28">
-        <v>-45.733303249099436</v>
-      </c>
-      <c r="C28">
-        <v>594.77556814531465</v>
-      </c>
-      <c r="D28">
-        <v>5679.2387915255722</v>
-      </c>
-      <c r="E28">
-        <v>1.8718207166426761</v>
-      </c>
-      <c r="F28">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G28">
-        <v>1165.8513222407296</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="U28" t="s">
-        <v>82</v>
-      </c>
-      <c r="V28">
-        <v>4.5373593584471848E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>18.037531039975594</v>
-      </c>
-      <c r="B29">
-        <v>-41.69138110803349</v>
-      </c>
-      <c r="C29">
-        <v>565.78312242040852</v>
-      </c>
-      <c r="D29">
-        <v>6064.4370110113141</v>
-      </c>
-      <c r="E29">
-        <v>1.7895178955290192</v>
-      </c>
-      <c r="F29">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G29">
-        <v>1034.6751817872778</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="U29" t="s">
-        <v>83</v>
-      </c>
-      <c r="V29">
-        <v>1.1017027436232558</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>19.452137410531339</v>
-      </c>
-      <c r="B30">
-        <v>-34.595837642179312</v>
-      </c>
-      <c r="C30">
-        <v>512.03882601297448</v>
-      </c>
-      <c r="D30">
-        <v>6825.5995756684415</v>
-      </c>
-      <c r="E30">
-        <v>1.6358813547761384</v>
-      </c>
-      <c r="F30">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G30">
-        <v>804.39711759255351</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="U30" t="s">
-        <v>84</v>
-      </c>
-      <c r="V30">
-        <v>1.5202163514902139E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>21.25213741053134</v>
-      </c>
-      <c r="B31">
-        <v>-28.261666814553486</v>
-      </c>
-      <c r="C31">
-        <v>455.82766095248297</v>
-      </c>
-      <c r="D31">
-        <v>7694.9849689429857</v>
-      </c>
-      <c r="E31">
-        <v>1.4734737590132565</v>
-      </c>
-      <c r="F31">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G31">
-        <v>598.8285655170605</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="U31" t="s">
-        <v>85</v>
-      </c>
-      <c r="V31">
-        <v>3.5218118169203631E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>23.052137410531341</v>
-      </c>
-      <c r="B32">
-        <v>-23.884588947937846</v>
-      </c>
-      <c r="C32">
-        <v>409.13128255754532</v>
-      </c>
-      <c r="D32">
-        <v>8472.2675877965321</v>
-      </c>
-      <c r="E32">
-        <v>1.3367835559465349</v>
-      </c>
-      <c r="F32">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G32">
-        <v>456.77531437367065</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="U32" t="s">
-        <v>86</v>
-      </c>
-      <c r="V32">
-        <v>5.4588192338650305</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>24.852137410531341</v>
-      </c>
-      <c r="B33">
-        <v>-20.727766842799369</v>
-      </c>
-      <c r="C33">
-        <v>369.12358717746218</v>
-      </c>
-      <c r="D33">
-        <v>9171.8447226932258</v>
-      </c>
-      <c r="E33">
-        <v>1.2180033514885484</v>
-      </c>
-      <c r="F33">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G33">
-        <v>354.32412273814867</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="U33" t="s">
-        <v>87</v>
-      </c>
-      <c r="V33">
-        <v>6.6963498074836258E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>26.652137410531342</v>
-      </c>
-      <c r="B34">
-        <v>-18.281792048072234</v>
-      </c>
-      <c r="C34">
-        <v>334.08386769182437</v>
-      </c>
-      <c r="D34">
-        <v>9804.0705657555609</v>
-      </c>
-      <c r="E34">
-        <v>1.1124293896336017</v>
-      </c>
-      <c r="F34">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G34">
-        <v>274.94269924192224</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="U34" t="s">
-        <v>88</v>
-      </c>
-      <c r="V34">
-        <v>2.6363581919226875</v>
-      </c>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>28.452137410531343</v>
-      </c>
-      <c r="B35">
-        <v>-15.882874695346633</v>
-      </c>
-      <c r="C35">
-        <v>303.15823178571509</v>
-      </c>
-      <c r="D35">
-        <v>10376.968961663251</v>
-      </c>
-      <c r="E35">
-        <v>1.0179340621748745</v>
-      </c>
-      <c r="F35">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G35">
-        <v>197.08847330317909</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="U35" t="s">
-        <v>89</v>
-      </c>
-      <c r="V35">
-        <v>17.171897917299866</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>30.252137410531343</v>
-      </c>
-      <c r="B36">
-        <v>-13.620681138868854</v>
-      </c>
-      <c r="C36">
-        <v>276.76593600063137</v>
-      </c>
-      <c r="D36">
-        <v>10898.29171636667</v>
-      </c>
-      <c r="E36">
-        <v>0.93653245577495126</v>
-      </c>
-      <c r="F36">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G36">
-        <v>123.67146789318255</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="U36" t="s">
-        <v>90</v>
-      </c>
-      <c r="V36">
-        <v>10175.742307026649</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>32.052137410531344</v>
-      </c>
-      <c r="B37">
-        <v>-12.545255757248325</v>
-      </c>
-      <c r="C37">
-        <v>253.40503705455333</v>
-      </c>
-      <c r="D37">
-        <v>11375.173560044823</v>
-      </c>
-      <c r="E37">
-        <v>0.85879014375948848</v>
-      </c>
-      <c r="F37">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G37">
-        <v>88.769719174822029</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="U37" t="s">
-        <v>91</v>
-      </c>
-      <c r="V37">
-        <v>216.78369778735134</v>
-      </c>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>33.852137410531341</v>
-      </c>
-      <c r="B38">
-        <v>-11.913389325677002</v>
-      </c>
-      <c r="C38">
-        <v>231.42274302019197</v>
-      </c>
-      <c r="D38">
-        <v>11811.347655406194</v>
-      </c>
-      <c r="E38">
-        <v>0.78429210822964057</v>
-      </c>
-      <c r="F38">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G38">
-        <v>68.263188647303622</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="U38" t="s">
-        <v>92</v>
-      </c>
-      <c r="V38">
-        <v>3.9620382940354082E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>35.652137410531338</v>
-      </c>
-      <c r="B39">
-        <v>-11.424461259597875</v>
-      </c>
-      <c r="C39">
-        <v>210.44098941475278</v>
-      </c>
-      <c r="D39">
-        <v>12208.892952366932</v>
-      </c>
-      <c r="E39">
-        <v>0.71318490608171259</v>
-      </c>
-      <c r="F39">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G39">
-        <v>52.395565662681676</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="U39" t="s">
-        <v>93</v>
-      </c>
-      <c r="V39">
-        <v>2417.7841094874643</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>37.452137410531336</v>
-      </c>
-      <c r="B40">
-        <v>-11.042372606652352</v>
-      </c>
-      <c r="C40">
-        <v>190.23324042993457</v>
-      </c>
-      <c r="D40">
-        <v>12569.397047024524</v>
-      </c>
-      <c r="E40">
-        <v>0.64470080703836308</v>
-      </c>
-      <c r="F40">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G40">
-        <v>39.995298399929744</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="U40" t="s">
-        <v>94</v>
-      </c>
-      <c r="V40">
-        <v>0.26413588626902723</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>39.252137410531333</v>
-      </c>
-      <c r="B41">
-        <v>-10.746204273335103</v>
-      </c>
-      <c r="C41">
-        <v>170.63503794159354</v>
-      </c>
-      <c r="D41">
-        <v>12894.098364664609</v>
-      </c>
-      <c r="E41">
-        <v>0.57828246220977697</v>
-      </c>
-      <c r="F41">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G41">
-        <v>30.383480672326893</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="U41" t="s">
-        <v>95</v>
-      </c>
-      <c r="V41">
-        <v>409.41144253987727</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>41.05213741053133</v>
-      </c>
-      <c r="B42">
-        <v>-10.513747345961264</v>
-      </c>
-      <c r="C42">
-        <v>151.51007090267919</v>
-      </c>
-      <c r="D42">
-        <v>13183.96647457576</v>
-      </c>
-      <c r="E42">
-        <v>0.51346791320296747</v>
-      </c>
-      <c r="F42">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G42">
-        <v>22.839346596917164</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="U42" t="s">
-        <v>96</v>
-      </c>
-      <c r="V42">
-        <v>22.831531676802577</v>
-      </c>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>42.852137410531327</v>
-      </c>
-      <c r="B43">
-        <v>-10.328963280082133</v>
-      </c>
-      <c r="C43">
-        <v>132.75779912235802</v>
-      </c>
-      <c r="D43">
-        <v>13439.757704012083</v>
-      </c>
-      <c r="E43">
-        <v>0.44991642912346169</v>
-      </c>
-      <c r="F43">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G43">
-        <v>16.842382842210025</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="U43" t="s">
-        <v>97</v>
-      </c>
-      <c r="V43">
-        <v>5.8330119607457478</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>44.652137410531324</v>
-      </c>
-      <c r="B44">
-        <v>-10.182331946742487</v>
-      </c>
-      <c r="C44">
-        <v>114.30269799426569</v>
-      </c>
-      <c r="D44">
-        <v>13662.07276396077</v>
-      </c>
-      <c r="E44">
-        <v>0.3873720569392643</v>
-      </c>
-      <c r="F44">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G44">
-        <v>12.083624086910042</v>
-      </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
-      <c r="U44" t="s">
-        <v>98</v>
-      </c>
-      <c r="V44">
-        <v>2.4597556798014728</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>46.452137410531321</v>
-      </c>
-      <c r="B45">
-        <v>-10.065623989412309</v>
-      </c>
-      <c r="C45">
-        <v>96.083941527841247</v>
-      </c>
-      <c r="D45">
-        <v>13851.389235105291</v>
-      </c>
-      <c r="E45">
-        <v>0.32562865725478429</v>
-      </c>
-      <c r="F45">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G45">
-        <v>8.2959956100435139</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>48.252137410531319</v>
-      </c>
-      <c r="B46">
-        <v>-9.9751660909906015</v>
-      </c>
-      <c r="C46">
-        <v>78.050885422714799</v>
-      </c>
-      <c r="D46">
-        <v>14008.086052469687</v>
-      </c>
-      <c r="E46">
-        <v>0.26451459644150027</v>
-      </c>
-      <c r="F46">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G46">
-        <v>5.3602839425840436</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>50.052137410531316</v>
-      </c>
-      <c r="B47">
-        <v>-9.9070354363267334</v>
-      </c>
-      <c r="C47">
-        <v>60.160013731704609</v>
-      </c>
-      <c r="D47">
-        <v>14132.457583714615</v>
-      </c>
-      <c r="E47">
-        <v>0.20388239887315632</v>
-      </c>
-      <c r="F47">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G47">
-        <v>3.1491784305376442</v>
-      </c>
-      <c r="H47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>51.852137410531313</v>
-      </c>
-      <c r="B48">
-        <v>-9.858111201092731</v>
-      </c>
-      <c r="C48">
-        <v>42.374021655029509</v>
-      </c>
-      <c r="D48">
-        <v>14224.725010828279</v>
-      </c>
-      <c r="E48">
-        <v>0.143605638513635</v>
-      </c>
-      <c r="F48">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G48">
-        <v>1.5613961505601874</v>
-      </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>53.65213741053131</v>
-      </c>
-      <c r="B49">
-        <v>-9.8264607938878239</v>
-      </c>
-      <c r="C49">
-        <v>24.660403301048571</v>
-      </c>
-      <c r="D49">
-        <v>14285.047459530417</v>
-      </c>
-      <c r="E49">
-        <v>8.3574152835467194E-2</v>
-      </c>
-      <c r="F49">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G49">
-        <v>0.53421697292637893</v>
-      </c>
-      <c r="H49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>55.452137410531307</v>
-      </c>
-      <c r="B50">
-        <v>-9.811334504012958</v>
-      </c>
-      <c r="C50">
-        <v>6.9888533117958538</v>
-      </c>
-      <c r="D50">
-        <v>14313.527701478539</v>
-      </c>
-      <c r="E50">
-        <v>2.3685236923917299E-2</v>
-      </c>
-      <c r="F50">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G50">
-        <v>4.3309860934955945E-2</v>
-      </c>
-      <c r="H50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>56.674231989357395</v>
-      </c>
-      <c r="B51">
-        <v>-9.8093313640016451</v>
-      </c>
-      <c r="C51">
-        <v>-4.9999999999999503</v>
-      </c>
-      <c r="D51">
-        <v>14314.742748730931</v>
-      </c>
-      <c r="E51">
-        <v>1.6945009336467896E-2</v>
-      </c>
-      <c r="F51">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G51">
-        <v>-2.1699846402632925E-2</v>
-      </c>
-      <c r="H51">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA51"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2:AA24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H1" t="s">
-        <v>131</v>
-      </c>
-      <c r="K1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" t="s">
-        <v>46</v>
-      </c>
-      <c r="U1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>-9.8077912979337363</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>53.737018790651931</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0.11868906443783601</v>
-      </c>
-      <c r="K2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2">
-        <v>46964.380599746386</v>
-      </c>
-      <c r="O2" t="s">
-        <v>47</v>
-      </c>
-      <c r="U2" t="s">
-        <v>57</v>
-      </c>
-      <c r="V2">
-        <v>300</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z2">
-        <v>32.453900860855732</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1.2927625756433149E-4</v>
-      </c>
-      <c r="B3">
-        <v>-9.8077625538079936</v>
-      </c>
-      <c r="C3">
-        <v>-1.267912700009145E-3</v>
-      </c>
-      <c r="D3">
-        <v>-8.1955544419449058E-8</v>
-      </c>
-      <c r="E3">
-        <v>3.7259000016658353E-6</v>
-      </c>
-      <c r="F3">
-        <v>53.736858563643331</v>
-      </c>
-      <c r="G3">
-        <v>-7.5977496586787575E-9</v>
-      </c>
-      <c r="H3">
-        <v>0.12023332196588275</v>
-      </c>
-      <c r="K3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3">
-        <v>1.9100662847745531</v>
-      </c>
-      <c r="P3" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>28</v>
-      </c>
-      <c r="R3" t="s">
-        <v>29</v>
-      </c>
-      <c r="U3" t="s">
-        <v>58</v>
-      </c>
-      <c r="V3">
-        <v>4</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>7.7565754538598888E-4</v>
-      </c>
-      <c r="B4">
-        <v>-9.8076131197978125</v>
-      </c>
-      <c r="C4">
-        <v>-7.6074191152028653E-3</v>
-      </c>
-      <c r="D4">
-        <v>-2.9503849512409596E-6</v>
-      </c>
-      <c r="E4">
-        <v>2.2355232259197035E-5</v>
-      </c>
-      <c r="F4">
-        <v>53.736057428600333</v>
-      </c>
-      <c r="G4">
-        <v>-2.7351488294879236E-7</v>
-      </c>
-      <c r="H4">
-        <v>0.12826125810512462</v>
-      </c>
-      <c r="K4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4">
-        <v>4.2279193995071358</v>
-      </c>
-      <c r="P4" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q4">
-        <v>2.6105E-2</v>
-      </c>
-      <c r="U4" t="s">
-        <v>59</v>
-      </c>
-      <c r="V4">
-        <v>0.9</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>102</v>
-      </c>
-      <c r="Z4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4.0075639844942756E-3</v>
-      </c>
-      <c r="B5">
-        <v>-9.8067021435395496</v>
-      </c>
-      <c r="C5">
-        <v>-3.9303314216520127E-2</v>
-      </c>
-      <c r="D5">
-        <v>-7.8756727076969679E-5</v>
-      </c>
-      <c r="E5">
-        <v>1.1549708301983543E-4</v>
-      </c>
-      <c r="F5">
-        <v>53.732051753385349</v>
-      </c>
-      <c r="G5">
-        <v>-7.3007020691739814E-6</v>
-      </c>
-      <c r="H5">
-        <v>0.17719329330612149</v>
-      </c>
-      <c r="K5" t="s">
-        <v>44</v>
-      </c>
-      <c r="L5">
-        <v>277.07370707650551</v>
-      </c>
-      <c r="P5" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q5">
-        <v>18.918327048707731</v>
-      </c>
-      <c r="U5" t="s">
-        <v>53</v>
-      </c>
-      <c r="V5">
-        <v>3</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2.0167096180035708E-2</v>
-      </c>
-      <c r="B6">
-        <v>-9.7933985270463353</v>
-      </c>
-      <c r="C6">
-        <v>-0.19769530261646528</v>
-      </c>
-      <c r="D6">
-        <v>-1.9939277736046404E-3</v>
-      </c>
-      <c r="E6">
-        <v>5.8094923394804159E-4</v>
-      </c>
-      <c r="F6">
-        <v>53.712023377310416</v>
-      </c>
-      <c r="G6">
-        <v>-1.8471367947272326E-4</v>
-      </c>
-      <c r="H6">
-        <v>0.89151398970559792</v>
-      </c>
-      <c r="K6" t="s">
-        <v>45</v>
-      </c>
-      <c r="L6">
-        <v>864.56508502112433</v>
-      </c>
-      <c r="P6" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q6">
-        <v>5887436.804562035</v>
-      </c>
-      <c r="U6" t="s">
-        <v>60</v>
-      </c>
-      <c r="V6">
-        <v>300</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>104</v>
-      </c>
-      <c r="Z6">
-        <v>1.8241469247509919E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5.0193414275433001E-2</v>
-      </c>
-      <c r="B7">
-        <v>-9.4776570054937466</v>
-      </c>
-      <c r="C7">
-        <v>-0.4890847162890341</v>
-      </c>
-      <c r="D7">
-        <v>-1.2325530476494321E-2</v>
-      </c>
-      <c r="E7">
-        <v>1.437228676623566E-3</v>
-      </c>
-      <c r="F7">
-        <v>53.674808290655484</v>
-      </c>
-      <c r="G7">
-        <v>-1.1305114691530782E-3</v>
-      </c>
-      <c r="H7">
-        <v>17.837316005396374</v>
-      </c>
-      <c r="P7" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q7">
-        <v>853.90017992824039</v>
-      </c>
-      <c r="U7" t="s">
-        <v>61</v>
-      </c>
-      <c r="V7">
-        <v>45</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7.4181163493733826E-2</v>
-      </c>
-      <c r="B8">
-        <v>-6.3831947930205857</v>
-      </c>
-      <c r="C8">
-        <v>-0.69221630572312165</v>
-      </c>
-      <c r="D8">
-        <v>-2.6631639443629708E-2</v>
-      </c>
-      <c r="E8">
-        <v>2.0341526352147719E-3</v>
-      </c>
-      <c r="F8">
-        <v>53.645077500387444</v>
-      </c>
-      <c r="G8">
-        <v>-2.2645975682007743E-3</v>
-      </c>
-      <c r="H8">
-        <v>183.82896630957376</v>
-      </c>
-      <c r="P8" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q8">
-        <v>724.70128514490443</v>
-      </c>
-      <c r="U8" t="s">
-        <v>62</v>
-      </c>
-      <c r="V8">
-        <v>8</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA8">
-        <v>3.0020749999999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>9.8168912712034651E-2</v>
-      </c>
-      <c r="B9">
-        <v>12.345303705032707</v>
-      </c>
-      <c r="C9">
-        <v>-0.66771155223550616</v>
-      </c>
-      <c r="D9">
-        <v>-4.3842238455975062E-2</v>
-      </c>
-      <c r="E9">
-        <v>1.9621423804388784E-3</v>
-      </c>
-      <c r="F9">
-        <v>53.615346710119397</v>
-      </c>
-      <c r="G9">
-        <v>-2.1071035750547906E-3</v>
-      </c>
-      <c r="H9">
-        <v>1187.8621825097464</v>
-      </c>
-      <c r="O9" t="s">
-        <v>54</v>
-      </c>
-      <c r="U9" t="s">
-        <v>63</v>
-      </c>
-      <c r="V9">
-        <v>45</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>107</v>
-      </c>
-      <c r="AA9">
-        <v>8.9602332474964276E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>0.11929116538065165</v>
-      </c>
-      <c r="B10">
-        <v>32.787872632822051</v>
-      </c>
-      <c r="C10">
-        <v>-0.16331444965731223</v>
-      </c>
-      <c r="D10">
-        <v>-5.3393064528390849E-2</v>
-      </c>
-      <c r="E10">
-        <v>4.7991706511387995E-4</v>
-      </c>
-      <c r="F10">
-        <v>53.589167460938313</v>
-      </c>
-      <c r="G10">
-        <v>-1.2605431750961838E-4</v>
-      </c>
-      <c r="H10">
-        <v>2282.7844039457045</v>
-      </c>
-      <c r="P10" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>30</v>
-      </c>
-      <c r="R10" t="s">
-        <v>150</v>
-      </c>
-      <c r="U10" t="s">
-        <v>64</v>
-      </c>
-      <c r="V10">
-        <v>15</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA10">
-        <v>1831.9745409498933</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0.14024205540898918</v>
-      </c>
-      <c r="B11">
-        <v>38.142678623492507</v>
-      </c>
-      <c r="C11">
-        <v>0.59598417941665061</v>
-      </c>
-      <c r="D11">
-        <v>-4.9047600796110598E-2</v>
-      </c>
-      <c r="E11">
-        <v>1.7513636598513235E-3</v>
-      </c>
-      <c r="F11">
-        <v>53.563200601284549</v>
-      </c>
-      <c r="G11">
-        <v>1.67871814064406E-3</v>
-      </c>
-      <c r="H11">
-        <v>2568.5006231971997</v>
-      </c>
-      <c r="P11" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q11">
-        <v>7.7915071717360252E-3</v>
-      </c>
-      <c r="U11" t="s">
-        <v>65</v>
-      </c>
-      <c r="V11">
-        <v>2068428</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>109</v>
-      </c>
-      <c r="AA11">
-        <v>546.78577951537659</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>0.16576992529052567</v>
-      </c>
-      <c r="B12">
-        <v>38.960727251071539</v>
-      </c>
-      <c r="C12">
-        <v>1.5839627990373799</v>
-      </c>
-      <c r="D12">
-        <v>-2.1263561117739846E-2</v>
-      </c>
-      <c r="E12">
-        <v>4.6546466331182194E-3</v>
-      </c>
-      <c r="F12">
-        <v>53.531560961461288</v>
-      </c>
-      <c r="G12">
-        <v>1.1857608776918169E-2</v>
-      </c>
-      <c r="H12">
-        <v>2610.7850165843142</v>
-      </c>
-      <c r="P12" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q12">
-        <v>2.3647908810884664</v>
-      </c>
-      <c r="U12" t="s">
-        <v>66</v>
-      </c>
-      <c r="V12">
-        <v>3252.5</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA12">
-        <v>66.792845291262523</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>0.20281596178802641</v>
-      </c>
-      <c r="B13">
-        <v>39.069954535397791</v>
-      </c>
-      <c r="C13">
-        <v>3.0299289531513907</v>
-      </c>
-      <c r="D13">
-        <v>6.4188414534183058E-2</v>
-      </c>
-      <c r="E13">
-        <v>8.9037837262757793E-3</v>
-      </c>
-      <c r="F13">
-        <v>53.485645526405413</v>
-      </c>
-      <c r="G13">
-        <v>4.3387885944673577E-2</v>
-      </c>
-      <c r="H13">
-        <v>2614.4193095130436</v>
-      </c>
-      <c r="P13" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q13">
-        <v>4357255.0535812248</v>
-      </c>
-      <c r="U13" t="s">
-        <v>67</v>
-      </c>
-      <c r="V13">
-        <v>1.4356</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA13">
-        <v>0.14231669665470673</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>0.27159827498415007</v>
-      </c>
-      <c r="B14">
-        <v>39.145783922735184</v>
-      </c>
-      <c r="C14">
-        <v>5.719866076281459</v>
-      </c>
-      <c r="D14">
-        <v>0.36507408947003211</v>
-      </c>
-      <c r="E14">
-        <v>1.6808520631366213E-2</v>
-      </c>
-      <c r="F14">
-        <v>53.400395655349378</v>
-      </c>
-      <c r="G14">
-        <v>0.1610896289032433</v>
-      </c>
-      <c r="H14">
-        <v>2614.4193207207541</v>
-      </c>
-      <c r="P14" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q14">
-        <v>631.96616757961476</v>
-      </c>
-      <c r="U14" t="s">
-        <v>68</v>
-      </c>
-      <c r="V14">
-        <v>238.91946992864425</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA14">
-        <v>16.321321753211024</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>0.61550984096476835</v>
-      </c>
-      <c r="B15">
-        <v>39.507629901115472</v>
-      </c>
-      <c r="C15">
-        <v>19.245577403494039</v>
-      </c>
-      <c r="D15">
-        <v>4.6544599608515602</v>
-      </c>
-      <c r="E15">
-        <v>5.6558201191065055E-2</v>
-      </c>
-      <c r="F15">
-        <v>52.974146300069179</v>
-      </c>
-      <c r="G15">
-        <v>1.8601389068137313</v>
-      </c>
-      <c r="H15">
-        <v>2614.4194804611711</v>
-      </c>
-      <c r="P15" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q15">
-        <v>303.5087857798336</v>
-      </c>
-      <c r="U15" t="s">
-        <v>69</v>
-      </c>
-      <c r="V15">
-        <v>1632.6274728336584</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>113</v>
-      </c>
-      <c r="AA15">
-        <v>12071.729394727032</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2.3350676708678595</v>
-      </c>
-      <c r="B16">
-        <v>40.885651191846868</v>
-      </c>
-      <c r="C16">
-        <v>88.471053010922063</v>
-      </c>
-      <c r="D16">
-        <v>96.927309799530477</v>
-      </c>
-      <c r="E16">
-        <v>0.26026654212654726</v>
-      </c>
-      <c r="F16">
-        <v>50.842899523668208</v>
-      </c>
-      <c r="G16">
-        <v>36.90900105573791</v>
-      </c>
-      <c r="H16">
-        <v>2614.4229008897387</v>
-      </c>
-      <c r="O16" t="s">
-        <v>53</v>
-      </c>
-      <c r="P16">
-        <v>21.283117929796198</v>
-      </c>
-      <c r="U16" t="s">
-        <v>70</v>
-      </c>
-      <c r="V16">
-        <v>1469.3647255502926</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>114</v>
-      </c>
-      <c r="AA16">
-        <v>21.338591027161645</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>4.1350676708678593</v>
-      </c>
-      <c r="B17">
-        <v>41.475889309165005</v>
-      </c>
-      <c r="C17">
-        <v>162.73281170778512</v>
-      </c>
-      <c r="D17">
-        <v>322.85095564515456</v>
-      </c>
-      <c r="E17">
-        <v>0.47995905773358716</v>
-      </c>
-      <c r="F17">
-        <v>48.611951467831119</v>
-      </c>
-      <c r="G17">
-        <v>121.32398628143252</v>
-      </c>
-      <c r="H17">
-        <v>2614.4311483631209</v>
-      </c>
-      <c r="U17" t="s">
-        <v>71</v>
-      </c>
-      <c r="V17">
-        <v>92063</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA17">
-        <v>0.14231669665470673</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>5.9350676708678591</v>
-      </c>
-      <c r="B18">
-        <v>41.099769709888847</v>
-      </c>
-      <c r="C18">
-        <v>237.21022552752751</v>
-      </c>
-      <c r="D18">
-        <v>682.90287959451564</v>
-      </c>
-      <c r="E18">
-        <v>0.70250007265466463</v>
-      </c>
-      <c r="F18">
-        <v>46.381003411994023</v>
-      </c>
-      <c r="G18">
-        <v>253.19772248768462</v>
-      </c>
-      <c r="H18">
-        <v>2614.4439251058693</v>
-      </c>
-      <c r="U18" t="s">
-        <v>72</v>
-      </c>
-      <c r="V18">
-        <v>1.1724846115020683E-2</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA18">
-        <v>4.4325735113785898</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>7.735067670867859</v>
-      </c>
-      <c r="B19">
-        <v>39.39440721349758</v>
-      </c>
-      <c r="C19">
-        <v>310.00321680181412</v>
-      </c>
-      <c r="D19">
-        <v>1175.8390820170303</v>
-      </c>
-      <c r="E19">
-        <v>0.9233055962783604</v>
-      </c>
-      <c r="F19">
-        <v>44.150055356156926</v>
-      </c>
-      <c r="G19">
-        <v>442.08340268117257</v>
-      </c>
-      <c r="H19">
-        <v>2614.460704923978</v>
-      </c>
-      <c r="U19" t="s">
-        <v>73</v>
-      </c>
-      <c r="V19">
-        <v>1.4473248461150208</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA19">
-        <v>12071.729394727032</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>9.503446508989958</v>
-      </c>
-      <c r="B20">
-        <v>32.694573676337711</v>
-      </c>
-      <c r="C20">
-        <v>372.50406278211403</v>
-      </c>
-      <c r="D20">
-        <v>1781.2366794489831</v>
-      </c>
-      <c r="E20">
-        <v>1.1173213403125017</v>
-      </c>
-      <c r="F20">
-        <v>41.958299061216955</v>
-      </c>
-      <c r="G20">
-        <v>831.0606129055767</v>
-      </c>
-      <c r="H20">
-        <v>2614.4802266868842</v>
-      </c>
-      <c r="U20" t="s">
-        <v>74</v>
-      </c>
-      <c r="V20">
-        <v>2635.8007716814773</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>118</v>
-      </c>
-      <c r="AA20">
-        <v>7.4032209766824941</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>11.303446508989959</v>
-      </c>
-      <c r="B21">
-        <v>31.29192208938256</v>
-      </c>
-      <c r="C21">
-        <v>429.87720830998353</v>
-      </c>
-      <c r="D21">
-        <v>2503.7431171989729</v>
-      </c>
-      <c r="E21">
-        <v>1.3005001378925525</v>
-      </c>
-      <c r="F21">
-        <v>39.727351005379859</v>
-      </c>
-      <c r="G21">
-        <v>981.63154213403072</v>
-      </c>
-      <c r="H21">
-        <v>2614.5020279747077</v>
-      </c>
-      <c r="U21" t="s">
-        <v>75</v>
-      </c>
-      <c r="V21">
-        <v>592.58110874133922</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>119</v>
-      </c>
-      <c r="AA21">
-        <v>2.0105798841732372</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>13.103446508989959</v>
-      </c>
-      <c r="B22">
-        <v>30.717596443922417</v>
-      </c>
-      <c r="C22">
-        <v>485.6101317711437</v>
-      </c>
-      <c r="D22">
-        <v>3327.8379963220764</v>
-      </c>
-      <c r="E22">
-        <v>1.4837979384511213</v>
-      </c>
-      <c r="F22">
-        <v>37.49640294954277</v>
-      </c>
-      <c r="G22">
-        <v>1094.8859264552373</v>
-      </c>
-      <c r="H22">
-        <v>2614.5250132930091</v>
-      </c>
-      <c r="U22" t="s">
-        <v>76</v>
-      </c>
-      <c r="V22">
-        <v>8.8045295423009077E-4</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA22">
-        <v>9.4138008608557318</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>14.90344650898996</v>
-      </c>
-      <c r="B23">
-        <v>30.78616506191095</v>
-      </c>
-      <c r="C23">
-        <v>540.86773333256019</v>
-      </c>
-      <c r="D23">
-        <v>4251.6323108320721</v>
-      </c>
-      <c r="E23">
-        <v>1.6715769334284727</v>
-      </c>
-      <c r="F23">
-        <v>35.26545489370568</v>
-      </c>
-      <c r="G23">
-        <v>1182.9063174766882</v>
-      </c>
-      <c r="H23">
-        <v>2614.5485453249394</v>
-      </c>
-      <c r="U23" t="s">
-        <v>77</v>
-      </c>
-      <c r="V23">
-        <v>1.3647048084662576</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z23">
-        <v>53.737018790651931</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>16.703446508989959</v>
-      </c>
-      <c r="B24">
-        <v>32.11927527460405</v>
-      </c>
-      <c r="C24">
-        <v>597.2087865858515</v>
-      </c>
-      <c r="D24">
-        <v>5275.5408889114688</v>
-      </c>
-      <c r="E24">
-        <v>1.8697393776984526</v>
-      </c>
-      <c r="F24">
-        <v>33.034506837868584</v>
-      </c>
-      <c r="G24">
-        <v>1229.4591348585516</v>
-      </c>
-      <c r="H24">
-        <v>2614.5720656243334</v>
-      </c>
-      <c r="U24" t="s">
-        <v>78</v>
-      </c>
-      <c r="V24">
-        <v>3.3481749037418129E-2</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>121</v>
-      </c>
-      <c r="Z24">
-        <v>0.39606063769020622</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>16.910570229076576</v>
-      </c>
-      <c r="B25">
-        <v>32.389892579251153</v>
-      </c>
-      <c r="C25">
-        <v>603.89063214461294</v>
-      </c>
-      <c r="D25">
-        <v>5399.9280999914481</v>
-      </c>
-      <c r="E25">
-        <v>1.893676874471854</v>
-      </c>
-      <c r="F25">
-        <v>32.777794470843588</v>
-      </c>
-      <c r="G25">
-        <v>1231.355343927984</v>
-      </c>
-      <c r="H25">
-        <v>2614.5747495823557</v>
-      </c>
-      <c r="U25" t="s">
-        <v>79</v>
-      </c>
-      <c r="V25">
-        <v>1.3181790959613437</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>17.056344586235362</v>
-      </c>
-      <c r="B26">
-        <v>18.605894766498089</v>
-      </c>
-      <c r="C26">
-        <v>608.42542046287576</v>
-      </c>
-      <c r="D26">
-        <v>5488.3047523584919</v>
-      </c>
-      <c r="E26">
-        <v>1.9100662847745531</v>
-      </c>
-      <c r="F26">
-        <v>32.597119460457876</v>
-      </c>
-      <c r="G26">
-        <v>1232.5342841481561</v>
-      </c>
-      <c r="H26">
-        <v>2158.8106004274941</v>
-      </c>
-      <c r="U26" t="s">
-        <v>80</v>
-      </c>
-      <c r="V26">
-        <v>1.2394155865761627</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>17.202118943394147</v>
-      </c>
-      <c r="B27">
-        <v>-46.870015201803916</v>
-      </c>
-      <c r="C27">
-        <v>602.70752823196938</v>
-      </c>
-      <c r="D27">
-        <v>5576.6521215743205</v>
-      </c>
-      <c r="E27">
-        <v>1.8942712547979834</v>
-      </c>
-      <c r="F27">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G27">
-        <v>1202.7420592611506</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="U27" t="s">
-        <v>81</v>
-      </c>
-      <c r="V27">
-        <v>0.13771284295290698</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>17.373460836350826</v>
-      </c>
-      <c r="B28">
-        <v>-45.733303249099436</v>
-      </c>
-      <c r="C28">
-        <v>594.77556814531465</v>
-      </c>
-      <c r="D28">
-        <v>5679.2387915255722</v>
-      </c>
-      <c r="E28">
-        <v>1.8718207166426761</v>
-      </c>
-      <c r="F28">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G28">
-        <v>1165.8513222407296</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="U28" t="s">
-        <v>82</v>
-      </c>
-      <c r="V28">
-        <v>4.5373593584471848E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>18.037531039975594</v>
-      </c>
-      <c r="B29">
-        <v>-41.69138110803349</v>
-      </c>
-      <c r="C29">
-        <v>565.78312242040852</v>
-      </c>
-      <c r="D29">
-        <v>6064.4370110113141</v>
-      </c>
-      <c r="E29">
-        <v>1.7895178955290192</v>
-      </c>
-      <c r="F29">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G29">
-        <v>1034.6751817872778</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="U29" t="s">
-        <v>83</v>
-      </c>
-      <c r="V29">
-        <v>1.1017027436232558</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>19.452137410531339</v>
-      </c>
-      <c r="B30">
-        <v>-34.595837642179312</v>
-      </c>
-      <c r="C30">
-        <v>512.03882601297448</v>
-      </c>
-      <c r="D30">
-        <v>6825.5995756684415</v>
-      </c>
-      <c r="E30">
-        <v>1.6358813547761384</v>
-      </c>
-      <c r="F30">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G30">
-        <v>804.39711759255351</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="U30" t="s">
-        <v>84</v>
-      </c>
-      <c r="V30">
-        <v>1.5202163514902139E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>21.25213741053134</v>
-      </c>
-      <c r="B31">
-        <v>-28.261666814553486</v>
-      </c>
-      <c r="C31">
-        <v>455.82766095248297</v>
-      </c>
-      <c r="D31">
-        <v>7694.9849689429857</v>
-      </c>
-      <c r="E31">
-        <v>1.4734737590132565</v>
-      </c>
-      <c r="F31">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G31">
-        <v>598.8285655170605</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="U31" t="s">
-        <v>85</v>
-      </c>
-      <c r="V31">
-        <v>3.5218118169203631E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>23.052137410531341</v>
-      </c>
-      <c r="B32">
-        <v>-23.884588947937846</v>
-      </c>
-      <c r="C32">
-        <v>409.13128255754532</v>
-      </c>
-      <c r="D32">
-        <v>8472.2675877965321</v>
-      </c>
-      <c r="E32">
-        <v>1.3367835559465349</v>
-      </c>
-      <c r="F32">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G32">
-        <v>456.77531437367065</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="U32" t="s">
-        <v>86</v>
-      </c>
-      <c r="V32">
-        <v>5.4588192338650305</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>24.852137410531341</v>
-      </c>
-      <c r="B33">
-        <v>-20.727766842799369</v>
-      </c>
-      <c r="C33">
-        <v>369.12358717746218</v>
-      </c>
-      <c r="D33">
-        <v>9171.8447226932258</v>
-      </c>
-      <c r="E33">
-        <v>1.2180033514885484</v>
-      </c>
-      <c r="F33">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G33">
-        <v>354.32412273814867</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="U33" t="s">
-        <v>87</v>
-      </c>
-      <c r="V33">
-        <v>6.6963498074836258E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>26.652137410531342</v>
-      </c>
-      <c r="B34">
-        <v>-18.281792048072234</v>
-      </c>
-      <c r="C34">
-        <v>334.08386769182437</v>
-      </c>
-      <c r="D34">
-        <v>9804.0705657555609</v>
-      </c>
-      <c r="E34">
-        <v>1.1124293896336017</v>
-      </c>
-      <c r="F34">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G34">
-        <v>274.94269924192224</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="U34" t="s">
-        <v>88</v>
-      </c>
-      <c r="V34">
-        <v>2.6363581919226875</v>
-      </c>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>28.452137410531343</v>
-      </c>
-      <c r="B35">
-        <v>-15.882874695346633</v>
-      </c>
-      <c r="C35">
-        <v>303.15823178571509</v>
-      </c>
-      <c r="D35">
-        <v>10376.968961663251</v>
-      </c>
-      <c r="E35">
-        <v>1.0179340621748745</v>
-      </c>
-      <c r="F35">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G35">
-        <v>197.08847330317909</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="U35" t="s">
-        <v>89</v>
-      </c>
-      <c r="V35">
-        <v>17.171897917299866</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>30.252137410531343</v>
-      </c>
-      <c r="B36">
-        <v>-13.620681138868854</v>
-      </c>
-      <c r="C36">
-        <v>276.76593600063137</v>
-      </c>
-      <c r="D36">
-        <v>10898.29171636667</v>
-      </c>
-      <c r="E36">
-        <v>0.93653245577495126</v>
-      </c>
-      <c r="F36">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G36">
-        <v>123.67146789318255</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="U36" t="s">
-        <v>90</v>
-      </c>
-      <c r="V36">
-        <v>10175.742307026649</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>32.052137410531344</v>
-      </c>
-      <c r="B37">
-        <v>-12.545255757248325</v>
-      </c>
-      <c r="C37">
-        <v>253.40503705455333</v>
-      </c>
-      <c r="D37">
-        <v>11375.173560044823</v>
-      </c>
-      <c r="E37">
-        <v>0.85879014375948848</v>
-      </c>
-      <c r="F37">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G37">
-        <v>88.769719174822029</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="U37" t="s">
-        <v>91</v>
-      </c>
-      <c r="V37">
-        <v>216.78369778735134</v>
-      </c>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>33.852137410531341</v>
-      </c>
-      <c r="B38">
-        <v>-11.913389325677002</v>
-      </c>
-      <c r="C38">
-        <v>231.42274302019197</v>
-      </c>
-      <c r="D38">
-        <v>11811.347655406194</v>
-      </c>
-      <c r="E38">
-        <v>0.78429210822964057</v>
-      </c>
-      <c r="F38">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G38">
-        <v>68.263188647303622</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="U38" t="s">
-        <v>92</v>
-      </c>
-      <c r="V38">
-        <v>3.9620382940354082E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>35.652137410531338</v>
-      </c>
-      <c r="B39">
-        <v>-11.424461259597875</v>
-      </c>
-      <c r="C39">
-        <v>210.44098941475278</v>
-      </c>
-      <c r="D39">
-        <v>12208.892952366932</v>
-      </c>
-      <c r="E39">
-        <v>0.71318490608171259</v>
-      </c>
-      <c r="F39">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G39">
-        <v>52.395565662681676</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="U39" t="s">
-        <v>93</v>
-      </c>
-      <c r="V39">
-        <v>2417.7841094874643</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>37.452137410531336</v>
-      </c>
-      <c r="B40">
-        <v>-11.042372606652352</v>
-      </c>
-      <c r="C40">
-        <v>190.23324042993457</v>
-      </c>
-      <c r="D40">
-        <v>12569.397047024524</v>
-      </c>
-      <c r="E40">
-        <v>0.64470080703836308</v>
-      </c>
-      <c r="F40">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G40">
-        <v>39.995298399929744</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="U40" t="s">
-        <v>94</v>
-      </c>
-      <c r="V40">
-        <v>0.26413588626902723</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>39.252137410531333</v>
-      </c>
-      <c r="B41">
-        <v>-10.746204273335103</v>
-      </c>
-      <c r="C41">
-        <v>170.63503794159354</v>
-      </c>
-      <c r="D41">
-        <v>12894.098364664609</v>
-      </c>
-      <c r="E41">
-        <v>0.57828246220977697</v>
-      </c>
-      <c r="F41">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G41">
-        <v>30.383480672326893</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="U41" t="s">
-        <v>95</v>
-      </c>
-      <c r="V41">
-        <v>409.41144253987727</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>41.05213741053133</v>
-      </c>
-      <c r="B42">
-        <v>-10.513747345961264</v>
-      </c>
-      <c r="C42">
-        <v>151.51007090267919</v>
-      </c>
-      <c r="D42">
-        <v>13183.96647457576</v>
-      </c>
-      <c r="E42">
-        <v>0.51346791320296747</v>
-      </c>
-      <c r="F42">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G42">
-        <v>22.839346596917164</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="U42" t="s">
-        <v>96</v>
-      </c>
-      <c r="V42">
-        <v>22.831531676802577</v>
-      </c>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>42.852137410531327</v>
-      </c>
-      <c r="B43">
-        <v>-10.328963280082133</v>
-      </c>
-      <c r="C43">
-        <v>132.75779912235802</v>
-      </c>
-      <c r="D43">
-        <v>13439.757704012083</v>
-      </c>
-      <c r="E43">
-        <v>0.44991642912346169</v>
-      </c>
-      <c r="F43">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G43">
-        <v>16.842382842210025</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="U43" t="s">
-        <v>97</v>
-      </c>
-      <c r="V43">
-        <v>5.8330119607457478</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>44.652137410531324</v>
-      </c>
-      <c r="B44">
-        <v>-10.182331946742487</v>
-      </c>
-      <c r="C44">
-        <v>114.30269799426569</v>
-      </c>
-      <c r="D44">
-        <v>13662.07276396077</v>
-      </c>
-      <c r="E44">
-        <v>0.3873720569392643</v>
-      </c>
-      <c r="F44">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G44">
-        <v>12.083624086910042</v>
-      </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
-      <c r="U44" t="s">
-        <v>98</v>
-      </c>
-      <c r="V44">
-        <v>2.4597556798014728</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>46.452137410531321</v>
-      </c>
-      <c r="B45">
-        <v>-10.065623989412309</v>
-      </c>
-      <c r="C45">
-        <v>96.083941527841247</v>
-      </c>
-      <c r="D45">
-        <v>13851.389235105291</v>
-      </c>
-      <c r="E45">
-        <v>0.32562865725478429</v>
-      </c>
-      <c r="F45">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G45">
-        <v>8.2959956100435139</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>48.252137410531319</v>
-      </c>
-      <c r="B46">
-        <v>-9.9751660909906015</v>
-      </c>
-      <c r="C46">
-        <v>78.050885422714799</v>
-      </c>
-      <c r="D46">
-        <v>14008.086052469687</v>
-      </c>
-      <c r="E46">
-        <v>0.26451459644150027</v>
-      </c>
-      <c r="F46">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G46">
-        <v>5.3602839425840436</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>50.052137410531316</v>
-      </c>
-      <c r="B47">
-        <v>-9.9070354363267334</v>
-      </c>
-      <c r="C47">
-        <v>60.160013731704609</v>
-      </c>
-      <c r="D47">
-        <v>14132.457583714615</v>
-      </c>
-      <c r="E47">
-        <v>0.20388239887315632</v>
-      </c>
-      <c r="F47">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G47">
-        <v>3.1491784305376442</v>
-      </c>
-      <c r="H47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>51.852137410531313</v>
-      </c>
-      <c r="B48">
-        <v>-9.858111201092731</v>
-      </c>
-      <c r="C48">
-        <v>42.374021655029509</v>
-      </c>
-      <c r="D48">
-        <v>14224.725010828279</v>
-      </c>
-      <c r="E48">
-        <v>0.143605638513635</v>
-      </c>
-      <c r="F48">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G48">
-        <v>1.5613961505601874</v>
-      </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>53.65213741053131</v>
-      </c>
-      <c r="B49">
-        <v>-9.8264607938878239</v>
-      </c>
-      <c r="C49">
-        <v>24.660403301048571</v>
-      </c>
-      <c r="D49">
-        <v>14285.047459530417</v>
-      </c>
-      <c r="E49">
-        <v>8.3574152835467194E-2</v>
-      </c>
-      <c r="F49">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G49">
-        <v>0.53421697292637893</v>
-      </c>
-      <c r="H49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>55.452137410531307</v>
-      </c>
-      <c r="B50">
-        <v>-9.811334504012958</v>
-      </c>
-      <c r="C50">
-        <v>6.9888533117958538</v>
-      </c>
-      <c r="D50">
-        <v>14313.527701478539</v>
-      </c>
-      <c r="E50">
-        <v>2.3685236923917299E-2</v>
-      </c>
-      <c r="F50">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G50">
-        <v>4.3309860934955945E-2</v>
-      </c>
-      <c r="H50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>56.674231989357395</v>
-      </c>
-      <c r="B51">
-        <v>-9.8093313640016451</v>
-      </c>
-      <c r="C51">
-        <v>-4.9999999999999503</v>
-      </c>
-      <c r="D51">
-        <v>14314.742748730931</v>
-      </c>
-      <c r="E51">
-        <v>1.6945009336467896E-2</v>
-      </c>
-      <c r="F51">
-        <v>32.453900860855732</v>
-      </c>
-      <c r="G51">
-        <v>-2.1699846402632925E-2</v>
-      </c>
-      <c r="H51">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13640,7 +10046,16 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
+      <c r="A14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14" s="2">
+        <f>'Propellant Parameters (Tanks)'!N26*0.453592</f>
+        <v>11.562209199342742</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C30" t="str">
@@ -13668,7 +10083,7 @@
       </c>
       <c r="C31" s="3">
         <f>SUM(B:B)</f>
-        <v>23.040136054421769</v>
+        <v>34.602345253764511</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -13698,7 +10113,7 @@
         <v>9</v>
       </c>
       <c r="C34" s="1">
-        <v>6</v>
+        <v>6.125</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -13730,7 +10145,9 @@
       <c r="C37" s="1">
         <v>5</v>
       </c>
-      <c r="D37" s="1"/>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
       <c r="E37" s="1"/>
     </row>
   </sheetData>
@@ -14045,13 +10462,15 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -14261,17 +10680,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>133</v>
       </c>
@@ -14287,13 +10706,49 @@
       <c r="F20" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J20" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>162</v>
+      </c>
+      <c r="K21" t="s">
+        <v>165</v>
+      </c>
+      <c r="L21" t="s">
+        <v>145</v>
+      </c>
+      <c r="M21" t="s">
+        <v>163</v>
+      </c>
+      <c r="N21" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>164</v>
+      </c>
+      <c r="K22">
+        <v>2</v>
+      </c>
+      <c r="L22">
+        <v>2.52</v>
+      </c>
+      <c r="M22" t="s">
+        <v>166</v>
+      </c>
+      <c r="N22" s="13">
+        <f>K22*L22</f>
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>133</v>
       </c>
@@ -14309,8 +10764,44 @@
       <c r="F23" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>168</v>
+      </c>
+      <c r="K23" s="8">
+        <f>C20</f>
+        <v>56.603313253621714</v>
+      </c>
+      <c r="L23">
+        <v>0.249</v>
+      </c>
+      <c r="M23" t="s">
+        <v>170</v>
+      </c>
+      <c r="N23" s="13">
+        <f>K23*L23</f>
+        <v>14.094225000151807</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>169</v>
+      </c>
+      <c r="K24" s="8">
+        <f>C23</f>
+        <v>14.981999088208545</v>
+      </c>
+      <c r="L24">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="M24" t="s">
+        <v>170</v>
+      </c>
+      <c r="N24" s="13">
+        <f>K24*L24</f>
+        <v>4.0751037519927245</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>147</v>
       </c>
@@ -14326,8 +10817,36 @@
       <c r="F25" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>171</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>2.2810000000000001</v>
+      </c>
+      <c r="M25" t="s">
+        <v>166</v>
+      </c>
+      <c r="N25">
+        <f>K25*L25</f>
+        <v>2.2810000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J26" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="14">
+        <f>SUM(N22:N25)</f>
+        <v>25.490328752144531</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
Altitude ft. to m.
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="173">
   <si>
     <t>Total inert mass</t>
   </si>
@@ -504,9 +504,6 @@
   </si>
   <si>
     <t>Launch Altitude</t>
-  </si>
-  <si>
-    <t>ft</t>
   </si>
   <si>
     <t>Tank</t>
@@ -962,7 +959,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,8 +1025,8 @@
         <v>9</v>
       </c>
       <c r="C7" s="11">
-        <f>101325*(1-(0.0000225577)*(C13*0.3048))^5.25588</f>
-        <v>85592.941945501399</v>
+        <f>101325*(1-(0.0000225577)*C13)^5.25588</f>
+        <v>85589.183879933975</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
@@ -1037,7 +1034,7 @@
         <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1072,12 +1069,13 @@
         <v>9</v>
       </c>
       <c r="C13" s="1">
-        <v>4595</v>
+        <f>4595/3.28</f>
+        <v>1400.9146341463415</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" t="s">
-        <v>159</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -9896,7 +9894,7 @@
   <dimension ref="A2:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10047,7 +10045,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B14" s="2">
         <f>'Propellant Parameters (Tanks)'!N26*0.453592</f>
@@ -10462,7 +10460,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10707,24 +10705,24 @@
         <v>53</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L21" t="s">
         <v>145</v>
       </c>
       <c r="M21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -10732,7 +10730,7 @@
         <v>144</v>
       </c>
       <c r="J22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K22">
         <v>2</v>
@@ -10741,7 +10739,7 @@
         <v>2.52</v>
       </c>
       <c r="M22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N22" s="13">
         <f>K22*L22</f>
@@ -10765,7 +10763,7 @@
         <v>53</v>
       </c>
       <c r="J23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K23" s="8">
         <f>C20</f>
@@ -10775,7 +10773,7 @@
         <v>0.249</v>
       </c>
       <c r="M23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N23" s="13">
         <f>K23*L23</f>
@@ -10784,7 +10782,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K24" s="8">
         <f>C23</f>
@@ -10794,7 +10792,7 @@
         <v>0.27200000000000002</v>
       </c>
       <c r="M24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N24" s="13">
         <f>K24*L24</f>
@@ -10818,7 +10816,7 @@
         <v>140</v>
       </c>
       <c r="J25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -10827,7 +10825,7 @@
         <v>2.2810000000000001</v>
       </c>
       <c r="M25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N25">
         <f>K25*L25</f>
@@ -10836,7 +10834,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J26" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
@@ -10867,7 +10865,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>

</xml_diff>

<commit_message>
added more mass parameterizations
not sure if Monte Carlo or range inputs will work with the way things are calculated
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" tabRatio="882"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" tabRatio="882" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="188">
   <si>
     <t>Total inert mass</t>
   </si>
@@ -476,9 +476,6 @@
     <t>Fuel Mass</t>
   </si>
   <si>
-    <t>Add more items as needed</t>
-  </si>
-  <si>
     <t>C2H6</t>
   </si>
   <si>
@@ -546,6 +543,54 @@
   </si>
   <si>
     <t>DO NOT INPUT, CALCULATED FROM LAUNCH ALTITUDE. Need to implement temperature compensation</t>
+  </si>
+  <si>
+    <t>Thickness</t>
+  </si>
+  <si>
+    <t>Fins:</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Material Density</t>
+  </si>
+  <si>
+    <t>kg/m^3</t>
+  </si>
+  <si>
+    <t>Body Tube:</t>
+  </si>
+  <si>
+    <t>Root chord</t>
+  </si>
+  <si>
+    <t>Tip chord</t>
+  </si>
+  <si>
+    <t>Bulkheads:</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Recovery:</t>
+  </si>
+  <si>
+    <t>Nose Cone:</t>
+  </si>
+  <si>
+    <t>Outer Dia.</t>
+  </si>
+  <si>
+    <t>Inner Dia.</t>
+  </si>
+  <si>
+    <t>Couplers:</t>
   </si>
 </sst>
 </file>
@@ -554,7 +599,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -637,7 +682,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -651,8 +696,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -958,7 +1004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -970,7 +1016,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G1" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1034,17 +1080,17 @@
         <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -1053,17 +1099,17 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -8635,7 +8681,7 @@
         <v>30</v>
       </c>
       <c r="R10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="U10" t="s">
         <v>64</v>
@@ -9891,22 +9937,67 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F37"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G1" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="I1" t="str">
+        <f>IF(H2="Single value","Value",IF(H2="Range of values","Start",IF(H2="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="J1" t="str">
+        <f>IF(H2="Single value","",IF(H2="Range of values","Step",IF(H2="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="K1" t="str">
+        <f>IF(H2="Single value","",IF(H2="Range of values","End",IF(H2="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="L1" t="s">
+        <v>139</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="P1" t="str">
+        <f>IF(O2="Single value","Value",IF(O2="Range of values","Start",IF(O2="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="Q1" t="str">
+        <f>IF(O2="Single value","",IF(O2="Range of values","Step",IF(O2="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="R1" t="str">
+        <f>IF(O2="Single value","",IF(O2="Range of values","End",IF(O2="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="S1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>146</v>
       </c>
@@ -9916,19 +10007,62 @@
       <c r="C2" s="5" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="15">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>125</v>
       </c>
       <c r="B3" s="2">
+        <f>I9*I10</f>
         <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="15">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -9938,8 +10072,40 @@
       <c r="C4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="15">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="P4" t="str">
+        <f>IF(O5="Single value","Value",IF(O5="Range of values","Start",IF(O5="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="Q4" t="str">
+        <f>IF(O5="Single value","",IF(O5="Range of values","Step",IF(O5="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="R4" t="str">
+        <f>IF(O5="Single value","",IF(O5="Range of values","End",IF(O5="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="S4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -9949,8 +10115,36 @@
       <c r="C5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="15">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>126</v>
       </c>
@@ -9960,33 +10154,97 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="15">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>124</v>
       </c>
       <c r="B7" s="2">
+        <f>I13*I14</f>
         <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="N7" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="P7" t="str">
+        <f>IF(O8="Single value","Value",IF(O8="Range of values","Start",IF(O8="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="Q7" t="str">
+        <f>IF(O8="Single value","",IF(O8="Range of values","Step",IF(O8="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="R7" t="str">
+        <f>IF(O8="Single value","",IF(O8="Range of values","End",IF(O8="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="S7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>123</v>
       </c>
       <c r="B8" s="2">
-        <v>2</v>
+        <f>P2</f>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="E8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="I8" t="str">
+        <f>IF(H9="Single value","Value",IF(H9="Range of values","Start",IF(H9="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="J8" t="str">
+        <f>IF(H9="Single value","",IF(H9="Range of values","Step",IF(H9="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="K8" t="str">
+        <f>IF(H9="Single value","",IF(H9="Range of values","End",IF(H9="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="L8" t="s">
+        <v>139</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P8" s="15">
+        <f>5.909/12/3.28</f>
+        <v>0.15012703252032522</v>
+      </c>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>122</v>
       </c>
@@ -9996,8 +10254,37 @@
       <c r="C9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="15">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" s="15">
+        <f>5.625/12/3.28</f>
+        <v>0.14291158536585366</v>
+      </c>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -10008,44 +10295,120 @@
       <c r="C10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="15">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" t="s">
+        <v>182</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P10" s="15">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="2">
-        <v>3</v>
+        <f>I6*(I2*(I3+I4)/2*I5)</f>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="N11" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P11" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="2">
-        <f>2.56/2.205*3</f>
-        <v>3.4829931972789119</v>
+        <f>P11*P10*((PI()*(P8-P9)^2))</f>
+        <v>4.9067917679042165E-4</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="I12" t="str">
+        <f>IF(H13="Single value","Value",IF(H13="Range of values","Start",IF(H13="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="J12" t="str">
+        <f>IF(H13="Single value","",IF(H13="Range of values","Step",IF(H13="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="K12" t="str">
+        <f>IF(H13="Single value","",IF(H13="Range of values","End",IF(H13="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="L12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="2">
+        <f>P5</f>
         <v>1</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G13" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="15">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B14" s="2">
         <f>'Propellant Parameters (Tanks)'!N26*0.453592</f>
@@ -10053,6 +10416,20 @@
       </c>
       <c r="C14" t="s">
         <v>3</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="15">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -10081,7 +10458,7 @@
       </c>
       <c r="C31" s="3">
         <f>SUM(B:B)</f>
-        <v>34.602345253764511</v>
+        <v>28.119842735662392</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -10158,7 +10535,7 @@
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B31 B34 B37 B25</xm:sqref>
+          <xm:sqref>B31 B34 B37 B25 L16 O2 H9:H10 H2:H6 O5 O8:O11 H13:H14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -10460,7 +10837,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10495,7 +10872,7 @@
         <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -10523,7 +10900,7 @@
         <v>139</v>
       </c>
       <c r="N5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -10540,7 +10917,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J6" s="1">
         <v>1593</v>
@@ -10566,7 +10943,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J8" s="1">
         <v>465.5</v>
@@ -10589,7 +10966,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="1"/>
       <c r="F10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J10" s="4">
         <f>93.19</f>
@@ -10601,7 +10978,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -10705,24 +11082,24 @@
         <v>53</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L21" t="s">
         <v>145</v>
       </c>
       <c r="M21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -10730,7 +11107,7 @@
         <v>144</v>
       </c>
       <c r="J22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K22">
         <v>2</v>
@@ -10739,7 +11116,7 @@
         <v>2.52</v>
       </c>
       <c r="M22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N22" s="13">
         <f>K22*L22</f>
@@ -10763,7 +11140,7 @@
         <v>53</v>
       </c>
       <c r="J23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K23" s="8">
         <f>C20</f>
@@ -10773,7 +11150,7 @@
         <v>0.249</v>
       </c>
       <c r="M23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N23" s="13">
         <f>K23*L23</f>
@@ -10782,7 +11159,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K24" s="8">
         <f>C23</f>
@@ -10792,7 +11169,7 @@
         <v>0.27200000000000002</v>
       </c>
       <c r="M24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N24" s="13">
         <f>K24*L24</f>
@@ -10816,7 +11193,7 @@
         <v>140</v>
       </c>
       <c r="J25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -10825,7 +11202,7 @@
         <v>2.2810000000000001</v>
       </c>
       <c r="M25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N25">
         <f>K25*L25</f>
@@ -10834,7 +11211,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J26" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>

</xml_diff>

<commit_message>
changed climate data link + temp
Truth or Consequences is closer to launch site and took mid June average daily high of 97 F
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" tabRatio="882" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" tabRatio="882"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
@@ -488,9 +488,6 @@
     <t>in to m</t>
   </si>
   <si>
-    <t>Las Cruces US Climate Data</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -594,6 +591,9 @@
   </si>
   <si>
     <t>Length (total)</t>
+  </si>
+  <si>
+    <t>Truth of Consequences US Climate Data</t>
   </si>
 </sst>
 </file>
@@ -1007,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,7 +1019,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G1" s="10" t="s">
-        <v>153</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1044,7 +1044,8 @@
         <v>9</v>
       </c>
       <c r="C4" s="1">
-        <v>300</v>
+        <f>273.15+(5/9*(97-32))</f>
+        <v>309.26111111111106</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1083,36 +1084,38 @@
         <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -1129,7 +1132,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G1" r:id="rId1"/>
+    <hyperlink ref="G1" r:id="rId1" display="https://www.usclimatedata.com/climate/truth-or-consequences/new-mexico/united-states/usnm0332"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -9942,7 +9945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
@@ -9964,7 +9967,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G1" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I1" t="str">
         <f>IF(H2="Single value","Value",IF(H2="Range of values","Start",IF(H2="Monte Carlo","Mean","ERROR")))</f>
@@ -9982,7 +9985,7 @@
         <v>139</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P1" t="str">
         <f>IF(O2="Single value","Value",IF(O2="Range of values","Start",IF(O2="Monte Carlo","Mean","ERROR")))</f>
@@ -10051,7 +10054,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>9</v>
@@ -10062,7 +10065,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -10077,7 +10080,7 @@
         <v>3</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P4" t="str">
         <f>IF(O5="Single value","Value",IF(O5="Range of values","Start",IF(O5="Monte Carlo","Mean","ERROR")))</f>
@@ -10106,7 +10109,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I5" t="str">
         <f>IF(H6="Single value","Value",IF(H6="Range of values","Start",IF(H6="Monte Carlo","Mean","ERROR")))</f>
@@ -10175,7 +10178,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>9</v>
@@ -10186,10 +10189,10 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P7" t="str">
         <f>IF(O8="Single value","Value",IF(O8="Range of values","Start",IF(O8="Monte Carlo","Mean","ERROR")))</f>
@@ -10219,7 +10222,7 @@
         <v>3</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>9</v>
@@ -10245,7 +10248,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I9" t="str">
         <f>IF(H10="Single value","Value",IF(H10="Range of values","Start",IF(H10="Monte Carlo","Mean","ERROR")))</f>
@@ -10263,7 +10266,7 @@
         <v>139</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>9</v>
@@ -10304,7 +10307,7 @@
         <v>3</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>9</v>
@@ -10330,7 +10333,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>9</v>
@@ -10341,10 +10344,10 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>9</v>
@@ -10355,7 +10358,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -10382,7 +10385,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I13" t="str">
         <f>IF(H14="Single value","Value",IF(H14="Range of values","Start",IF(H14="Monte Carlo","Mean","ERROR")))</f>
@@ -10400,7 +10403,7 @@
         <v>139</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="P13" t="str">
         <f>IF(O14="Single value","Value",IF(O14="Range of values","Start",IF(O14="Monte Carlo","Mean","ERROR")))</f>
@@ -10420,7 +10423,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B14" s="2">
         <f>'Propellant Parameters (Tanks)'!N26*0.453592</f>
@@ -10430,7 +10433,7 @@
         <v>3</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>9</v>
@@ -10441,7 +10444,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>145</v>
@@ -10460,7 +10463,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G15" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>9</v>
@@ -10474,7 +10477,7 @@
         <v>53</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>9</v>
@@ -10485,7 +10488,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -11138,24 +11141,24 @@
         <v>53</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L21" t="s">
         <v>145</v>
       </c>
       <c r="M21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -11163,7 +11166,7 @@
         <v>144</v>
       </c>
       <c r="J22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K22">
         <v>2</v>
@@ -11172,7 +11175,7 @@
         <v>2.52</v>
       </c>
       <c r="M22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N22" s="13">
         <f>K22*L22</f>
@@ -11196,7 +11199,7 @@
         <v>53</v>
       </c>
       <c r="J23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K23" s="8">
         <f>C20</f>
@@ -11206,7 +11209,7 @@
         <v>0.249</v>
       </c>
       <c r="M23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N23" s="13">
         <f>K23*L23</f>
@@ -11215,7 +11218,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K24" s="8">
         <f>C23</f>
@@ -11225,7 +11228,7 @@
         <v>0.27200000000000002</v>
       </c>
       <c r="M24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N24" s="13">
         <f>K24*L24</f>
@@ -11249,7 +11252,7 @@
         <v>140</v>
       </c>
       <c r="J25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -11258,7 +11261,7 @@
         <v>2.2810000000000001</v>
       </c>
       <c r="M25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N25">
         <f>K25*L25</f>
@@ -11267,7 +11270,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J26" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>

</xml_diff>

<commit_message>
Cleaned things up, exposed some physics issues
Physics is broken, I'm just putting this up so other people can look at it
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" tabRatio="551" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" tabRatio="551" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
@@ -12,16 +12,17 @@
     <sheet name="Engine Parameters" sheetId="4" r:id="rId3"/>
     <sheet name="Propellant Parameters (Tanks)" sheetId="5" r:id="rId4"/>
     <sheet name="Validation" sheetId="3" state="hidden" r:id="rId5"/>
+    <sheet name="Results 05-Oct-2017 17-09-13" sheetId="13" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="190">
   <si>
     <t>Total inert mass</t>
   </si>
@@ -68,9 +69,6 @@
     <t>Expansion ratio</t>
   </si>
   <si>
-    <t>C*</t>
-  </si>
-  <si>
     <t>Engine mass</t>
   </si>
   <si>
@@ -369,6 +367,231 @@
   </si>
   <si>
     <t>Oxidizer temperature</t>
+  </si>
+  <si>
+    <t>Time (s)</t>
+  </si>
+  <si>
+    <t>Acceleration (m/s)</t>
+  </si>
+  <si>
+    <t>Velocity (m/s)</t>
+  </si>
+  <si>
+    <t>Altitude (m)</t>
+  </si>
+  <si>
+    <t>Mach Number</t>
+  </si>
+  <si>
+    <t>Mass (kg)</t>
+  </si>
+  <si>
+    <t>Drag (N)</t>
+  </si>
+  <si>
+    <t>Thrust (N)</t>
+  </si>
+  <si>
+    <t>Maximums</t>
+  </si>
+  <si>
+    <t>alt</t>
+  </si>
+  <si>
+    <t>mach</t>
+  </si>
+  <si>
+    <t>accel</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>load</t>
+  </si>
+  <si>
+    <t>thrust</t>
+  </si>
+  <si>
+    <t>Propellants</t>
+  </si>
+  <si>
+    <t>ox</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Cv_valves</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>p_psi</t>
+  </si>
+  <si>
+    <t>rho</t>
+  </si>
+  <si>
+    <t>U_initial</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>pct_psi</t>
+  </si>
+  <si>
+    <t>eps</t>
+  </si>
+  <si>
+    <t>cstar_eta</t>
+  </si>
+  <si>
+    <t>epsc</t>
+  </si>
+  <si>
+    <t>Lstar</t>
+  </si>
+  <si>
+    <t>MR</t>
+  </si>
+  <si>
+    <t>thetac</t>
+  </si>
+  <si>
+    <t>alpn</t>
+  </si>
+  <si>
+    <t>injector_f_Atotal</t>
+  </si>
+  <si>
+    <t>injector_ox_Atotal</t>
+  </si>
+  <si>
+    <t>injector_f_Cd</t>
+  </si>
+  <si>
+    <t>injector_ox_Cd</t>
+  </si>
+  <si>
+    <t>thrustGL</t>
+  </si>
+  <si>
+    <t>thrustGL_lb</t>
+  </si>
+  <si>
+    <t>At</t>
+  </si>
+  <si>
+    <t>At_in2</t>
+  </si>
+  <si>
+    <t>dt</t>
+  </si>
+  <si>
+    <t>dt_in</t>
+  </si>
+  <si>
+    <t>Ae</t>
+  </si>
+  <si>
+    <t>Ae_in2</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>de_in</t>
+  </si>
+  <si>
+    <t>Vc</t>
+  </si>
+  <si>
+    <t>Vc_in3</t>
+  </si>
+  <si>
+    <t>Ac</t>
+  </si>
+  <si>
+    <t>Ac_in2</t>
+  </si>
+  <si>
+    <t>dc_in</t>
+  </si>
+  <si>
+    <t>Lc_in</t>
+  </si>
+  <si>
+    <t>Ln_in</t>
+  </si>
+  <si>
+    <t>Rocket</t>
+  </si>
+  <si>
+    <t>minert</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>TW</t>
+  </si>
+  <si>
+    <t>Cd</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>tank</t>
+  </si>
+  <si>
+    <t>Vox</t>
+  </si>
+  <si>
+    <t>Vf</t>
+  </si>
+  <si>
+    <t>Vox_in3</t>
+  </si>
+  <si>
+    <t>Vf_in3</t>
+  </si>
+  <si>
+    <t>mwet</t>
+  </si>
+  <si>
+    <t>Mprop</t>
+  </si>
+  <si>
+    <t>Engine throat area</t>
+  </si>
+  <si>
+    <t>Throat area</t>
+  </si>
+  <si>
+    <t>in^2</t>
+  </si>
+  <si>
+    <t>C* efficiency</t>
+  </si>
+  <si>
+    <t>Diameter</t>
+  </si>
+  <si>
+    <t>Length (straight section)</t>
+  </si>
+  <si>
+    <t>impulse</t>
   </si>
 </sst>
 </file>
@@ -828,7 +1051,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,7 +1062,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G1" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -858,7 +1081,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
@@ -869,7 +1092,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -888,7 +1111,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>9</v>
@@ -900,20 +1123,20 @@
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -924,17 +1147,17 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -946,7 +1169,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -971,10 +1194,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,7 +1218,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G1" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I1" t="str">
         <f>IF(H2="Single value","Value",IF(H2="Range of values","Start",IF(H2="Monte Carlo","Mean","ERROR")))</f>
@@ -1010,10 +1233,10 @@
         <v/>
       </c>
       <c r="L1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P1" t="str">
         <f>IF(O2="Single value","Value",IF(O2="Range of values","Start",IF(O2="Monte Carlo","Mean","ERROR")))</f>
@@ -1028,21 +1251,21 @@
         <v/>
       </c>
       <c r="S1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>9</v>
@@ -1056,7 +1279,7 @@
         <v>3</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>9</v>
@@ -1072,7 +1295,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2">
         <f>I6*I7</f>
@@ -1082,7 +1305,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>9</v>
@@ -1093,12 +1316,12 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2">
         <f>I14*I15</f>
@@ -1108,7 +1331,7 @@
         <v>3</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P4" t="str">
         <f>IF(O5="Single value","Value",IF(O5="Range of values","Start",IF(O5="Monte Carlo","Mean","ERROR")))</f>
@@ -1123,12 +1346,12 @@
         <v/>
       </c>
       <c r="S4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="2">
         <v>0.5</v>
@@ -1137,7 +1360,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I5" t="str">
         <f>IF(H6="Single value","Value",IF(H6="Range of values","Start",IF(H6="Monte Carlo","Mean","ERROR")))</f>
@@ -1152,10 +1375,10 @@
         <v/>
       </c>
       <c r="L5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>9</v>
@@ -1171,7 +1394,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
@@ -1180,7 +1403,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>9</v>
@@ -1196,7 +1419,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="2">
         <f>I10*I11</f>
@@ -1206,7 +1429,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>9</v>
@@ -1217,10 +1440,10 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P7" t="str">
         <f>IF(O8="Single value","Value",IF(O8="Range of values","Start",IF(O8="Monte Carlo","Mean","ERROR")))</f>
@@ -1235,12 +1458,12 @@
         <v/>
       </c>
       <c r="S7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2">
         <f>P2</f>
@@ -1250,7 +1473,7 @@
         <v>3</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>9</v>
@@ -1262,12 +1485,12 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="2">
         <v>4</v>
@@ -1276,7 +1499,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I9" t="str">
         <f>IF(H10="Single value","Value",IF(H10="Range of values","Start",IF(H10="Monte Carlo","Mean","ERROR")))</f>
@@ -1291,10 +1514,10 @@
         <v/>
       </c>
       <c r="L9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>9</v>
@@ -1306,12 +1529,12 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2">
         <f>11.151/2.205</f>
@@ -1321,7 +1544,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>9</v>
@@ -1335,7 +1558,7 @@
         <v>3</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>9</v>
@@ -1346,7 +1569,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1361,7 +1584,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>9</v>
@@ -1372,10 +1595,10 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>9</v>
@@ -1386,7 +1609,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1413,7 +1636,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I13" t="str">
         <f>IF(H14="Single value","Value",IF(H14="Range of values","Start",IF(H14="Monte Carlo","Mean","ERROR")))</f>
@@ -1428,10 +1651,10 @@
         <v/>
       </c>
       <c r="L13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P13" t="str">
         <f>IF(O14="Single value","Value",IF(O14="Range of values","Start",IF(O14="Monte Carlo","Mean","ERROR")))</f>
@@ -1446,22 +1669,22 @@
         <v/>
       </c>
       <c r="S13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="2">
         <f>'Propellant Parameters (Tanks)'!N34*0.453592</f>
-        <v>3.3207470319999999</v>
+        <v>11.562209199342742</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>9</v>
@@ -1472,10 +1695,10 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>9</v>
@@ -1491,7 +1714,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G15" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>9</v>
@@ -1502,10 +1725,10 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>9</v>
@@ -1516,7 +1739,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1533,7 +1756,7 @@
         <v/>
       </c>
       <c r="F30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1545,7 +1768,7 @@
       </c>
       <c r="C31" s="3">
         <f>SUM(B:B)</f>
-        <v>24.202723666476995</v>
+        <v>32.444185833819738</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1553,64 +1776,76 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C33" t="str">
-        <f>IF(B34="Single value","Value",IF(B34="Range of values","Start",IF(B34="Monte Carlo","Mean","ERROR")))</f>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>187</v>
+      </c>
+      <c r="C34">
+        <v>6.125</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C35" t="str">
+        <f>IF(B36="Single value","Value",IF(B36="Range of values","Start",IF(B36="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
       </c>
-      <c r="D33" t="str">
-        <f>IF(B34="Single value","",IF(B34="Range of values","Step",IF(B34="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E33" t="str">
-        <f>IF(B34="Single value","",IF(B34="Range of values","End",IF(B34="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="D35" t="str">
+        <f>IF(B36="Single value","",IF(B36="Range of values","Step",IF(B36="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E35" t="str">
+        <f>IF(B36="Single value","",IF(B36="Range of values","End",IF(B36="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="1">
-        <v>6.125</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" t="s">
+      <c r="C36" s="1">
+        <f>C34*2.54/100</f>
+        <v>0.15557500000000002</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C38" t="str">
+        <f>IF(B39="Single value","Value",IF(B39="Range of values","Start",IF(B39="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D38" t="str">
+        <f>IF(B39="Single value","",IF(B39="Range of values","Step",IF(B39="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E38" t="str">
+        <f>IF(B39="Single value","",IF(B39="Range of values","End",IF(B39="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C36" t="str">
-        <f>IF(B37="Single value","Value",IF(B37="Range of values","Start",IF(B37="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D36" t="str">
-        <f>IF(B37="Single value","",IF(B37="Range of values","Step",IF(B37="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E36" t="str">
-        <f>IF(B37="Single value","",IF(B37="Range of values","End",IF(B37="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="1">
-        <v>5</v>
-      </c>
-      <c r="D37" s="1">
+      <c r="D39" s="1">
         <v>1</v>
       </c>
-      <c r="E37" s="1"/>
+      <c r="E39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1622,7 +1857,7 @@
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B31 B34 B37 B25 H14:H15 O2 H6:H7 O14:O15 O5 O8:O11 H10:H11 H2 H3</xm:sqref>
+          <xm:sqref>B31:B33 B36 B39 B25 H14:H15 O2 H6:H7 O14:O15 O5 O8:O11 H10:H11 H2 H3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1632,10 +1867,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F50"/>
+  <dimension ref="A2:F54"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1717,7 +1952,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>186</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -1744,7 +1979,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>9</v>
@@ -1774,7 +2009,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>9</v>
@@ -1801,7 +2036,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>9</v>
@@ -1831,7 +2066,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>9</v>
@@ -1842,7 +2077,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1861,7 +2096,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>9</v>
@@ -1872,239 +2107,281 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C26" t="str">
-        <f>IF(B27="Single value","Value",IF(B27="Range of values","Start",IF(B27="Monte Carlo","Mean","ERROR")))</f>
+      <c r="B26" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C27" t="str">
+        <f>IF(B28="Single value","Value",IF(B28="Range of values","Start",IF(B28="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
       </c>
-      <c r="D26" t="str">
-        <f>IF(B27="Single value","",IF(B27="Range of values","Step",IF(B27="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E26" t="str">
-        <f>IF(B27="Single value","",IF(B27="Range of values","End",IF(B27="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="1" t="s">
+      <c r="D27" t="str">
+        <f>IF(B28="Single value","",IF(B28="Range of values","Step",IF(B28="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E27" t="str">
+        <f>IF(B28="Single value","",IF(B28="Range of values","End",IF(B28="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C28" s="1">
+        <f>C26*2.54^2/100^2</f>
+        <v>6.4515999999999998E-4</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C30" t="str">
+        <f>IF(B31="Single value","Value",IF(B31="Range of values","Start",IF(B31="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D30" t="str">
+        <f>IF(B31="Single value","",IF(B31="Range of values","Step",IF(B31="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E30" t="str">
+        <f>IF(B31="Single value","",IF(B31="Range of values","End",IF(B31="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="1">
         <v>8</v>
       </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>109</v>
-      </c>
-      <c r="B30">
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34">
         <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>110</v>
-      </c>
-      <c r="B31">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>110</v>
-      </c>
-      <c r="B32">
-        <f>B31 * 2.54/100</f>
-        <v>6.3500000000000004E-4</v>
-      </c>
-      <c r="C32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>111</v>
-      </c>
-      <c r="B33">
-        <f>(PI() / 4) *B32^2</f>
-        <v>3.1669217443593616E-7</v>
-      </c>
-      <c r="C33" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B35">
-        <v>18</v>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B36">
-        <v>5.0999999999999997E-2</v>
+        <f>B35 * 2.54/100</f>
+        <v>6.3500000000000004E-4</v>
       </c>
       <c r="C36" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B37">
-        <f>B36 * 2.54/100</f>
+        <f>(PI() / 4) *B36^2</f>
+        <v>3.1669217443593616E-7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41">
+        <f>B40 * 2.54/100</f>
         <v>1.2953999999999999E-3</v>
       </c>
-      <c r="C37" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>107</v>
-      </c>
-      <c r="B38">
-        <f>(PI() / 4) *B37^2</f>
+      <c r="C41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>106</v>
+      </c>
+      <c r="B42">
+        <f>(PI() / 4) *B41^2</f>
         <v>1.3179461531325915E-6</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C44" t="str">
+        <f>IF(B45="Single value","Value",IF(B45="Range of values","Start",IF(B45="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D44" t="str">
+        <f>IF(B45="Single value","",IF(B45="Range of values","Step",IF(B45="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E44" t="str">
+        <f>IF(B45="Single value","",IF(B45="Range of values","End",IF(B45="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="9">
+        <f>B34*B37</f>
+        <v>5.7004591398468508E-6</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C47" t="str">
+        <f>IF(B48="Single value","Value",IF(B48="Range of values","Start",IF(B48="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D47" t="str">
+        <f>IF(B48="Single value","",IF(B48="Range of values","Step",IF(B48="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E47" t="str">
+        <f>IF(B48="Single value","",IF(B48="Range of values","End",IF(B48="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C40" t="str">
-        <f>IF(B41="Single value","Value",IF(B41="Range of values","Start",IF(B41="Monte Carlo","Mean","ERROR")))</f>
+      <c r="B48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="9">
+        <f>B42*B39</f>
+        <v>2.3723030756386648E-5</v>
+      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="str">
+        <f>IF(B51="Single value","Value",IF(B51="Range of values","Start",IF(B51="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
       </c>
-      <c r="D40" t="str">
-        <f>IF(B41="Single value","",IF(B41="Range of values","Step",IF(B41="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E40" t="str">
-        <f>IF(B41="Single value","",IF(B41="Range of values","End",IF(B41="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B41" s="1" t="s">
+      <c r="D50" t="str">
+        <f>IF(B51="Single value","",IF(B51="Range of values","Step",IF(B51="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E50" t="str">
+        <f>IF(B51="Single value","",IF(B51="Range of values","End",IF(B51="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="9">
-        <f>B30*B33</f>
-        <v>5.7004591398468508E-6</v>
-      </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C43" t="str">
-        <f>IF(B44="Single value","Value",IF(B44="Range of values","Start",IF(B44="Monte Carlo","Mean","ERROR")))</f>
+      <c r="C51" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C53" t="str">
+        <f>IF(B54="Single value","Value",IF(B54="Range of values","Start",IF(B54="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
       </c>
-      <c r="D43" t="str">
-        <f>IF(B44="Single value","",IF(B44="Range of values","Step",IF(B44="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E43" t="str">
-        <f>IF(B44="Single value","",IF(B44="Range of values","End",IF(B44="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="D53" t="str">
+        <f>IF(B54="Single value","",IF(B54="Range of values","Step",IF(B54="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E53" t="str">
+        <f>IF(B54="Single value","",IF(B54="Range of values","End",IF(B54="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" t="s">
         <v>102</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="9">
-        <f>B38*B35</f>
-        <v>2.3723030756386648E-5</v>
-      </c>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C46" t="str">
-        <f>IF(B47="Single value","Value",IF(B47="Range of values","Start",IF(B47="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D46" t="str">
-        <f>IF(B47="Single value","",IF(B47="Range of values","Step",IF(B47="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E46" t="str">
-        <f>IF(B47="Single value","",IF(B47="Range of values","End",IF(B47="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C49" t="str">
-        <f>IF(B50="Single value","Value",IF(B50="Range of values","Start",IF(B50="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D49" t="str">
-        <f>IF(B50="Single value","",IF(B50="Range of values","Step",IF(B50="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E49" t="str">
-        <f>IF(B50="Single value","",IF(B50="Range of values","End",IF(B50="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" s="1">
-        <v>1</v>
-      </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2116,13 +2393,13 @@
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B3 B6 B9 B12 B15 B18 B21 B24 B27</xm:sqref>
+          <xm:sqref>B3 B6 B9 B12 B15 B18 B21 B24 B31 B28</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>[1]Validation!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>B41 B44 B47 B50</xm:sqref>
+          <xm:sqref>B45 B48 B51 B54</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2132,10 +2409,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2148,34 +2425,34 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -2192,18 +2469,18 @@
         <v/>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
@@ -2215,13 +2492,13 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J6" s="1">
         <v>1593</v>
       </c>
       <c r="K6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N6" s="6">
         <v>1.6387100000000001E-5</v>
@@ -2229,7 +2506,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -2241,18 +2518,18 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J8" s="1">
         <v>465.5</v>
       </c>
       <c r="K8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -2264,24 +2541,24 @@
       <c r="D10" s="4"/>
       <c r="E10" s="1"/>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J10" s="4">
         <f>93.19</f>
         <v>93.19</v>
       </c>
       <c r="K10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>9</v>
@@ -2293,7 +2570,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J12" s="4">
         <v>5.625</v>
@@ -2307,7 +2584,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
@@ -2319,7 +2596,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G14" s="6"/>
       <c r="J14" s="1">
@@ -2331,7 +2608,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>9</v>
@@ -2343,7 +2620,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G16" s="6"/>
       <c r="J16" s="1">
@@ -2369,7 +2646,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>9</v>
@@ -2380,7 +2657,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -2399,7 +2676,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>9</v>
@@ -2410,7 +2687,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -2425,7 +2702,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>9</v>
@@ -2437,7 +2714,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J28" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -2450,24 +2727,24 @@
         <v/>
       </c>
       <c r="J29" t="s">
+        <v>69</v>
+      </c>
+      <c r="K29" t="s">
+        <v>72</v>
+      </c>
+      <c r="L29" t="s">
+        <v>55</v>
+      </c>
+      <c r="M29" t="s">
         <v>70</v>
       </c>
-      <c r="K29" t="s">
-        <v>73</v>
-      </c>
-      <c r="L29" t="s">
-        <v>56</v>
-      </c>
-      <c r="M29" t="s">
-        <v>71</v>
-      </c>
       <c r="N29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>9</v>
@@ -2477,7 +2754,7 @@
       </c>
       <c r="D30" s="1"/>
       <c r="J30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K30">
         <v>2</v>
@@ -2486,7 +2763,7 @@
         <v>2.52</v>
       </c>
       <c r="M30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N30" s="13">
         <f>K30*L30</f>
@@ -2495,51 +2772,51 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K31" s="8">
-        <f>C47</f>
-        <v>0</v>
+        <f>C34</f>
+        <v>56.603313253621714</v>
       </c>
       <c r="L31">
         <v>0.249</v>
       </c>
       <c r="M31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N31" s="13">
         <f>K31*L31</f>
-        <v>0</v>
+        <v>14.094225000151807</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K32" s="8">
-        <f>C50</f>
-        <v>0</v>
+        <f>C37</f>
+        <v>14.981999088208545</v>
       </c>
       <c r="L32">
         <v>0.27200000000000002</v>
       </c>
       <c r="M32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N32" s="13">
         <f>K32*L32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+        <v>4.0751037519927245</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K33">
         <v>1</v>
@@ -2548,16 +2825,16 @@
         <v>2.2810000000000001</v>
       </c>
       <c r="M33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N33">
         <f>K33*L33</f>
         <v>2.2810000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>9</v>
@@ -2568,27 +2845,30 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J34" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
       <c r="M34" s="12"/>
       <c r="N34" s="14">
         <f>SUM(N30:N33)</f>
-        <v>7.3209999999999997</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+        <v>25.490328752144531</v>
+      </c>
+      <c r="O34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>9</v>
@@ -2599,12 +2879,15 @@
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J37" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>9</v>
@@ -2615,12 +2898,12 @@
       <c r="D39" s="4"/>
       <c r="E39" s="1"/>
       <c r="F39" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>9</v>
@@ -2631,24 +2914,24 @@
       <c r="D41" s="4"/>
       <c r="E41" s="1"/>
       <c r="F41" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="16"/>
       <c r="B47" s="16"/>
       <c r="C47" s="17"/>
       <c r="D47" s="16"/>
       <c r="E47" s="16"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="16"/>
       <c r="B48" s="16"/>
       <c r="C48" s="16"/>
@@ -2766,4 +3049,2923 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA95"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O1" t="s">
+        <v>130</v>
+      </c>
+      <c r="U1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>65.787653732895365</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>55.081701984038048</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>4164.0474336078441</v>
+      </c>
+      <c r="K2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L2">
+        <v>27029.908419645024</v>
+      </c>
+      <c r="O2" t="s">
+        <v>131</v>
+      </c>
+      <c r="U2" t="s">
+        <v>141</v>
+      </c>
+      <c r="V2">
+        <v>300</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z2">
+        <v>32.444200000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1.97190475740888E-7</v>
+      </c>
+      <c r="B3">
+        <v>65.78765388403238</v>
+      </c>
+      <c r="C3">
+        <v>1.2972698772114685E-5</v>
+      </c>
+      <c r="D3">
+        <v>1.2790463201195469E-12</v>
+      </c>
+      <c r="E3">
+        <v>3.8738705252333493E-8</v>
+      </c>
+      <c r="F3">
+        <v>55.08170172798831</v>
+      </c>
+      <c r="G3">
+        <v>2.8921011299572942E-12</v>
+      </c>
+      <c r="H3">
+        <v>4164.0474225759717</v>
+      </c>
+      <c r="K3" t="s">
+        <v>125</v>
+      </c>
+      <c r="L3">
+        <v>1.3523213227778674</v>
+      </c>
+      <c r="P3" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" t="s">
+        <v>28</v>
+      </c>
+      <c r="U3" t="s">
+        <v>142</v>
+      </c>
+      <c r="V3">
+        <v>4</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z3">
+        <v>0.15558</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1.183142854445328E-6</v>
+      </c>
+      <c r="B4">
+        <v>65.787654639715953</v>
+      </c>
+      <c r="C4">
+        <v>7.7836193474666252E-5</v>
+      </c>
+      <c r="D4">
+        <v>4.6045667836894432E-11</v>
+      </c>
+      <c r="E4">
+        <v>2.3243223402829236E-7</v>
+      </c>
+      <c r="F4">
+        <v>55.081700447739628</v>
+      </c>
+      <c r="G4">
+        <v>1.0411564293096423E-10</v>
+      </c>
+      <c r="H4">
+        <v>4164.0473674166124</v>
+      </c>
+      <c r="K4" t="s">
+        <v>126</v>
+      </c>
+      <c r="L4">
+        <v>7.1297238714387561</v>
+      </c>
+      <c r="P4" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q4">
+        <v>2.6105E-2</v>
+      </c>
+      <c r="U4" t="s">
+        <v>143</v>
+      </c>
+      <c r="V4">
+        <v>0.9</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6.1129047479675275E-6</v>
+      </c>
+      <c r="B5">
+        <v>65.787658418094907</v>
+      </c>
+      <c r="C5">
+        <v>4.0215368803679939E-4</v>
+      </c>
+      <c r="D5">
+        <v>1.2291635636202613E-9</v>
+      </c>
+      <c r="E5">
+        <v>1.2008999407651507E-6</v>
+      </c>
+      <c r="F5">
+        <v>55.081694046496288</v>
+      </c>
+      <c r="G5">
+        <v>2.7793095466633026E-9</v>
+      </c>
+      <c r="H5">
+        <v>4164.0470916198183</v>
+      </c>
+      <c r="K5" t="s">
+        <v>127</v>
+      </c>
+      <c r="L5">
+        <v>634.19020444036164</v>
+      </c>
+      <c r="P5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q5">
+        <v>20.11290193008751</v>
+      </c>
+      <c r="U5" t="s">
+        <v>33</v>
+      </c>
+      <c r="V5">
+        <v>3</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3.0761714215578524E-5</v>
+      </c>
+      <c r="B6">
+        <v>65.787677309015422</v>
+      </c>
+      <c r="C6">
+        <v>2.0237416870720407E-3</v>
+      </c>
+      <c r="D6">
+        <v>3.1126877784331845E-8</v>
+      </c>
+      <c r="E6">
+        <v>6.0432400458484385E-6</v>
+      </c>
+      <c r="F6">
+        <v>55.081662040281834</v>
+      </c>
+      <c r="G6">
+        <v>7.0382220301014603E-8</v>
+      </c>
+      <c r="H6">
+        <v>4164.0457126358524</v>
+      </c>
+      <c r="K6" t="s">
+        <v>128</v>
+      </c>
+      <c r="L6">
+        <v>1452.0211533386487</v>
+      </c>
+      <c r="P6" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q6">
+        <v>3</v>
+      </c>
+      <c r="U6" t="s">
+        <v>144</v>
+      </c>
+      <c r="V6">
+        <v>300</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1.540057615536335E-4</v>
+      </c>
+      <c r="B7">
+        <v>65.787771739266802</v>
+      </c>
+      <c r="C7">
+        <v>1.0131694836636548E-2</v>
+      </c>
+      <c r="D7">
+        <v>7.8016919698645153E-7</v>
+      </c>
+      <c r="E7">
+        <v>3.0254979852788109E-5</v>
+      </c>
+      <c r="F7">
+        <v>55.081502009265257</v>
+      </c>
+      <c r="G7">
+        <v>1.7640748503768922E-6</v>
+      </c>
+      <c r="H7">
+        <v>4164.0388177164759</v>
+      </c>
+      <c r="K7" t="s">
+        <v>129</v>
+      </c>
+      <c r="L7">
+        <v>980.56219199326779</v>
+      </c>
+      <c r="P7" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q7">
+        <v>295</v>
+      </c>
+      <c r="U7" t="s">
+        <v>145</v>
+      </c>
+      <c r="V7">
+        <v>45</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA7">
+        <v>3.0020749999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7.7022599824390836E-4</v>
+      </c>
+      <c r="B8">
+        <v>65.788243281725087</v>
+      </c>
+      <c r="C8">
+        <v>5.0671789290904878E-2</v>
+      </c>
+      <c r="D8">
+        <v>1.9514303160151828E-5</v>
+      </c>
+      <c r="E8">
+        <v>1.5131466049410735E-4</v>
+      </c>
+      <c r="F8">
+        <v>55.080701855574802</v>
+      </c>
+      <c r="G8">
+        <v>4.412505775578403E-5</v>
+      </c>
+      <c r="H8">
+        <v>4164.0043431309687</v>
+      </c>
+      <c r="K8" t="s">
+        <v>189</v>
+      </c>
+      <c r="L8">
+        <v>60971.54567181399</v>
+      </c>
+      <c r="P8" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q8">
+        <v>5268095.5963083049</v>
+      </c>
+      <c r="U8" t="s">
+        <v>146</v>
+      </c>
+      <c r="V8">
+        <v>8</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>178</v>
+      </c>
+      <c r="AA8">
+        <v>8.7724299999999977E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3.8513271816952824E-3</v>
+      </c>
+      <c r="B9">
+        <v>65.790585771423025</v>
+      </c>
+      <c r="C9">
+        <v>0.25338046006318843</v>
+      </c>
+      <c r="D9">
+        <v>4.8791784678872159E-4</v>
+      </c>
+      <c r="E9">
+        <v>7.5663754992655861E-4</v>
+      </c>
+      <c r="F9">
+        <v>55.07670112193361</v>
+      </c>
+      <c r="G9">
+        <v>1.103313741390698E-3</v>
+      </c>
+      <c r="H9">
+        <v>4163.8319704895139</v>
+      </c>
+      <c r="L9">
+        <f>L8/((F2-F72)*9.81)</f>
+        <v>315.26745996966417</v>
+      </c>
+      <c r="P9" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q9">
+        <v>764.07236746577178</v>
+      </c>
+      <c r="U9" t="s">
+        <v>147</v>
+      </c>
+      <c r="V9">
+        <v>45</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA9">
+        <v>1831.9745409498933</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1.9256833098952153E-2</v>
+      </c>
+      <c r="B10">
+        <v>65.801917329629433</v>
+      </c>
+      <c r="C10">
+        <v>1.2671263798802739</v>
+      </c>
+      <c r="D10">
+        <v>1.2199472700847406E-2</v>
+      </c>
+      <c r="E10">
+        <v>3.7838574058091652E-3</v>
+      </c>
+      <c r="F10">
+        <v>55.056698324000998</v>
+      </c>
+      <c r="G10">
+        <v>2.7592569628493765E-2</v>
+      </c>
+      <c r="H10">
+        <v>4162.9701146863399</v>
+      </c>
+      <c r="P10" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q10">
+        <v>770.46167133068411</v>
+      </c>
+      <c r="U10" t="s">
+        <v>155</v>
+      </c>
+      <c r="V10">
+        <v>6.4515999999999998E-4</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>180</v>
+      </c>
+      <c r="AA10">
+        <v>535.32534737689991</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9.6284362685236491E-2</v>
+      </c>
+      <c r="B11">
+        <v>65.848588019926666</v>
+      </c>
+      <c r="C11">
+        <v>6.3406080736987152</v>
+      </c>
+      <c r="D11">
+        <v>0.30514020759123611</v>
+      </c>
+      <c r="E11">
+        <v>1.8934211342632706E-2</v>
+      </c>
+      <c r="F11">
+        <v>54.95670609071405</v>
+      </c>
+      <c r="G11">
+        <v>0.72881761979343263</v>
+      </c>
+      <c r="H11">
+        <v>4158.675602669322</v>
+      </c>
+      <c r="P11" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q11">
+        <v>4449999.4977064431</v>
+      </c>
+      <c r="U11" t="s">
+        <v>148</v>
+      </c>
+      <c r="V11">
+        <v>15</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z11">
+        <v>55.081701984038048</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.23275717372040602</v>
+      </c>
+      <c r="B12">
+        <v>65.889793528240858</v>
+      </c>
+      <c r="C12">
+        <v>15.339951063589698</v>
+      </c>
+      <c r="D12">
+        <v>1.7842658713445527</v>
+      </c>
+      <c r="E12">
+        <v>4.5808678893517862E-2</v>
+      </c>
+      <c r="F12">
+        <v>54.779738044207029</v>
+      </c>
+      <c r="G12">
+        <v>4.314828408401425</v>
+      </c>
+      <c r="H12">
+        <v>4151.1296878859948</v>
+      </c>
+      <c r="O12" t="s">
+        <v>140</v>
+      </c>
+      <c r="U12" t="s">
+        <v>149</v>
+      </c>
+      <c r="V12">
+        <v>5.7004999999999999E-6</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z12">
+        <v>0.41098043757976288</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.58692462251640787</v>
+      </c>
+      <c r="B13">
+        <v>65.701749023875365</v>
+      </c>
+      <c r="C13">
+        <v>38.725913758009952</v>
+      </c>
+      <c r="D13">
+        <v>11.356095575400241</v>
+      </c>
+      <c r="E13">
+        <v>0.11565752391744742</v>
+      </c>
+      <c r="F13">
+        <v>54.321358000668482</v>
+      </c>
+      <c r="G13">
+        <v>26.743651526082271</v>
+      </c>
+      <c r="H13">
+        <v>4128.6444035086452</v>
+      </c>
+      <c r="P13" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>29</v>
+      </c>
+      <c r="R13" t="s">
+        <v>59</v>
+      </c>
+      <c r="U13" t="s">
+        <v>150</v>
+      </c>
+      <c r="V13">
+        <v>2.3723E-5</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z13">
+        <v>7.6042678693378898E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.65988657716657184</v>
+      </c>
+      <c r="B14">
+        <v>65.642225759049694</v>
+      </c>
+      <c r="C14">
+        <v>43.519881194394834</v>
+      </c>
+      <c r="D14">
+        <v>14.35650035894259</v>
+      </c>
+      <c r="E14">
+        <v>0.12997957083082068</v>
+      </c>
+      <c r="F14">
+        <v>54.227445239279994</v>
+      </c>
+      <c r="G14">
+        <v>33.578024290016323</v>
+      </c>
+      <c r="H14">
+        <v>4125.1594648206756</v>
+      </c>
+      <c r="P14" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q14">
+        <v>7.628199999999999E-3</v>
+      </c>
+      <c r="U14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.73284853181673582</v>
+      </c>
+      <c r="B15">
+        <v>65.567579152032749</v>
+      </c>
+      <c r="C15">
+        <v>48.308968329288227</v>
+      </c>
+      <c r="D15">
+        <v>17.706511192592487</v>
+      </c>
+      <c r="E15">
+        <v>0.14428863064572478</v>
+      </c>
+      <c r="F15">
+        <v>54.133620543018225</v>
+      </c>
+      <c r="G15">
+        <v>41.225371231400281</v>
+      </c>
+      <c r="H15">
+        <v>4121.6866384988625</v>
+      </c>
+      <c r="P15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q15">
+        <v>2.5246000539505382</v>
+      </c>
+      <c r="U15" t="s">
+        <v>152</v>
+      </c>
+      <c r="V15">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.82460881937370956</v>
+      </c>
+      <c r="B16">
+        <v>65.455152206198207</v>
+      </c>
+      <c r="C16">
+        <v>54.324122616806022</v>
+      </c>
+      <c r="D16">
+        <v>22.415355286059388</v>
+      </c>
+      <c r="E16">
+        <v>0.16226352227642057</v>
+      </c>
+      <c r="F16">
+        <v>54.015732790920218</v>
+      </c>
+      <c r="G16">
+        <v>51.891441469397407</v>
+      </c>
+      <c r="H16">
+        <v>4117.3937915073393</v>
+      </c>
+      <c r="P16" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q16">
+        <v>2</v>
+      </c>
+      <c r="U16" t="s">
+        <v>153</v>
+      </c>
+      <c r="V16">
+        <v>2701.7574823170662</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.86469037362827361</v>
+      </c>
+      <c r="B17">
+        <v>65.398869524339688</v>
+      </c>
+      <c r="C17">
+        <v>56.947254617299059</v>
+      </c>
+      <c r="D17">
+        <v>24.645323003055186</v>
+      </c>
+      <c r="E17">
+        <v>0.17010311079404694</v>
+      </c>
+      <c r="F17">
+        <v>53.964317269944829</v>
+      </c>
+      <c r="G17">
+        <v>56.908115769127662</v>
+      </c>
+      <c r="H17">
+        <v>4115.5034122944799</v>
+      </c>
+      <c r="P17" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q17">
+        <v>295</v>
+      </c>
+      <c r="U17" t="s">
+        <v>154</v>
+      </c>
+      <c r="V17">
+        <v>607.40950591660658</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.88528183975786545</v>
+      </c>
+      <c r="B18">
+        <v>65.368376816372319</v>
+      </c>
+      <c r="C18">
+        <v>58.293786227869589</v>
+      </c>
+      <c r="D18">
+        <v>25.831814439868094</v>
+      </c>
+      <c r="E18">
+        <v>0.174127647656448</v>
+      </c>
+      <c r="F18">
+        <v>53.937916005913472</v>
+      </c>
+      <c r="G18">
+        <v>59.568708410660911</v>
+      </c>
+      <c r="H18">
+        <v>4114.5336825930635</v>
+      </c>
+      <c r="P18" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q18">
+        <v>3918396.6301116217</v>
+      </c>
+      <c r="U18" t="s">
+        <v>157</v>
+      </c>
+      <c r="V18">
+        <v>2.8660830844226021E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.88889701326702231</v>
+      </c>
+      <c r="B19">
+        <v>65.362913661429687</v>
+      </c>
+      <c r="C19">
+        <v>58.530100089404549</v>
+      </c>
+      <c r="D19">
+        <v>26.042983751907691</v>
+      </c>
+      <c r="E19">
+        <v>0.17483396407300358</v>
+      </c>
+      <c r="F19">
+        <v>53.933281988181442</v>
+      </c>
+      <c r="G19">
+        <v>60.041588812082516</v>
+      </c>
+      <c r="H19">
+        <v>4114.3635391871867</v>
+      </c>
+      <c r="P19" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q19">
+        <v>568.31515964466087</v>
+      </c>
+      <c r="U19" t="s">
+        <v>158</v>
+      </c>
+      <c r="V19">
+        <v>1.1283791670955128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.89251218677617916</v>
+      </c>
+      <c r="B20">
+        <v>69.942591178814197</v>
+      </c>
+      <c r="C20">
+        <v>58.766394140834969</v>
+      </c>
+      <c r="D20">
+        <v>26.255007343786932</v>
+      </c>
+      <c r="E20">
+        <v>0.17554022654023732</v>
+      </c>
+      <c r="F20">
+        <v>53.928648174352205</v>
+      </c>
+      <c r="G20">
+        <v>60.516203310845576</v>
+      </c>
+      <c r="H20">
+        <v>4361.4656339860621</v>
+      </c>
+      <c r="P20" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q20">
+        <v>330.95619595062249</v>
+      </c>
+      <c r="U20" t="s">
+        <v>159</v>
+      </c>
+      <c r="V20">
+        <v>2.5806399999999999E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.89550750703687865</v>
+      </c>
+      <c r="B21">
+        <v>69.940864237446377</v>
+      </c>
+      <c r="C21">
+        <v>58.97589173657444</v>
+      </c>
+      <c r="D21">
+        <v>26.431345272435117</v>
+      </c>
+      <c r="E21">
+        <v>0.17616637573989724</v>
+      </c>
+      <c r="F21">
+        <v>53.924648719035773</v>
+      </c>
+      <c r="G21">
+        <v>60.938552633622137</v>
+      </c>
+      <c r="H21">
+        <v>4361.4758916774308</v>
+      </c>
+      <c r="P21" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q21">
+        <v>860512.87157219567</v>
+      </c>
+      <c r="U21" t="s">
+        <v>160</v>
+      </c>
+      <c r="V21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.91048410834037596</v>
+      </c>
+      <c r="B22">
+        <v>69.931843638798796</v>
+      </c>
+      <c r="C22">
+        <v>60.023294291627977</v>
+      </c>
+      <c r="D22">
+        <v>27.322447141164272</v>
+      </c>
+      <c r="E22">
+        <v>0.17929692484986159</v>
+      </c>
+      <c r="F22">
+        <v>53.904651664612338</v>
+      </c>
+      <c r="G22">
+        <v>63.071014333416912</v>
+      </c>
+      <c r="H22">
+        <v>4361.5273187768489</v>
+      </c>
+      <c r="O22" t="s">
+        <v>33</v>
+      </c>
+      <c r="P22">
+        <v>22.63750198403805</v>
+      </c>
+      <c r="U22" t="s">
+        <v>161</v>
+      </c>
+      <c r="V22">
+        <v>5.7321661688452041E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.98536711485786255</v>
+      </c>
+      <c r="B23">
+        <v>69.877151501681041</v>
+      </c>
+      <c r="C23">
+        <v>65.25787199215155</v>
+      </c>
+      <c r="D23">
+        <v>32.013190158462493</v>
+      </c>
+      <c r="E23">
+        <v>0.19494390635000208</v>
+      </c>
+      <c r="F23">
+        <v>53.804671947685421</v>
+      </c>
+      <c r="G23">
+        <v>74.246891579378826</v>
+      </c>
+      <c r="H23">
+        <v>4361.787936572835</v>
+      </c>
+      <c r="U23" t="s">
+        <v>162</v>
+      </c>
+      <c r="V23">
+        <v>2.2567583341910256</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1.0286252562950227</v>
+      </c>
+      <c r="B24">
+        <v>69.838135297268806</v>
+      </c>
+      <c r="C24">
+        <v>68.279745130429987</v>
+      </c>
+      <c r="D24">
+        <v>34.901491223332876</v>
+      </c>
+      <c r="E24">
+        <v>0.20397797170418361</v>
+      </c>
+      <c r="F24">
+        <v>53.74693209372348</v>
+      </c>
+      <c r="G24">
+        <v>81.088539830779169</v>
+      </c>
+      <c r="H24">
+        <v>4361.9314590447857</v>
+      </c>
+      <c r="U24" t="s">
+        <v>163</v>
+      </c>
+      <c r="V24">
+        <v>2.9032199999999998E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1.0319638287815596</v>
+      </c>
+      <c r="B25">
+        <v>65.052479876115214</v>
+      </c>
+      <c r="C25">
+        <v>68.51289907758553</v>
+      </c>
+      <c r="D25">
+        <v>35.129837305682734</v>
+      </c>
+      <c r="E25">
+        <v>0.20467503738196999</v>
+      </c>
+      <c r="F25">
+        <v>53.742476546310023</v>
+      </c>
+      <c r="G25">
+        <v>81.628172622179605</v>
+      </c>
+      <c r="H25">
+        <v>4104.9232415629076</v>
+      </c>
+      <c r="U25" t="s">
+        <v>164</v>
+      </c>
+      <c r="V25">
+        <v>1771.6535433070865</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1.0353024012680965</v>
+      </c>
+      <c r="B26">
+        <v>65.046193352561417</v>
+      </c>
+      <c r="C26">
+        <v>68.730075777577383</v>
+      </c>
+      <c r="D26">
+        <v>35.35893511878038</v>
+      </c>
+      <c r="E26">
+        <v>0.20532437810858126</v>
+      </c>
+      <c r="F26">
+        <v>53.738206521290905</v>
+      </c>
+      <c r="G26">
+        <v>82.132208245665737</v>
+      </c>
+      <c r="H26">
+        <v>4104.7697860232947</v>
+      </c>
+      <c r="U26" t="s">
+        <v>165</v>
+      </c>
+      <c r="V26">
+        <v>0.193548</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1.0519952637007806</v>
+      </c>
+      <c r="B27">
+        <v>65.014353712402709</v>
+      </c>
+      <c r="C27">
+        <v>69.81573730750965</v>
+      </c>
+      <c r="D27">
+        <v>36.515298625782357</v>
+      </c>
+      <c r="E27">
+        <v>0.20857049710221512</v>
+      </c>
+      <c r="F27">
+        <v>53.716857249934613</v>
+      </c>
+      <c r="G27">
+        <v>84.67365372034439</v>
+      </c>
+      <c r="H27">
+        <v>4104.0027809080957</v>
+      </c>
+      <c r="U27" t="s">
+        <v>166</v>
+      </c>
+      <c r="V27">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1.1354595758642005</v>
+      </c>
+      <c r="B28">
+        <v>64.840799406492991</v>
+      </c>
+      <c r="C28">
+        <v>75.237938720789884</v>
+      </c>
+      <c r="D28">
+        <v>42.568761187958621</v>
+      </c>
+      <c r="E28">
+        <v>0.2247848740698403</v>
+      </c>
+      <c r="F28">
+        <v>53.610132228983893</v>
+      </c>
+      <c r="G28">
+        <v>98.135288529029836</v>
+      </c>
+      <c r="H28">
+        <v>4100.1745157104715</v>
+      </c>
+      <c r="U28" t="s">
+        <v>167</v>
+      </c>
+      <c r="V28">
+        <v>19.544100476116796</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1.3162929425472734</v>
+      </c>
+      <c r="B29">
+        <v>64.410879604319717</v>
+      </c>
+      <c r="C29">
+        <v>86.939957081514407</v>
+      </c>
+      <c r="D29">
+        <v>57.233092007317737</v>
+      </c>
+      <c r="E29">
+        <v>0.25979086613939201</v>
+      </c>
+      <c r="F29">
+        <v>53.379133044677786</v>
+      </c>
+      <c r="G29">
+        <v>130.07539505373396</v>
+      </c>
+      <c r="H29">
+        <v>4091.9216021457282</v>
+      </c>
+      <c r="U29" t="s">
+        <v>156</v>
+      </c>
+      <c r="V29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1.3516421620558319</v>
+      </c>
+      <c r="B30">
+        <v>64.314937350191414</v>
+      </c>
+      <c r="C30">
+        <v>89.215676992689964</v>
+      </c>
+      <c r="D30">
+        <v>60.346580952748404</v>
+      </c>
+      <c r="E30">
+        <v>0.26660077157273182</v>
+      </c>
+      <c r="F30">
+        <v>53.334074649197625</v>
+      </c>
+      <c r="G30">
+        <v>136.93183591418546</v>
+      </c>
+      <c r="H30">
+        <v>4090.3167779163919</v>
+      </c>
+      <c r="U30" t="s">
+        <v>168</v>
+      </c>
+      <c r="V30">
+        <v>5.8434509568333688</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1.3572646990402468</v>
+      </c>
+      <c r="B31">
+        <v>64.299386275840035</v>
+      </c>
+      <c r="C31">
+        <v>89.577259870082202</v>
+      </c>
+      <c r="D31">
+        <v>60.849215931149914</v>
+      </c>
+      <c r="E31">
+        <v>0.26768284907649437</v>
+      </c>
+      <c r="F31">
+        <v>53.326910806466451</v>
+      </c>
+      <c r="G31">
+        <v>138.03714120429038</v>
+      </c>
+      <c r="H31">
+        <v>4090.0617730579811</v>
+      </c>
+      <c r="U31" t="s">
+        <v>169</v>
+      </c>
+      <c r="V31">
+        <v>2.1055841909013528</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1.3628872360246618</v>
+      </c>
+      <c r="B32">
+        <v>64.421199641371174</v>
+      </c>
+      <c r="C32">
+        <v>89.938755083606026</v>
+      </c>
+      <c r="D32">
+        <v>61.35388367641886</v>
+      </c>
+      <c r="E32">
+        <v>0.26876468368240064</v>
+      </c>
+      <c r="F32">
+        <v>53.319747441286466</v>
+      </c>
+      <c r="G32">
+        <v>139.14653448498854</v>
+      </c>
+      <c r="H32">
+        <v>4097.1353516266145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1.3682761299922588</v>
+      </c>
+      <c r="B33">
+        <v>64.406590117385164</v>
+      </c>
+      <c r="C33">
+        <v>90.285886275262584</v>
+      </c>
+      <c r="D33">
+        <v>61.839489442753319</v>
+      </c>
+      <c r="E33">
+        <v>0.26980354667589901</v>
+      </c>
+      <c r="F33">
+        <v>53.312765863383262</v>
+      </c>
+      <c r="G33">
+        <v>140.21595842224505</v>
+      </c>
+      <c r="H33">
+        <v>4096.9076505290841</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1.3952205998302434</v>
+      </c>
+      <c r="B34">
+        <v>64.335624664518335</v>
+      </c>
+      <c r="C34">
+        <v>92.020621677646602</v>
+      </c>
+      <c r="D34">
+        <v>64.295568543119543</v>
+      </c>
+      <c r="E34">
+        <v>0.27499537728021789</v>
+      </c>
+      <c r="F34">
+        <v>53.277859522434753</v>
+      </c>
+      <c r="G34">
+        <v>145.44961581038319</v>
+      </c>
+      <c r="H34">
+        <v>4095.7697908897644</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1.4522021504058817</v>
+      </c>
+      <c r="B35">
+        <v>64.094869767300906</v>
+      </c>
+      <c r="C35">
+        <v>95.68340080206211</v>
+      </c>
+      <c r="D35">
+        <v>69.643432597170673</v>
+      </c>
+      <c r="E35">
+        <v>0.2859591028288726</v>
+      </c>
+      <c r="F35">
+        <v>53.204056756808988</v>
+      </c>
+      <c r="G35">
+        <v>156.99063560136773</v>
+      </c>
+      <c r="H35">
+        <v>4089.0295213054214</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1.4664334115125222</v>
+      </c>
+      <c r="B36">
+        <v>64.050771525958339</v>
+      </c>
+      <c r="C36">
+        <v>96.595334892707669</v>
+      </c>
+      <c r="D36">
+        <v>71.011617559144838</v>
+      </c>
+      <c r="E36">
+        <v>0.28868911391710267</v>
+      </c>
+      <c r="F36">
+        <v>53.185648606504678</v>
+      </c>
+      <c r="G36">
+        <v>159.97563604909561</v>
+      </c>
+      <c r="H36">
+        <v>4088.3086762340427</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1.4730446097400363</v>
+      </c>
+      <c r="B37">
+        <v>64.030113730076593</v>
+      </c>
+      <c r="C37">
+        <v>97.018739826963156</v>
+      </c>
+      <c r="D37">
+        <v>71.651628125258611</v>
+      </c>
+      <c r="E37">
+        <v>0.28995668570232308</v>
+      </c>
+      <c r="F37">
+        <v>53.177098220948672</v>
+      </c>
+      <c r="G37">
+        <v>161.37089160618544</v>
+      </c>
+      <c r="H37">
+        <v>4087.9738720764894</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1.4766244902885011</v>
+      </c>
+      <c r="B38">
+        <v>64.018882333250531</v>
+      </c>
+      <c r="C38">
+        <v>97.247945994164084</v>
+      </c>
+      <c r="D38">
+        <v>71.999353898505191</v>
+      </c>
+      <c r="E38">
+        <v>0.29064288561572182</v>
+      </c>
+      <c r="F38">
+        <v>53.172468598220078</v>
+      </c>
+      <c r="G38">
+        <v>162.12866943452099</v>
+      </c>
+      <c r="H38">
+        <v>4087.7925969409698</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1.4802043708369659</v>
+      </c>
+      <c r="B39">
+        <v>63.856216708701453</v>
+      </c>
+      <c r="C39">
+        <v>97.477111897029417</v>
+      </c>
+      <c r="D39">
+        <v>72.347900130414743</v>
+      </c>
+      <c r="E39">
+        <v>0.29132897355230974</v>
+      </c>
+      <c r="F39">
+        <v>53.167839139736529</v>
+      </c>
+      <c r="G39">
+        <v>162.88804807615136</v>
+      </c>
+      <c r="H39">
+        <v>4079.5616080773616</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1.4832977623324253</v>
+      </c>
+      <c r="B40">
+        <v>63.846155893002177</v>
+      </c>
+      <c r="C40">
+        <v>97.674633523671432</v>
+      </c>
+      <c r="D40">
+        <v>72.649740510713457</v>
+      </c>
+      <c r="E40">
+        <v>0.29192033265546913</v>
+      </c>
+      <c r="F40">
+        <v>53.163908190276899</v>
+      </c>
+      <c r="G40">
+        <v>163.5439475191591</v>
+      </c>
+      <c r="H40">
+        <v>4079.3930570634498</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1.4987647198097218</v>
+      </c>
+      <c r="B41">
+        <v>63.795488730459155</v>
+      </c>
+      <c r="C41">
+        <v>98.661870876106988</v>
+      </c>
+      <c r="D41">
+        <v>74.168105387048101</v>
+      </c>
+      <c r="E41">
+        <v>0.29487611405176228</v>
+      </c>
+      <c r="F41">
+        <v>53.144254257502844</v>
+      </c>
+      <c r="G41">
+        <v>166.84150761339333</v>
+      </c>
+      <c r="H41">
+        <v>4078.5503154526746</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1.5760995071962047</v>
+      </c>
+      <c r="B42">
+        <v>63.533127907003248</v>
+      </c>
+      <c r="C42">
+        <v>103.58850336445877</v>
+      </c>
+      <c r="D42">
+        <v>81.988691404246396</v>
+      </c>
+      <c r="E42">
+        <v>0.30962886208465334</v>
+      </c>
+      <c r="F42">
+        <v>53.04600495430369</v>
+      </c>
+      <c r="G42">
+        <v>183.77702313361635</v>
+      </c>
+      <c r="H42">
+        <v>4074.3369494526405</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1.9627734441286191</v>
+      </c>
+      <c r="B43">
+        <v>62.018501073069672</v>
+      </c>
+      <c r="C43">
+        <v>127.95172084967442</v>
+      </c>
+      <c r="D43">
+        <v>126.76794953740345</v>
+      </c>
+      <c r="E43">
+        <v>0.38265118566232487</v>
+      </c>
+      <c r="F43">
+        <v>52.555267152422431</v>
+      </c>
+      <c r="G43">
+        <v>278.48684293723875</v>
+      </c>
+      <c r="H43">
+        <v>4053.4529059904771</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>2.3140317542024285</v>
+      </c>
+      <c r="B44">
+        <v>60.36601867995175</v>
+      </c>
+      <c r="C44">
+        <v>149.51739289582929</v>
+      </c>
+      <c r="D44">
+        <v>175.51282037142909</v>
+      </c>
+      <c r="E44">
+        <v>0.44740010298280414</v>
+      </c>
+      <c r="F44">
+        <v>52.111969530860179</v>
+      </c>
+      <c r="G44">
+        <v>377.54116346103501</v>
+      </c>
+      <c r="H44">
+        <v>4034.5517107077549</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>2.7954019103451002</v>
+      </c>
+      <c r="B45">
+        <v>57.698984571549417</v>
+      </c>
+      <c r="C45">
+        <v>178.07187077238544</v>
+      </c>
+      <c r="D45">
+        <v>254.40044311166309</v>
+      </c>
+      <c r="E45">
+        <v>0.53333578192206277</v>
+      </c>
+      <c r="F45">
+        <v>51.50747424551065</v>
+      </c>
+      <c r="G45">
+        <v>531.32229562064379</v>
+      </c>
+      <c r="H45">
+        <v>4008.5395797803008</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>3.1454353119362026</v>
+      </c>
+      <c r="B46">
+        <v>55.513068461012253</v>
+      </c>
+      <c r="C46">
+        <v>197.95514365075641</v>
+      </c>
+      <c r="D46">
+        <v>320.23023360328011</v>
+      </c>
+      <c r="E46">
+        <v>0.59334517410571364</v>
+      </c>
+      <c r="F46">
+        <v>51.070910480243619</v>
+      </c>
+      <c r="G46">
+        <v>653.84253480862651</v>
+      </c>
+      <c r="H46">
+        <v>3989.9511164758087</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>3.495468713527305</v>
+      </c>
+      <c r="B47">
+        <v>53.095427303889252</v>
+      </c>
+      <c r="C47">
+        <v>217.03963572076998</v>
+      </c>
+      <c r="D47">
+        <v>392.88223362014764</v>
+      </c>
+      <c r="E47">
+        <v>0.65110381591850719</v>
+      </c>
+      <c r="F47">
+        <v>50.63650342521435</v>
+      </c>
+      <c r="G47">
+        <v>786.02768486195203</v>
+      </c>
+      <c r="H47">
+        <v>3971.3385699999121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>3.7836008032649535</v>
+      </c>
+      <c r="B48">
+        <v>50.988224087935748</v>
+      </c>
+      <c r="C48">
+        <v>232.0792268561583</v>
+      </c>
+      <c r="D48">
+        <v>457.59756505295053</v>
+      </c>
+      <c r="E48">
+        <v>0.6967517609705427</v>
+      </c>
+      <c r="F48">
+        <v>50.280681929649283</v>
+      </c>
+      <c r="G48">
+        <v>898.97271028363582</v>
+      </c>
+      <c r="H48">
+        <v>3955.9488775366749</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>4.0717328930026015</v>
+      </c>
+      <c r="B49">
+        <v>48.804651129203798</v>
+      </c>
+      <c r="C49">
+        <v>246.50253864066747</v>
+      </c>
+      <c r="D49">
+        <v>526.55780632421465</v>
+      </c>
+      <c r="E49">
+        <v>0.74065517356642929</v>
+      </c>
+      <c r="F49">
+        <v>49.926316139512039</v>
+      </c>
+      <c r="G49">
+        <v>1014.3749265344077</v>
+      </c>
+      <c r="H49">
+        <v>3940.7885292182427</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>4.4188736132167348</v>
+      </c>
+      <c r="B50">
+        <v>46.0945897437159</v>
+      </c>
+      <c r="C50">
+        <v>263.04306442684987</v>
+      </c>
+      <c r="D50">
+        <v>615.02335967031797</v>
+      </c>
+      <c r="E50">
+        <v>0.79117949865453219</v>
+      </c>
+      <c r="F50">
+        <v>49.501119580583683</v>
+      </c>
+      <c r="G50">
+        <v>1155.2532011340631</v>
+      </c>
+      <c r="H50">
+        <v>3922.5929831412163</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>4.7910198845103373</v>
+      </c>
+      <c r="B51">
+        <v>43.200818545588582</v>
+      </c>
+      <c r="C51">
+        <v>279.74023465988648</v>
+      </c>
+      <c r="D51">
+        <v>716.0493801864385</v>
+      </c>
+      <c r="E51">
+        <v>0.84240737485924888</v>
+      </c>
+      <c r="F51">
+        <v>49.047535721979912</v>
+      </c>
+      <c r="G51">
+        <v>1302.9390868735759</v>
+      </c>
+      <c r="H51">
+        <v>3902.9891031397269</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>5.2270961920660604</v>
+      </c>
+      <c r="B52">
+        <v>39.770738531298974</v>
+      </c>
+      <c r="C52">
+        <v>297.93204059896993</v>
+      </c>
+      <c r="D52">
+        <v>842.05023858273307</v>
+      </c>
+      <c r="E52">
+        <v>0.89853200822463719</v>
+      </c>
+      <c r="F52">
+        <v>48.518849782958</v>
+      </c>
+      <c r="G52">
+        <v>1474.5181183094178</v>
+      </c>
+      <c r="H52">
+        <v>3880.1185232376306</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>5.4754579573430178</v>
+      </c>
+      <c r="B53">
+        <v>36.34963149994924</v>
+      </c>
+      <c r="C53">
+        <v>307.48383002455358</v>
+      </c>
+      <c r="D53">
+        <v>917.24747272005266</v>
+      </c>
+      <c r="E53">
+        <v>0.92816874913561231</v>
+      </c>
+      <c r="F53">
+        <v>48.219618824961081</v>
+      </c>
+      <c r="G53">
+        <v>1641.3031379717308</v>
+      </c>
+      <c r="H53">
+        <v>3867.1029739999503</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>5.7238197226199752</v>
+      </c>
+      <c r="B54">
+        <v>31.33470540960294</v>
+      </c>
+      <c r="C54">
+        <v>315.98561534596064</v>
+      </c>
+      <c r="D54">
+        <v>994.69207245760958</v>
+      </c>
+      <c r="E54">
+        <v>0.95471253272627088</v>
+      </c>
+      <c r="F54">
+        <v>47.921452206479145</v>
+      </c>
+      <c r="G54">
+        <v>1857.9230740226828</v>
+      </c>
+      <c r="H54">
+        <v>3829.6371078586344</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>5.8587533565708485</v>
+      </c>
+      <c r="B55">
+        <v>29.020919011621132</v>
+      </c>
+      <c r="C55">
+        <v>320.0660309549985</v>
+      </c>
+      <c r="D55">
+        <v>1037.6077043496743</v>
+      </c>
+      <c r="E55">
+        <v>0.96753622336117551</v>
+      </c>
+      <c r="F55">
+        <v>47.760733075176077</v>
+      </c>
+      <c r="G55">
+        <v>1967.2417296350411</v>
+      </c>
+      <c r="H55">
+        <v>3821.834887612858</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>5.9936869905217218</v>
+      </c>
+      <c r="B56">
+        <v>26.791127053422493</v>
+      </c>
+      <c r="C56">
+        <v>323.84152064285712</v>
+      </c>
+      <c r="D56">
+        <v>1081.0532663203467</v>
+      </c>
+      <c r="E56">
+        <v>0.97945727174429598</v>
+      </c>
+      <c r="F56">
+        <v>47.600349017836059</v>
+      </c>
+      <c r="G56">
+        <v>2072.4619070330077</v>
+      </c>
+      <c r="H56">
+        <v>3814.6883292220796</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>6.1250651795554596</v>
+      </c>
+      <c r="B57">
+        <v>24.780137008269982</v>
+      </c>
+      <c r="C57">
+        <v>327.23860383466189</v>
+      </c>
+      <c r="D57">
+        <v>1123.8247858275054</v>
+      </c>
+      <c r="E57">
+        <v>0.99023790021428049</v>
+      </c>
+      <c r="F57">
+        <v>47.444867453296716</v>
+      </c>
+      <c r="G57">
+        <v>2165.8438400710447</v>
+      </c>
+      <c r="H57">
+        <v>3806.9683056197878</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>6.4832444363982047</v>
+      </c>
+      <c r="B58">
+        <v>19.763162405629977</v>
+      </c>
+      <c r="C58">
+        <v>335.27373487117143</v>
+      </c>
+      <c r="D58">
+        <v>1242.5233407488504</v>
+      </c>
+      <c r="E58">
+        <v>1.0159959156605463</v>
+      </c>
+      <c r="F58">
+        <v>47.02187822227107</v>
+      </c>
+      <c r="G58">
+        <v>2395.5306494791043</v>
+      </c>
+      <c r="H58">
+        <v>3786.1162907640819</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>6.8557952559440709</v>
+      </c>
+      <c r="B59">
+        <v>15.438083219340074</v>
+      </c>
+      <c r="C59">
+        <v>341.88952456659314</v>
+      </c>
+      <c r="D59">
+        <v>1368.707188247035</v>
+      </c>
+      <c r="E59">
+        <v>1.0376156325693484</v>
+      </c>
+      <c r="F59">
+        <v>46.584489360662673</v>
+      </c>
+      <c r="G59">
+        <v>2588.4290637956383</v>
+      </c>
+      <c r="H59">
+        <v>3764.5981279041116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>7.1672420079755961</v>
+      </c>
+      <c r="B60">
+        <v>12.83739177710566</v>
+      </c>
+      <c r="C60">
+        <v>346.29693083673328</v>
+      </c>
+      <c r="D60">
+        <v>1475.8935643981438</v>
+      </c>
+      <c r="E60">
+        <v>1.0523497480054442</v>
+      </c>
+      <c r="F60">
+        <v>46.221050291761713</v>
+      </c>
+      <c r="G60">
+        <v>2699.3572014997139</v>
+      </c>
+      <c r="H60">
+        <v>3746.1434358065453</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>7.4786887600071212</v>
+      </c>
+      <c r="B61">
+        <v>11.995706913647505</v>
+      </c>
+      <c r="C61">
+        <v>350.22044326175705</v>
+      </c>
+      <c r="D61">
+        <v>1584.361210722994</v>
+      </c>
+      <c r="E61">
+        <v>1.0656678903865546</v>
+      </c>
+      <c r="F61">
+        <v>45.859486696600193</v>
+      </c>
+      <c r="G61">
+        <v>2727.8504522551939</v>
+      </c>
+      <c r="H61">
+        <v>3727.8489783715745</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>7.9374865326908886</v>
+      </c>
+      <c r="B62">
+        <v>10.991396042985238</v>
+      </c>
+      <c r="C62">
+        <v>355.62582973951811</v>
+      </c>
+      <c r="D62">
+        <v>1746.288800038194</v>
+      </c>
+      <c r="E62">
+        <v>1.0842409357242653</v>
+      </c>
+      <c r="F62">
+        <v>45.329639396831332</v>
+      </c>
+      <c r="G62">
+        <v>2758.1245249992116</v>
+      </c>
+      <c r="H62">
+        <v>3701.0443065784066</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>8.7771913007536373</v>
+      </c>
+      <c r="B63">
+        <v>9.3580463176904107</v>
+      </c>
+      <c r="C63">
+        <v>364.63025304655719</v>
+      </c>
+      <c r="D63">
+        <v>2048.72280458552</v>
+      </c>
+      <c r="E63">
+        <v>1.1157983626814951</v>
+      </c>
+      <c r="F63">
+        <v>44.367298917975504</v>
+      </c>
+      <c r="G63">
+        <v>2800.5648211493512</v>
+      </c>
+      <c r="H63">
+        <v>3650.9992617999214</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>9.616896068816386</v>
+      </c>
+      <c r="B64">
+        <v>8.1409716308753861</v>
+      </c>
+      <c r="C64">
+        <v>372.46720483943056</v>
+      </c>
+      <c r="D64">
+        <v>2358.1997500885059</v>
+      </c>
+      <c r="E64">
+        <v>1.144118887214155</v>
+      </c>
+      <c r="F64">
+        <v>43.41871744041913</v>
+      </c>
+      <c r="G64">
+        <v>2821.1308026706479</v>
+      </c>
+      <c r="H64">
+        <v>3600.5389676926056</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>10.342928859592737</v>
+      </c>
+      <c r="B65">
+        <v>7.5436289345806404</v>
+      </c>
+      <c r="C65">
+        <v>378.53775862214195</v>
+      </c>
+      <c r="D65">
+        <v>2630.8051134323628</v>
+      </c>
+      <c r="E65">
+        <v>1.1666921646514257</v>
+      </c>
+      <c r="F65">
+        <v>42.610552347058878</v>
+      </c>
+      <c r="G65">
+        <v>2816.9356394188922</v>
+      </c>
+      <c r="H65">
+        <v>3556.3833535472763</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>11.045133151641782</v>
+      </c>
+      <c r="B66">
+        <v>7.1280012913247521</v>
+      </c>
+      <c r="C66">
+        <v>384.0583479127626</v>
+      </c>
+      <c r="D66">
+        <v>2898.5278157930115</v>
+      </c>
+      <c r="E66">
+        <v>1.1876588067917706</v>
+      </c>
+      <c r="F66">
+        <v>41.839013153505753</v>
+      </c>
+      <c r="G66">
+        <v>2804.8162250474261</v>
+      </c>
+      <c r="H66">
+        <v>3513.48548386926</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>11.791262059146158</v>
+      </c>
+      <c r="B67">
+        <v>6.9779950936275146</v>
+      </c>
+      <c r="C67">
+        <v>389.72356843197707</v>
+      </c>
+      <c r="D67">
+        <v>3187.1523522425828</v>
+      </c>
+      <c r="E67">
+        <v>1.2095461689886391</v>
+      </c>
+      <c r="F67">
+        <v>41.029667884618028</v>
+      </c>
+      <c r="G67">
+        <v>2777.9327243883336</v>
+      </c>
+      <c r="H67">
+        <v>3466.7385875284676</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>12.646241917353638</v>
+      </c>
+      <c r="B68">
+        <v>6.7003949838851771</v>
+      </c>
+      <c r="C68">
+        <v>396.13348652452856</v>
+      </c>
+      <c r="D68">
+        <v>3523.0323604972641</v>
+      </c>
+      <c r="E68">
+        <v>1.2346683780404948</v>
+      </c>
+      <c r="F68">
+        <v>40.115178065310346</v>
+      </c>
+      <c r="G68">
+        <v>2750.2235399288338</v>
+      </c>
+      <c r="H68">
+        <v>3412.5409746359942</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>14.166572173766362</v>
+      </c>
+      <c r="B69">
+        <v>6.368182487050861</v>
+      </c>
+      <c r="C69">
+        <v>408.09364742176768</v>
+      </c>
+      <c r="D69">
+        <v>4133.94273598165</v>
+      </c>
+      <c r="E69">
+        <v>1.281921196681155</v>
+      </c>
+      <c r="F69">
+        <v>38.515692020376356</v>
+      </c>
+      <c r="G69">
+        <v>2689.4753210710965</v>
+      </c>
+      <c r="H69">
+        <v>3312.5892151917938</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>15.485165804275145</v>
+      </c>
+      <c r="B70">
+        <v>6.2484655241055851</v>
+      </c>
+      <c r="C70">
+        <v>418.02422088129083</v>
+      </c>
+      <c r="D70">
+        <v>4678.2743171655657</v>
+      </c>
+      <c r="E70">
+        <v>1.3224255501800191</v>
+      </c>
+      <c r="F70">
+        <v>37.170822445037672</v>
+      </c>
+      <c r="G70">
+        <v>2626.4123780536802</v>
+      </c>
+      <c r="H70">
+        <v>3223.3187487899677</v>
+      </c>
+      <c r="K70">
+        <f>F2-F71</f>
+        <v>18.886909537442207</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>16.469703176840373</v>
+      </c>
+      <c r="B71">
+        <v>-80.873686127584406</v>
+      </c>
+      <c r="C71">
+        <v>425.14965661132982</v>
+      </c>
+      <c r="D71">
+        <v>5093.1916565429592</v>
+      </c>
+      <c r="E71">
+        <v>1.3523213227778674</v>
+      </c>
+      <c r="F71">
+        <v>36.194792446595841</v>
+      </c>
+      <c r="G71">
+        <v>2572.1353698779494</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>17.027344616304145</v>
+      </c>
+      <c r="B72">
+        <v>-69.732924350860443</v>
+      </c>
+      <c r="C72">
+        <v>383.28160240211332</v>
+      </c>
+      <c r="D72">
+        <v>5318.3102109736119</v>
+      </c>
+      <c r="E72">
+        <v>1.2227899666099531</v>
+      </c>
+      <c r="F72">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G72">
+        <v>2119.3244408985565</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>17.584986055767917</v>
+      </c>
+      <c r="B73">
+        <v>-59.109306614573271</v>
+      </c>
+      <c r="C73">
+        <v>347.41522788282168</v>
+      </c>
+      <c r="D73">
+        <v>5521.7673035281905</v>
+      </c>
+      <c r="E73">
+        <v>1.1113748773574117</v>
+      </c>
+      <c r="F73">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G73">
+        <v>1743.5935672274436</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>17.853171835514114</v>
+      </c>
+      <c r="B74">
+        <v>-54.675847306604098</v>
+      </c>
+      <c r="C74">
+        <v>332.17780959170994</v>
+      </c>
+      <c r="D74">
+        <v>5612.8695458643342</v>
+      </c>
+      <c r="E74">
+        <v>1.0639269720530962</v>
+      </c>
+      <c r="F74">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G74">
+        <v>1586.793164528583</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>18.121357615260312</v>
+      </c>
+      <c r="B75">
+        <v>-47.960332543405748</v>
+      </c>
+      <c r="C75">
+        <v>318.30645858878324</v>
+      </c>
+      <c r="D75">
+        <v>5700.0512899612322</v>
+      </c>
+      <c r="E75">
+        <v>1.0206916364337437</v>
+      </c>
+      <c r="F75">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G75">
+        <v>1349.2821497535344</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>18.370116845688738</v>
+      </c>
+      <c r="B76">
+        <v>-42.098146095779612</v>
+      </c>
+      <c r="C76">
+        <v>307.13306914434503</v>
+      </c>
+      <c r="D76">
+        <v>5777.8128466286262</v>
+      </c>
+      <c r="E76">
+        <v>0.98589284064812555</v>
+      </c>
+      <c r="F76">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G76">
+        <v>1141.9512300738782</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>18.691400091274833</v>
+      </c>
+      <c r="B77">
+        <v>-36.173584636323298</v>
+      </c>
+      <c r="C77">
+        <v>294.60159977639495</v>
+      </c>
+      <c r="D77">
+        <v>5874.4257470849616</v>
+      </c>
+      <c r="E77">
+        <v>0.94689899422296109</v>
+      </c>
+      <c r="F77">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G77">
+        <v>932.414261732461</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>19.014752373660581</v>
+      </c>
+      <c r="B78">
+        <v>-31.837000468240014</v>
+      </c>
+      <c r="C78">
+        <v>283.66201955089235</v>
+      </c>
+      <c r="D78">
+        <v>5967.8783217614109</v>
+      </c>
+      <c r="E78">
+        <v>0.91288921203943174</v>
+      </c>
+      <c r="F78">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G78">
+        <v>779.0400912126828</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>19.29764329271844</v>
+      </c>
+      <c r="B79">
+        <v>-29.995885250132979</v>
+      </c>
+      <c r="C79">
+        <v>274.93893991756147</v>
+      </c>
+      <c r="D79">
+        <v>6046.8779411936785</v>
+      </c>
+      <c r="E79">
+        <v>0.8857634349109279</v>
+      </c>
+      <c r="F79">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G79">
+        <v>713.92443601872037</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>19.729005492310531</v>
+      </c>
+      <c r="B80">
+        <v>-27.844633568469298</v>
+      </c>
+      <c r="C80">
+        <v>262.4759232495548</v>
+      </c>
+      <c r="D80">
+        <v>6162.7552467340565</v>
+      </c>
+      <c r="E80">
+        <v>0.84694315810188969</v>
+      </c>
+      <c r="F80">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G80">
+        <v>637.84002730764098</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>20.253833455885662</v>
+      </c>
+      <c r="B81">
+        <v>-25.60009719781165</v>
+      </c>
+      <c r="C81">
+        <v>248.46869701502027</v>
+      </c>
+      <c r="D81">
+        <v>6296.7833230082597</v>
+      </c>
+      <c r="E81">
+        <v>0.803210714872722</v>
+      </c>
+      <c r="F81">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G81">
+        <v>558.4563717142006</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>20.883434573175116</v>
+      </c>
+      <c r="B82">
+        <v>-23.357491874397628</v>
+      </c>
+      <c r="C82">
+        <v>233.07423155476556</v>
+      </c>
+      <c r="D82">
+        <v>6448.2986453964631</v>
+      </c>
+      <c r="E82">
+        <v>0.75500888224424889</v>
+      </c>
+      <c r="F82">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G82">
+        <v>479.14101244748775</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>21.498803304040162</v>
+      </c>
+      <c r="B83">
+        <v>-21.530545480276228</v>
+      </c>
+      <c r="C83">
+        <v>219.27633616641094</v>
+      </c>
+      <c r="D83">
+        <v>6587.4225595516982</v>
+      </c>
+      <c r="E83">
+        <v>0.71167096695981313</v>
+      </c>
+      <c r="F83">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G83">
+        <v>414.526473233709</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>22.313036094653683</v>
+      </c>
+      <c r="B84">
+        <v>-19.541032561605597</v>
+      </c>
+      <c r="C84">
+        <v>202.5909314106342</v>
+      </c>
+      <c r="D84">
+        <v>6759.0608988694512</v>
+      </c>
+      <c r="E84">
+        <v>0.65907594055524277</v>
+      </c>
+      <c r="F84">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G84">
+        <v>344.16236134000189</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>23.121177527408207</v>
+      </c>
+      <c r="B85">
+        <v>-17.917648553912244</v>
+      </c>
+      <c r="C85">
+        <v>187.47785956239062</v>
+      </c>
+      <c r="D85">
+        <v>6916.5887107788922</v>
+      </c>
+      <c r="E85">
+        <v>0.6112420295911104</v>
+      </c>
+      <c r="F85">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G85">
+        <v>286.7473162343307</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>24.125703314005069</v>
+      </c>
+      <c r="B86">
+        <v>-16.341790038163658</v>
+      </c>
+      <c r="C86">
+        <v>170.29988358849684</v>
+      </c>
+      <c r="D86">
+        <v>7096.1540068059057</v>
+      </c>
+      <c r="E86">
+        <v>0.55662537032482295</v>
+      </c>
+      <c r="F86">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G86">
+        <v>231.01312929329995</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>25.381201960539926</v>
+      </c>
+      <c r="B87">
+        <v>-14.809306062975811</v>
+      </c>
+      <c r="C87">
+        <v>150.78591408055814</v>
+      </c>
+      <c r="D87">
+        <v>7297.5143677279248</v>
+      </c>
+      <c r="E87">
+        <v>0.49423452060021511</v>
+      </c>
+      <c r="F87">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G87">
+        <v>176.8129917151621</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>27.181201960539926</v>
+      </c>
+      <c r="B88">
+        <v>-13.181198022233716</v>
+      </c>
+      <c r="C88">
+        <v>125.67891869537505</v>
+      </c>
+      <c r="D88">
+        <v>7545.8941476900145</v>
+      </c>
+      <c r="E88">
+        <v>0.41338402669848689</v>
+      </c>
+      <c r="F88">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G88">
+        <v>119.23086933800812</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>28.981201960539927</v>
+      </c>
+      <c r="B89">
+        <v>-12.025986769143632</v>
+      </c>
+      <c r="C89">
+        <v>103.04453173802273</v>
+      </c>
+      <c r="D89">
+        <v>7751.4329674621986</v>
+      </c>
+      <c r="E89">
+        <v>0.33992354822657284</v>
+      </c>
+      <c r="F89">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G89">
+        <v>78.373927364686267</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>30.781201960539928</v>
+      </c>
+      <c r="B90">
+        <v>-11.197342680963486</v>
+      </c>
+      <c r="C90">
+        <v>82.183471817216741</v>
+      </c>
+      <c r="D90">
+        <v>7917.9138782930713</v>
+      </c>
+      <c r="E90">
+        <v>0.27175082299122449</v>
+      </c>
+      <c r="F90">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G90">
+        <v>49.066851852089634</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>32.581201960539929</v>
+      </c>
+      <c r="B91">
+        <v>-10.608419130627054</v>
+      </c>
+      <c r="C91">
+        <v>62.589589239985429</v>
+      </c>
+      <c r="D91">
+        <v>8048.0520075898667</v>
+      </c>
+      <c r="E91">
+        <v>0.20734669519046914</v>
+      </c>
+      <c r="F91">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G91">
+        <v>28.238094117557743</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>34.381201960539926</v>
+      </c>
+      <c r="B92">
+        <v>-10.203494597491307</v>
+      </c>
+      <c r="C92">
+        <v>43.882646571600056</v>
+      </c>
+      <c r="D92">
+        <v>8143.7678055298702</v>
+      </c>
+      <c r="E92">
+        <v>0.14557422954385749</v>
+      </c>
+      <c r="F92">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G92">
+        <v>13.91692289485019</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>36.181201960539923</v>
+      </c>
+      <c r="B93">
+        <v>-9.9472509894857417</v>
+      </c>
+      <c r="C93">
+        <v>25.767639832521368</v>
+      </c>
+      <c r="D93">
+        <v>8206.3840615204153</v>
+      </c>
+      <c r="E93">
+        <v>8.5557395410178927E-2</v>
+      </c>
+      <c r="F93">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G93">
+        <v>4.8542253187025111</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>37.98120196053992</v>
+      </c>
+      <c r="B94">
+        <v>-9.8233874629661333</v>
+      </c>
+      <c r="C94">
+        <v>7.9932641624532401</v>
+      </c>
+      <c r="D94">
+        <v>8236.7354193683313</v>
+      </c>
+      <c r="E94">
+        <v>2.6551983413584748E-2</v>
+      </c>
+      <c r="F94">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G94">
+        <v>0.47348118892905627</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>39.305243654412855</v>
+      </c>
+      <c r="B95">
+        <v>-9.8151044074164524</v>
+      </c>
+      <c r="C95">
+        <v>4.9999999999956124</v>
+      </c>
+      <c r="D95">
+        <v>8238.7158226688971</v>
+      </c>
+      <c r="E95">
+        <v>1.660944812150875E-2</v>
+      </c>
+      <c r="F95">
+        <v>35.367506907531705</v>
+      </c>
+      <c r="G95">
+        <v>0.1805301645602026</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Monte Carlo mostly implemented
Need to read in # of runs from Excel still
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" tabRatio="551"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" tabRatio="551" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
@@ -842,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1537,11 +1537,11 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C30" t="str">
         <f>IF(B31="Single value","Value",IF(B31="Range of values","Start",IF(B31="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
+        <v>Mean</v>
       </c>
       <c r="D30" t="str">
         <f>IF(B31="Single value","",IF(B31="Range of values","Step",IF(B31="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
+        <v>Standard deviation</v>
       </c>
       <c r="E30" t="str">
         <f>IF(B31="Single value","",IF(B31="Range of values","End",IF(B31="Monte Carlo","","ERROR")))</f>
@@ -1556,13 +1556,15 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C31" s="3">
         <f>SUM(B:B)</f>
         <v>32.444185833819738</v>
       </c>
-      <c r="D31" s="1"/>
+      <c r="D31" s="1">
+        <v>2</v>
+      </c>
       <c r="E31" s="1"/>
       <c r="F31" t="s">
         <v>3</v>
@@ -1661,8 +1663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1723,7 +1725,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="1">
-        <v>4</v>
+        <v>4.49</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1907,7 +1909,7 @@
         <v>116</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="D26" t="s">
         <v>117</v>
@@ -1936,7 +1938,7 @@
       </c>
       <c r="C28" s="1">
         <f>C26*2.54^2/100^2</f>
-        <v>6.4515999999999998E-4</v>
+        <v>9.03224E-4</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1976,7 +1978,7 @@
         <v>108</v>
       </c>
       <c r="B34">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2019,7 +2021,7 @@
         <v>105</v>
       </c>
       <c r="B39">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2080,7 +2082,7 @@
       </c>
       <c r="C45" s="9">
         <f>B34*B37</f>
-        <v>5.7004591398468508E-6</v>
+        <v>7.6006121864624678E-6</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -2111,7 +2113,7 @@
       </c>
       <c r="C48" s="9">
         <f>B42*B39</f>
-        <v>2.3723030756386648E-5</v>
+        <v>3.1630707675182194E-5</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -2204,7 +2206,7 @@
   <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2250,11 +2252,11 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C5" t="str">
         <f>IF(B6="Single value","Value",IF(B6="Range of values","Start",IF(B6="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
+        <v>Mean</v>
       </c>
       <c r="D5" t="str">
         <f>IF(B6="Single value","",IF(B6="Range of values","Step",IF(B6="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
+        <v>Standard deviation</v>
       </c>
       <c r="E5" t="str">
         <f>IF(B6="Single value","",IF(B6="Range of values","End",IF(B6="Monte Carlo","","ERROR")))</f>
@@ -2275,13 +2277,15 @@
         <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" s="9">
         <f>$N$6*J6</f>
         <v>2.6104650300000001E-2</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1">
+        <v>1E-3</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
Fixed simconfig; Monte Carlo run # from Excel
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" tabRatio="551" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525" tabRatio="551" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="122">
   <si>
     <t>Total inert mass</t>
   </si>
@@ -384,6 +384,9 @@
   </si>
   <si>
     <t>Length (straight section)</t>
+  </si>
+  <si>
+    <t># of Monte Carlo runs</t>
   </si>
 </sst>
 </file>
@@ -516,27 +519,27 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="Simulation Conditions (Weather)"/>
+      <sheetName val="Rocket Parameters (Mass)"/>
+      <sheetName val="Engine Parameters"/>
+      <sheetName val="Propellant Parameters (Tanks)"/>
+      <sheetName val="Validation"/>
+      <sheetName val="Results 06-Oct-2017 15-52-58"/>
+      <sheetName val="Results 06-Oct-2017 16-04-00"/>
       <sheetName val="Simulation Conditions"/>
       <sheetName val="Rocket Parameters"/>
-      <sheetName val="Engine Parameters"/>
       <sheetName val="Propellant Parameters"/>
-      <sheetName val="Validation"/>
       <sheetName val="Results 27-Aug-2017 14-21-21"/>
       <sheetName val="Results 27-Aug-2017 14-26-37"/>
       <sheetName val="Results 27-Aug-2017 14-31-00"/>
       <sheetName val="Results 27-Aug-2017 14-32-33"/>
       <sheetName val="Results 27-Aug-2017 14-33-36"/>
-      <sheetName val="Results 27-Aug-2017 14-34-48"/>
-      <sheetName val="Results 27-Aug-2017 14-35-18"/>
-      <sheetName val="Results 27-Aug-2017 14-35-43"/>
-      <sheetName val="Results 24-Sep-2017 12-20-16"/>
-      <sheetName val="Results 24-Sep-2017 12-37-10"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
       <sheetData sheetId="5" refreshError="1"/>
       <sheetData sheetId="6" refreshError="1"/>
@@ -840,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,19 +967,55 @@
         <v>33</v>
       </c>
     </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17">
+      <formula1>1</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="G1" r:id="rId1" display="https://www.usclimatedata.com/climate/truth-or-consequences/new-mexico/united-states/usnm0332"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Validation!#REF!</xm:f>
+            <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B4 B7 B10 B13</xm:sqref>
+          <xm:sqref>B4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Validation!$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>B17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Validation!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B13 B10 B7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -988,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,7 +1509,7 @@
       </c>
       <c r="B14" s="2">
         <f>'Propellant Parameters (Tanks)'!N34*0.453592</f>
-        <v>11.562209199342742</v>
+        <v>12.871986458369594</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -1537,11 +1576,11 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C30" t="str">
         <f>IF(B31="Single value","Value",IF(B31="Range of values","Start",IF(B31="Monte Carlo","Mean","ERROR")))</f>
-        <v>Mean</v>
+        <v>Value</v>
       </c>
       <c r="D30" t="str">
         <f>IF(B31="Single value","",IF(B31="Range of values","Step",IF(B31="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v>Standard deviation</v>
+        <v/>
       </c>
       <c r="E30" t="str">
         <f>IF(B31="Single value","",IF(B31="Range of values","End",IF(B31="Monte Carlo","","ERROR")))</f>
@@ -1556,15 +1595,13 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C31" s="3">
         <f>SUM(B:B)</f>
-        <v>32.444185833819738</v>
-      </c>
-      <c r="D31" s="1">
-        <v>2</v>
-      </c>
+        <v>33.75396309284659</v>
+      </c>
+      <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" t="s">
         <v>3</v>
@@ -1663,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2205,8 +2242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2252,11 +2289,11 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C5" t="str">
         <f>IF(B6="Single value","Value",IF(B6="Range of values","Start",IF(B6="Monte Carlo","Mean","ERROR")))</f>
-        <v>Mean</v>
+        <v>Value</v>
       </c>
       <c r="D5" t="str">
         <f>IF(B6="Single value","",IF(B6="Range of values","Step",IF(B6="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v>Standard deviation</v>
+        <v/>
       </c>
       <c r="E5" t="str">
         <f>IF(B6="Single value","",IF(B6="Range of values","End",IF(B6="Monte Carlo","","ERROR")))</f>
@@ -2277,15 +2314,13 @@
         <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="9">
         <f>$N$6*J6</f>
         <v>2.6104650300000001E-2</v>
       </c>
-      <c r="D6" s="1">
-        <v>1E-3</v>
-      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" t="s">
         <v>60</v>
@@ -2572,7 +2607,7 @@
       </c>
       <c r="K31" s="8">
         <f>C34</f>
-        <v>56.603313253621714</v>
+        <v>64.103507771388223</v>
       </c>
       <c r="L31">
         <v>0.249</v>
@@ -2582,7 +2617,7 @@
       </c>
       <c r="N31" s="13">
         <f>K31*L31</f>
-        <v>14.094225000151807</v>
+        <v>15.961773435075667</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -2594,7 +2629,7 @@
       </c>
       <c r="K32" s="8">
         <f>C37</f>
-        <v>14.981999088208545</v>
+        <v>18.732067085738368</v>
       </c>
       <c r="L32">
         <v>0.27200000000000002</v>
@@ -2604,7 +2639,7 @@
       </c>
       <c r="N32" s="13">
         <f>K32*L32</f>
-        <v>4.0751037519927245</v>
+        <v>5.0951222473208366</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -2636,12 +2671,13 @@
         <v>9</v>
       </c>
       <c r="C34" s="8">
-        <v>56.603313253621714</v>
+        <f>C6/((PI()/4)*C12^2)/N12</f>
+        <v>64.103507771388223</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="J34" s="12" t="s">
         <v>79</v>
@@ -2651,7 +2687,7 @@
       <c r="M34" s="12"/>
       <c r="N34" s="14">
         <f>SUM(N30:N33)</f>
-        <v>25.490328752144531</v>
+        <v>28.377895682396503</v>
       </c>
       <c r="O34" t="s">
         <v>50</v>
@@ -2670,7 +2706,8 @@
         <v>9</v>
       </c>
       <c r="C37" s="8">
-        <v>14.981999088208545</v>
+        <f>C8/((PI()/4)*C12^2)/N12</f>
+        <v>18.732067085738368</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>

</xml_diff>

<commit_message>
Began range of values implementation
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525" tabRatio="551" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525" tabRatio="551" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
     <sheet name="Rocket Parameters (Mass)" sheetId="1" r:id="rId2"/>
     <sheet name="Engine Parameters" sheetId="4" r:id="rId3"/>
     <sheet name="Propellant Parameters (Tanks)" sheetId="5" r:id="rId4"/>
-    <sheet name="Validation" sheetId="3" state="hidden" r:id="rId5"/>
+    <sheet name="Validation" sheetId="3" r:id="rId5"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId6"/>
@@ -1027,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,8 +1601,13 @@
         <f>SUM(B:B)</f>
         <v>33.75396309284659</v>
       </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="D31" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E31" s="3">
+        <f>C31+5</f>
+        <v>38.75396309284659</v>
+      </c>
       <c r="F31" t="s">
         <v>3</v>
       </c>
@@ -1701,7 +1706,7 @@
   <dimension ref="A2:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2242,8 +2247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2494,15 +2499,15 @@
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C21" t="str">
         <f>IF(B22="Single value","Value",IF(B22="Range of values","Start",IF(B22="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
+        <v>Start</v>
       </c>
       <c r="D21" t="str">
         <f>IF(B22="Single value","",IF(B22="Range of values","Step",IF(B22="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
+        <v>Step</v>
       </c>
       <c r="E21" t="str">
         <f>IF(B22="Single value","",IF(B22="Range of values","End",IF(B22="Monte Carlo","","ERROR")))</f>
-        <v/>
+        <v>End</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -2510,13 +2515,17 @@
         <v>113</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C22" s="1">
-        <v>295</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+        <v>290</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1">
+        <v>300</v>
+      </c>
       <c r="F22" t="s">
         <v>23</v>
       </c>
@@ -2829,7 +2838,7 @@
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B6 B47 B8 B10 B50 B12 B39 B14 B54 B52 B34 B37 B41 B16:B17 B20 B23:B24</xm:sqref>
+          <xm:sqref>B6 B47 B8 B10 B50 B12 B39 B14 B54 B52 B34 B37 B41 B16:B17 B20 B23:B24 B22</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -2839,9 +2848,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Validation!#REF!</xm:f>
+            <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B19 B22</xm:sqref>
+          <xm:sqref>B19</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Launch angle fully implemented; more outputs
Now outputs X and Y accelerations, velocities, and positions. Launch angle fully editable in Excel
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525" tabRatio="551" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525" tabRatio="551"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="124">
   <si>
     <t>Total inert mass</t>
   </si>
@@ -387,6 +387,12 @@
   </si>
   <si>
     <t># of Monte Carlo runs</t>
+  </si>
+  <si>
+    <t>Rail length (effective)</t>
+  </si>
+  <si>
+    <t>Launch angle</t>
   </si>
 </sst>
 </file>
@@ -843,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,7 +978,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>121</v>
       </c>
@@ -984,6 +990,48 @@
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="1">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="1">
+        <v>32</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1015,7 +1063,7 @@
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B13 B10 B7</xm:sqref>
+          <xm:sqref>B13 B10 B7 B20 B23</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1027,7 +1075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -1509,7 +1557,7 @@
       </c>
       <c r="B14" s="2">
         <f>'Propellant Parameters (Tanks)'!N34*0.453592</f>
-        <v>12.871986458369594</v>
+        <v>11.669614475230308</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -1599,14 +1647,14 @@
       </c>
       <c r="C31" s="3">
         <f>SUM(B:B)</f>
-        <v>33.75396309284659</v>
+        <v>32.551591109707303</v>
       </c>
       <c r="D31" s="1">
         <v>2.5</v>
       </c>
       <c r="E31" s="3">
         <f>C31+5</f>
-        <v>38.75396309284659</v>
+        <v>37.551591109707303</v>
       </c>
       <c r="F31" t="s">
         <v>3</v>
@@ -1706,7 +1754,7 @@
   <dimension ref="A2:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1767,7 +1815,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="1">
-        <v>4.49</v>
+        <v>4.99</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -2248,7 +2296,7 @@
   <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2323,7 +2371,7 @@
       </c>
       <c r="C6" s="9">
         <f>$N$6*J6</f>
-        <v>2.6104650300000001E-2</v>
+        <v>2.2941940000000001E-2</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -2331,7 +2379,7 @@
         <v>60</v>
       </c>
       <c r="J6" s="1">
-        <v>1593</v>
+        <v>1400</v>
       </c>
       <c r="K6" t="s">
         <v>44</v>
@@ -2349,7 +2397,7 @@
       </c>
       <c r="C8" s="9">
         <f>$N$6*J8</f>
-        <v>7.6281950500000006E-3</v>
+        <v>6.5548400000000001E-3</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -2357,7 +2405,7 @@
         <v>60</v>
       </c>
       <c r="J8" s="1">
-        <v>465.5</v>
+        <v>400</v>
       </c>
       <c r="K8" t="s">
         <v>44</v>
@@ -2499,15 +2547,15 @@
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C21" t="str">
         <f>IF(B22="Single value","Value",IF(B22="Range of values","Start",IF(B22="Monte Carlo","Mean","ERROR")))</f>
-        <v>Start</v>
+        <v>Value</v>
       </c>
       <c r="D21" t="str">
         <f>IF(B22="Single value","",IF(B22="Range of values","Step",IF(B22="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v>Step</v>
+        <v/>
       </c>
       <c r="E21" t="str">
         <f>IF(B22="Single value","",IF(B22="Range of values","End",IF(B22="Monte Carlo","","ERROR")))</f>
-        <v>End</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -2515,17 +2563,13 @@
         <v>113</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" s="1">
         <v>290</v>
       </c>
-      <c r="D22" s="1">
-        <v>2</v>
-      </c>
-      <c r="E22" s="1">
-        <v>300</v>
-      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
       <c r="F22" t="s">
         <v>23</v>
       </c>
@@ -2616,7 +2660,7 @@
       </c>
       <c r="K31" s="8">
         <f>C34</f>
-        <v>64.103507771388223</v>
+        <v>56.337043866882304</v>
       </c>
       <c r="L31">
         <v>0.249</v>
@@ -2626,7 +2670,7 @@
       </c>
       <c r="N31" s="13">
         <f>K31*L31</f>
-        <v>15.961773435075667</v>
+        <v>14.027923922853693</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -2638,7 +2682,7 @@
       </c>
       <c r="K32" s="8">
         <f>C37</f>
-        <v>18.732067085738368</v>
+        <v>16.096298247680657</v>
       </c>
       <c r="L32">
         <v>0.27200000000000002</v>
@@ -2648,7 +2692,7 @@
       </c>
       <c r="N32" s="13">
         <f>K32*L32</f>
-        <v>5.0951222473208366</v>
+        <v>4.3781931233691394</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -2681,7 +2725,7 @@
       </c>
       <c r="C34" s="8">
         <f>C6/((PI()/4)*C12^2)/N12</f>
-        <v>64.103507771388223</v>
+        <v>56.337043866882304</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -2696,7 +2740,7 @@
       <c r="M34" s="12"/>
       <c r="N34" s="14">
         <f>SUM(N30:N33)</f>
-        <v>28.377895682396503</v>
+        <v>25.727117046222833</v>
       </c>
       <c r="O34" t="s">
         <v>50</v>
@@ -2716,7 +2760,7 @@
       </c>
       <c r="C37" s="8">
         <f>C8/((PI()/4)*C12^2)/N12</f>
-        <v>18.732067085738368</v>
+        <v>16.096298247680657</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>

</xml_diff>

<commit_message>
Fully implemented Range of Values
Range of Values mode is now fully working. It borrows a lot of code from the Monte Carlo stuff, and it outputs data in the same way
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525" tabRatio="551"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465" tabRatio="551" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="123">
   <si>
     <t>Total inert mass</t>
   </si>
@@ -210,9 +210,6 @@
   </si>
   <si>
     <t>in to m</t>
-  </si>
-  <si>
-    <t>Value</t>
   </si>
   <si>
     <t>Launch Angle</t>
@@ -851,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +860,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G1" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -927,17 +924,26 @@
         <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>63</v>
+      <c r="C9" t="str">
+        <f>IF(B10="Single value","Value",IF(B10="Range of values","Start",IF(B10="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D9" t="str">
+        <f>IF(B10="Single value","",IF(B10="Range of values","Step",IF(B10="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E9" t="str">
+        <f>IF(B10="Single value","",IF(B10="Range of values","End",IF(B10="Monte Carlo","","ERROR")))</f>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -948,17 +954,26 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>63</v>
+      <c r="C12" t="str">
+        <f>IF(B13="Single value","Value",IF(B13="Range of values","Start",IF(B13="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D12" t="str">
+        <f>IF(B13="Single value","",IF(B13="Range of values","Step",IF(B13="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E12" t="str">
+        <f>IF(B13="Single value","",IF(B13="Range of values","End",IF(B13="Monte Carlo","","ERROR")))</f>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -974,31 +989,49 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>63</v>
+      <c r="C16" t="str">
+        <f>IF(B17="Single value","Value",IF(B17="Range of values","Start",IF(B17="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D16" t="str">
+        <f>IF(B17="Single value","",IF(B17="Range of values","Step",IF(B17="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E16" t="str">
+        <f>IF(B17="Single value","",IF(B17="Range of values","End",IF(B17="Monte Carlo","","ERROR")))</f>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>63</v>
+      <c r="C19" t="str">
+        <f>IF(B20="Single value","Value",IF(B20="Range of values","Start",IF(B20="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D19" t="str">
+        <f>IF(B20="Single value","",IF(B20="Range of values","Step",IF(B20="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E19" t="str">
+        <f>IF(B20="Single value","",IF(B20="Range of values","End",IF(B20="Monte Carlo","","ERROR")))</f>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>9</v>
@@ -1013,22 +1046,35 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>63</v>
+      <c r="C22" t="str">
+        <f>IF(B23="Single value","Value",IF(B23="Range of values","Start",IF(B23="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D22" t="str">
+        <f>IF(B23="Single value","",IF(B23="Range of values","Step",IF(B23="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E22" t="str">
+        <f>IF(B23="Single value","",IF(B23="Range of values","End",IF(B23="Monte Carlo","","ERROR")))</f>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="1">
-        <v>32</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>5</v>
+      </c>
+      <c r="E23" s="1">
+        <v>30</v>
+      </c>
       <c r="F23" t="s">
         <v>19</v>
       </c>
@@ -1075,7 +1121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -1097,7 +1143,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G1" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I1" t="str">
         <f>IF(H2="Single value","Value",IF(H2="Range of values","Start",IF(H2="Monte Carlo","Mean","ERROR")))</f>
@@ -1115,7 +1161,7 @@
         <v>49</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P1" t="str">
         <f>IF(O2="Single value","Value",IF(O2="Range of values","Start",IF(O2="Monte Carlo","Mean","ERROR")))</f>
@@ -1184,7 +1230,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>9</v>
@@ -1195,7 +1241,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -1210,7 +1256,7 @@
         <v>3</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P4" t="str">
         <f>IF(O5="Single value","Value",IF(O5="Range of values","Start",IF(O5="Monte Carlo","Mean","ERROR")))</f>
@@ -1239,7 +1285,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I5" t="str">
         <f>IF(H6="Single value","Value",IF(H6="Range of values","Start",IF(H6="Monte Carlo","Mean","ERROR")))</f>
@@ -1308,7 +1354,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>9</v>
@@ -1319,10 +1365,10 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P7" t="str">
         <f>IF(O8="Single value","Value",IF(O8="Range of values","Start",IF(O8="Monte Carlo","Mean","ERROR")))</f>
@@ -1352,7 +1398,7 @@
         <v>3</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>9</v>
@@ -1378,7 +1424,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I9" t="str">
         <f>IF(H10="Single value","Value",IF(H10="Range of values","Start",IF(H10="Monte Carlo","Mean","ERROR")))</f>
@@ -1396,7 +1442,7 @@
         <v>49</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>9</v>
@@ -1437,7 +1483,7 @@
         <v>3</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>9</v>
@@ -1463,7 +1509,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>9</v>
@@ -1474,10 +1520,10 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>9</v>
@@ -1488,7 +1534,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1515,7 +1561,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I13" t="str">
         <f>IF(H14="Single value","Value",IF(H14="Range of values","Start",IF(H14="Monte Carlo","Mean","ERROR")))</f>
@@ -1533,7 +1579,7 @@
         <v>49</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P13" t="str">
         <f>IF(O14="Single value","Value",IF(O14="Range of values","Start",IF(O14="Monte Carlo","Mean","ERROR")))</f>
@@ -1553,7 +1599,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14" s="2">
         <f>'Propellant Parameters (Tanks)'!N34*0.453592</f>
@@ -1563,7 +1609,7 @@
         <v>3</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>9</v>
@@ -1574,7 +1620,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>55</v>
@@ -1593,7 +1639,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G15" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>9</v>
@@ -1607,7 +1653,7 @@
         <v>33</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>9</v>
@@ -1618,7 +1664,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1650,11 +1696,11 @@
         <v>32.551591109707303</v>
       </c>
       <c r="D31" s="1">
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="E31" s="3">
-        <f>C31+5</f>
-        <v>37.551591109707303</v>
+        <f>C31+10</f>
+        <v>42.551591109707303</v>
       </c>
       <c r="F31" t="s">
         <v>3</v>
@@ -1662,7 +1708,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C34">
         <v>6.125</v>
@@ -1727,9 +1773,11 @@
         <v>5</v>
       </c>
       <c r="D39" s="1">
-        <v>1</v>
-      </c>
-      <c r="E39" s="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E39" s="1">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1741,7 +1789,7 @@
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B31:B33 B36 B39 B25 H14:H15 O2 H6:H7 O14:O15 O5 O8:O11 H10:H11 H2 H3</xm:sqref>
+          <xm:sqref>B31:B33 B36 B39 B25 H14:H15 O2 H6:H7 O14:O15 O5 O8:O11 H10:H11 H2:H3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1836,7 +1884,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -1996,13 +2044,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C26">
         <v>1.4</v>
       </c>
       <c r="D26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2021,7 +2069,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>9</v>
@@ -2033,7 +2081,7 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2065,7 +2113,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B34">
         <v>24</v>
@@ -2073,7 +2121,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B35">
         <v>2.5000000000000001E-2</v>
@@ -2084,7 +2132,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B36">
         <f>B35 * 2.54/100</f>
@@ -2096,19 +2144,19 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B37">
         <f>(PI() / 4) *B36^2</f>
         <v>3.1669217443593616E-7</v>
       </c>
       <c r="C37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B39">
         <v>24</v>
@@ -2116,7 +2164,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B40">
         <v>5.0999999999999997E-2</v>
@@ -2127,7 +2175,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B41">
         <f>B40 * 2.54/100</f>
@@ -2139,14 +2187,14 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B42">
         <f>(PI() / 4) *B41^2</f>
         <v>1.3179461531325915E-6</v>
       </c>
       <c r="C42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2165,7 +2213,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>9</v>
@@ -2177,7 +2225,7 @@
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2196,7 +2244,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>9</v>
@@ -2208,7 +2256,7 @@
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2227,7 +2275,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>9</v>
@@ -2254,7 +2302,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>9</v>
@@ -2265,7 +2313,7 @@
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2295,8 +2343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,7 +2578,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>9</v>
@@ -2560,7 +2608,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>9</v>
@@ -2583,10 +2631,14 @@
         <f>IF(B27="Single value","",IF(B27="Range of values","Step",IF(B27="Monte Carlo","Standard deviation","ERROR")))</f>
         <v/>
       </c>
+      <c r="E26" t="str">
+        <f>IF(B27="Single value","",IF(B27="Range of values","End",IF(B27="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>9</v>
@@ -2598,7 +2650,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J28" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -2610,25 +2662,29 @@
         <f>IF(B30="Single value","",IF(B30="Range of values","Step",IF(B30="Monte Carlo","Standard deviation","ERROR")))</f>
         <v/>
       </c>
+      <c r="E29" t="str">
+        <f>IF(B30="Single value","",IF(B30="Range of values","End",IF(B30="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
       <c r="J29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L29" t="s">
         <v>55</v>
       </c>
       <c r="M29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>9</v>
@@ -2638,7 +2694,7 @@
       </c>
       <c r="D30" s="1"/>
       <c r="J30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K30">
         <v>2</v>
@@ -2647,7 +2703,7 @@
         <v>2.52</v>
       </c>
       <c r="M30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N30" s="13">
         <f>K30*L30</f>
@@ -2656,7 +2712,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K31" s="8">
         <f>C34</f>
@@ -2666,7 +2722,7 @@
         <v>0.249</v>
       </c>
       <c r="M31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N31" s="13">
         <f>K31*L31</f>
@@ -2678,7 +2734,7 @@
         <v>46</v>
       </c>
       <c r="J32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K32" s="8">
         <f>C37</f>
@@ -2688,7 +2744,7 @@
         <v>0.27200000000000002</v>
       </c>
       <c r="M32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N32" s="13">
         <f>K32*L32</f>
@@ -2699,8 +2755,20 @@
       <c r="A33" t="s">
         <v>53</v>
       </c>
+      <c r="C33" t="str">
+        <f>IF(B34="Single value","Value",IF(B34="Range of values","Start",IF(B34="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D33" t="str">
+        <f>IF(B34="Single value","",IF(B34="Range of values","Step",IF(B34="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E33" t="str">
+        <f>IF(B34="Single value","",IF(B34="Range of values","End",IF(B34="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
       <c r="J33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K33">
         <v>1</v>
@@ -2709,7 +2777,7 @@
         <v>2.2810000000000001</v>
       </c>
       <c r="M33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N33">
         <f>K33*L33</f>
@@ -2733,7 +2801,7 @@
         <v>5</v>
       </c>
       <c r="J34" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
@@ -2750,6 +2818,18 @@
       <c r="A36" t="s">
         <v>54</v>
       </c>
+      <c r="C36" t="str">
+        <f>IF(B37="Single value","Value",IF(B37="Range of values","Start",IF(B37="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D36" t="str">
+        <f>IF(B37="Single value","",IF(B37="Range of values","Step",IF(B37="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E36" t="str">
+        <f>IF(B37="Single value","",IF(B37="Range of values","End",IF(B37="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -2768,7 +2848,21 @@
         <v>33</v>
       </c>
       <c r="J37" t="s">
-        <v>120</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C38" t="str">
+        <f>IF(B39="Single value","Value",IF(B39="Range of values","Start",IF(B39="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D38" t="str">
+        <f>IF(B39="Single value","",IF(B39="Range of values","Step",IF(B39="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E38" t="str">
+        <f>IF(B39="Single value","",IF(B39="Range of values","End",IF(B39="Monte Carlo","","ERROR")))</f>
+        <v/>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
@@ -2779,12 +2873,32 @@
         <v>9</v>
       </c>
       <c r="C39" s="7">
-        <v>41.668101</v>
-      </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="1"/>
+        <f>41.668101-2</f>
+        <v>39.668101</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E39" s="7">
+        <f>41.668101+2</f>
+        <v>43.668101</v>
+      </c>
       <c r="F39" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C40" t="str">
+        <f>IF(B41="Single value","Value",IF(B41="Range of values","Start",IF(B41="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D40" t="str">
+        <f>IF(B41="Single value","",IF(B41="Range of values","Step",IF(B41="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E40" t="str">
+        <f>IF(B41="Single value","",IF(B41="Range of values","End",IF(B41="Monte Carlo","","ERROR")))</f>
+        <v/>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
@@ -2882,7 +2996,7 @@
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B6 B47 B8 B10 B50 B12 B39 B14 B54 B52 B34 B37 B41 B16:B17 B20 B23:B24 B22</xm:sqref>
+          <xm:sqref>B6 B47 B8 B10 B50 B12 B39 B14 B54 B52 B34 B37 B41 B16:B17 B20 B22:B24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Changed Simulink to fixed time step
Apparently having a variable time step doesn't produce reliable results for some reason. I changed it to a fixed time step, but the time step is pretty big right now. Once we figure out more about what's going on we can change it back. I also added some time things to the monte carlo and range of values loops. Also supressed warnings.
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465" tabRatio="551" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465" tabRatio="551" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="120">
   <si>
     <t>Total inert mass</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Largest circular diameter</t>
   </si>
   <si>
-    <t>Thrust-to-weight ratio</t>
-  </si>
-  <si>
     <t>Parameter options</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>Propellant options</t>
   </si>
   <si>
-    <t>Mixture ratio</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
@@ -210,9 +204,6 @@
   </si>
   <si>
     <t>in to m</t>
-  </si>
-  <si>
-    <t>Launch Angle</t>
   </si>
   <si>
     <t>Degrees</t>
@@ -846,7 +837,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
@@ -860,7 +851,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G1" s="10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -879,10 +870,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
         <v>295</v>
@@ -890,7 +881,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -909,10 +900,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="11">
         <f>101325*(1-(0.0000225577)*C13)^5.25588</f>
@@ -921,10 +912,10 @@
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -943,10 +934,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>63</v>
+        <v>119</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
@@ -954,7 +945,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -973,10 +964,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="1">
         <f>4595/3.28</f>
@@ -985,7 +976,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1004,13 +995,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1031,10 +1022,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="1">
         <v>5</v>
@@ -1042,41 +1033,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C22" t="str">
-        <f>IF(B23="Single value","Value",IF(B23="Range of values","Start",IF(B23="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D22" t="str">
-        <f>IF(B23="Single value","",IF(B23="Range of values","Step",IF(B23="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E22" t="str">
-        <f>IF(B23="Single value","",IF(B23="Range of values","End",IF(B23="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1">
-        <v>5</v>
-      </c>
-      <c r="E23" s="1">
-        <v>30</v>
-      </c>
-      <c r="F23" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1092,24 +1049,18 @@
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B4</xm:sqref>
+          <xm:sqref>B4 B13 B10 B7 B20</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Validation!$A$2</xm:f>
           </x14:formula1>
           <xm:sqref>B17</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Validation!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>B13 B10 B7 B20 B23</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1119,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,7 +1094,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G1" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I1" t="str">
         <f>IF(H2="Single value","Value",IF(H2="Range of values","Start",IF(H2="Monte Carlo","Mean","ERROR")))</f>
@@ -1158,10 +1109,10 @@
         <v/>
       </c>
       <c r="L1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="P1" t="str">
         <f>IF(O2="Single value","Value",IF(O2="Range of values","Start",IF(O2="Monte Carlo","Mean","ERROR")))</f>
@@ -1176,24 +1127,24 @@
         <v/>
       </c>
       <c r="S1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I2" s="15">
         <v>1</v>
@@ -1204,10 +1155,10 @@
         <v>3</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P2" s="15">
         <v>1</v>
@@ -1220,7 +1171,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2">
         <f>I6*I7</f>
@@ -1230,10 +1181,10 @@
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I3" s="15">
         <v>4</v>
@@ -1241,12 +1192,12 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" s="2">
         <f>I14*I15</f>
@@ -1256,7 +1207,7 @@
         <v>3</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="P4" t="str">
         <f>IF(O5="Single value","Value",IF(O5="Range of values","Start",IF(O5="Monte Carlo","Mean","ERROR")))</f>
@@ -1271,12 +1222,12 @@
         <v/>
       </c>
       <c r="S4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2">
         <v>0.5</v>
@@ -1285,7 +1236,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I5" t="str">
         <f>IF(H6="Single value","Value",IF(H6="Range of values","Start",IF(H6="Monte Carlo","Mean","ERROR")))</f>
@@ -1300,13 +1251,13 @@
         <v/>
       </c>
       <c r="L5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P5" s="15">
         <v>1</v>
@@ -1319,7 +1270,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
@@ -1328,10 +1279,10 @@
         <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I6" s="15">
         <v>1</v>
@@ -1344,7 +1295,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2">
         <f>I10*I11</f>
@@ -1354,10 +1305,10 @@
         <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I7" s="15">
         <v>1</v>
@@ -1365,10 +1316,10 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="P7" t="str">
         <f>IF(O8="Single value","Value",IF(O8="Range of values","Start",IF(O8="Monte Carlo","Mean","ERROR")))</f>
@@ -1383,12 +1334,12 @@
         <v/>
       </c>
       <c r="S7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2">
         <f>P2</f>
@@ -1398,10 +1349,10 @@
         <v>3</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P8" s="15">
         <f>5.909/12/3.28</f>
@@ -1410,12 +1361,12 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="2">
         <v>4</v>
@@ -1424,7 +1375,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I9" t="str">
         <f>IF(H10="Single value","Value",IF(H10="Range of values","Start",IF(H10="Monte Carlo","Mean","ERROR")))</f>
@@ -1439,13 +1390,13 @@
         <v/>
       </c>
       <c r="L9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P9" s="15">
         <f>5.625/12/3.28</f>
@@ -1454,12 +1405,12 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" s="2">
         <f>11.151/2.205</f>
@@ -1469,10 +1420,10 @@
         <v>3</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I10" s="15">
         <v>1</v>
@@ -1483,10 +1434,10 @@
         <v>3</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P10" s="15">
         <v>3</v>
@@ -1494,7 +1445,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1509,10 +1460,10 @@
         <v>3</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I11" s="15">
         <v>1</v>
@@ -1520,13 +1471,13 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P11" s="15">
         <v>2700</v>
@@ -1534,7 +1485,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1561,7 +1512,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I13" t="str">
         <f>IF(H14="Single value","Value",IF(H14="Range of values","Start",IF(H14="Monte Carlo","Mean","ERROR")))</f>
@@ -1576,10 +1527,10 @@
         <v/>
       </c>
       <c r="L13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="P13" t="str">
         <f>IF(O14="Single value","Value",IF(O14="Range of values","Start",IF(O14="Monte Carlo","Mean","ERROR")))</f>
@@ -1594,12 +1545,12 @@
         <v/>
       </c>
       <c r="S13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B14" s="2">
         <f>'Propellant Parameters (Tanks)'!N34*0.453592</f>
@@ -1609,10 +1560,10 @@
         <v>3</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I14" s="15">
         <v>1</v>
@@ -1620,13 +1571,13 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P14" s="15">
         <v>1</v>
@@ -1639,10 +1590,10 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G15" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I15" s="15">
         <v>1</v>
@@ -1650,13 +1601,13 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P15" s="15">
         <v>1</v>
@@ -1664,24 +1615,24 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C30" t="str">
         <f>IF(B31="Single value","Value",IF(B31="Range of values","Start",IF(B31="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
+        <v>Start</v>
       </c>
       <c r="D30" t="str">
         <f>IF(B31="Single value","",IF(B31="Range of values","Step",IF(B31="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
+        <v>Step</v>
       </c>
       <c r="E30" t="str">
         <f>IF(B31="Single value","",IF(B31="Range of values","End",IF(B31="Monte Carlo","","ERROR")))</f>
-        <v/>
+        <v>End</v>
       </c>
       <c r="F30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1696,11 +1647,12 @@
         <v>32.551591109707303</v>
       </c>
       <c r="D31" s="1">
-        <v>0.5</v>
+        <f>1/8</f>
+        <v>0.125</v>
       </c>
       <c r="E31" s="3">
-        <f>C31+10</f>
-        <v>42.551591109707303</v>
+        <f>C31+5</f>
+        <v>37.551591109707303</v>
       </c>
       <c r="F31" t="s">
         <v>3</v>
@@ -1708,7 +1660,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C34">
         <v>6.125</v>
@@ -1736,7 +1688,7 @@
         <v>6</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C36" s="1">
         <f>C34*2.54/100</f>
@@ -1745,38 +1697,7 @@
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C38" t="str">
-        <f>IF(B39="Single value","Value",IF(B39="Range of values","Start",IF(B39="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D38" t="str">
-        <f>IF(B39="Single value","",IF(B39="Range of values","Step",IF(B39="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E38" t="str">
-        <f>IF(B39="Single value","",IF(B39="Range of values","End",IF(B39="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="1">
-        <v>5</v>
-      </c>
-      <c r="D39" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="E39" s="1">
-        <v>10</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1789,7 +1710,7 @@
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B31:B33 B36 B39 B25 H14:H15 O2 H6:H7 O14:O15 O5 O8:O11 H10:H11 H2:H3</xm:sqref>
+          <xm:sqref>B31:B33 B36 H2:H3 B25 H14:H15 O2 H6:H7 O14:O15 O5 O8:O11 H10:H11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1801,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1827,10 +1748,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
         <v>300</v>
@@ -1838,7 +1759,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1857,10 +1778,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
         <v>4.99</v>
@@ -1871,20 +1792,20 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" t="str">
         <f>IF(B9="Single value","Value",IF(B9="Range of values","Start",IF(B9="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
+        <v>Start</v>
       </c>
       <c r="D8" t="str">
         <f>IF(B9="Single value","",IF(B9="Range of values","Step",IF(B9="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
+        <v>Step</v>
       </c>
       <c r="E8" t="str">
         <f>IF(B9="Single value","",IF(B9="Range of values","End",IF(B9="Monte Carlo","","ERROR")))</f>
-        <v/>
+        <v>End</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -1892,8 +1813,13 @@
       <c r="C9" s="1">
         <v>0.9</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="D9" s="1">
+        <f>0.0025/2</f>
+        <v>1.25E-3</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" t="str">
@@ -1911,10 +1837,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
@@ -1941,10 +1867,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1">
         <v>300</v>
@@ -1968,10 +1894,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18" s="1">
         <v>45</v>
@@ -1998,10 +1924,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" s="1">
         <v>45</v>
@@ -2009,7 +1935,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2028,10 +1954,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C24" s="1">
         <v>15</v>
@@ -2039,18 +1965,18 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C26">
         <v>1.4</v>
       </c>
       <c r="D26" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2069,10 +1995,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C28" s="1">
         <f>C26*2.54^2/100^2</f>
@@ -2081,39 +2007,12 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C30" t="str">
-        <f>IF(B31="Single value","Value",IF(B31="Range of values","Start",IF(B31="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D30" t="str">
-        <f>IF(B31="Single value","",IF(B31="Range of values","Step",IF(B31="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E30" t="str">
-        <f>IF(B31="Single value","",IF(B31="Range of values","End",IF(B31="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="1">
-        <v>8</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+        <v>96</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B34">
         <v>24</v>
@@ -2121,7 +2020,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B35">
         <v>2.5000000000000001E-2</v>
@@ -2132,31 +2031,31 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B36">
         <f>B35 * 2.54/100</f>
         <v>6.3500000000000004E-4</v>
       </c>
       <c r="C36" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B37">
         <f>(PI() / 4) *B36^2</f>
         <v>3.1669217443593616E-7</v>
       </c>
       <c r="C37" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B39">
         <v>24</v>
@@ -2164,7 +2063,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B40">
         <v>5.0999999999999997E-2</v>
@@ -2175,26 +2074,26 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B41">
         <f>B40 * 2.54/100</f>
         <v>1.2953999999999999E-3</v>
       </c>
       <c r="C41" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B42">
         <f>(PI() / 4) *B41^2</f>
         <v>1.3179461531325915E-6</v>
       </c>
       <c r="C42" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2213,10 +2112,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C45" s="9">
         <f>B34*B37</f>
@@ -2225,7 +2124,7 @@
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2244,10 +2143,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C48" s="9">
         <f>B42*B39</f>
@@ -2256,7 +2155,7 @@
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2275,10 +2174,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C51" s="1">
         <v>0.8</v>
@@ -2302,10 +2201,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C54" s="1">
         <v>1</v>
@@ -2313,7 +2212,7 @@
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2325,7 +2224,7 @@
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B3 B6 B9 B12 B15 B18 B21 B24 B31 B28</xm:sqref>
+          <xm:sqref>B3 B6 B9 B12 B15 B18 B21 B24 B28</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -2357,34 +2256,34 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
         <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -2401,21 +2300,21 @@
         <v/>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="9">
         <f>$N$6*J6</f>
@@ -2424,13 +2323,13 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J6" s="1">
         <v>1400</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N6" s="6">
         <v>1.6387100000000001E-5</v>
@@ -2438,10 +2337,10 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="9">
         <f>$N$6*J8</f>
@@ -2450,21 +2349,21 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J8" s="1">
         <v>400</v>
       </c>
       <c r="K8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="9">
         <f>$N$6*J10</f>
@@ -2473,27 +2372,27 @@
       <c r="D10" s="4"/>
       <c r="E10" s="1"/>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J10" s="4">
         <f>93.19</f>
         <v>93.19</v>
       </c>
       <c r="K10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="9">
         <f>$N$12*J12</f>
@@ -2502,7 +2401,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J12" s="4">
         <v>5.625</v>
@@ -2516,10 +2415,10 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="9">
         <f>$N$12*J14</f>
@@ -2528,7 +2427,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G14" s="6"/>
       <c r="J14" s="1">
@@ -2540,10 +2439,10 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="9">
         <f>$N$12*J16</f>
@@ -2552,7 +2451,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G16" s="6"/>
       <c r="J16" s="1">
@@ -2578,10 +2477,10 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" s="1">
         <v>295</v>
@@ -2589,7 +2488,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -2608,10 +2507,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" s="1">
         <v>290</v>
@@ -2619,7 +2518,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -2638,10 +2537,10 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" s="1">
         <v>3</v>
@@ -2650,7 +2549,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J28" s="12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -2667,34 +2566,34 @@
         <v/>
       </c>
       <c r="J29" t="s">
+        <v>65</v>
+      </c>
+      <c r="K29" t="s">
         <v>68</v>
       </c>
-      <c r="K29" t="s">
-        <v>71</v>
-      </c>
       <c r="L29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M29" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N29" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C30" s="1">
         <v>2</v>
       </c>
       <c r="D30" s="1"/>
       <c r="J30" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K30">
         <v>2</v>
@@ -2703,7 +2602,7 @@
         <v>2.52</v>
       </c>
       <c r="M30" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N30" s="13">
         <f>K30*L30</f>
@@ -2712,7 +2611,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K31" s="8">
         <f>C34</f>
@@ -2722,7 +2621,7 @@
         <v>0.249</v>
       </c>
       <c r="M31" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N31" s="13">
         <f>K31*L31</f>
@@ -2731,10 +2630,10 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J32" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="K32" s="8">
         <f>C37</f>
@@ -2744,7 +2643,7 @@
         <v>0.27200000000000002</v>
       </c>
       <c r="M32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N32" s="13">
         <f>K32*L32</f>
@@ -2753,7 +2652,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C33" t="str">
         <f>IF(B34="Single value","Value",IF(B34="Range of values","Start",IF(B34="Monte Carlo","Mean","ERROR")))</f>
@@ -2768,7 +2667,7 @@
         <v/>
       </c>
       <c r="J33" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K33">
         <v>1</v>
@@ -2777,7 +2676,7 @@
         <v>2.2810000000000001</v>
       </c>
       <c r="M33" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N33">
         <f>K33*L33</f>
@@ -2786,10 +2685,10 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C34" s="8">
         <f>C6/((PI()/4)*C12^2)/N12</f>
@@ -2801,7 +2700,7 @@
         <v>5</v>
       </c>
       <c r="J34" s="12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
@@ -2811,12 +2710,12 @@
         <v>25.727117046222833</v>
       </c>
       <c r="O34" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C36" t="str">
         <f>IF(B37="Single value","Value",IF(B37="Range of values","Start",IF(B37="Monte Carlo","Mean","ERROR")))</f>
@@ -2833,10 +2732,10 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C37" s="8">
         <f>C8/((PI()/4)*C12^2)/N12</f>
@@ -2845,10 +2744,10 @@
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J37" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -2867,10 +2766,10 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C39" s="7">
         <f>41.668101-2</f>
@@ -2884,7 +2783,7 @@
         <v>43.668101</v>
       </c>
       <c r="F39" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
@@ -2903,10 +2802,10 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C41" s="7">
         <v>5.0911735</v>
@@ -2914,7 +2813,7 @@
       <c r="D41" s="4"/>
       <c r="E41" s="1"/>
       <c r="F41" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
@@ -3028,22 +2927,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the default Excel parameters
I changed the default excel parameters so that the default behavoir isn't to run ~1600 sims that take 8 hours total to complete.
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465" tabRatio="551" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465" tabRatio="551" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
@@ -1072,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1621,15 +1621,15 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C30" t="str">
         <f>IF(B31="Single value","Value",IF(B31="Range of values","Start",IF(B31="Monte Carlo","Mean","ERROR")))</f>
-        <v>Start</v>
+        <v>Value</v>
       </c>
       <c r="D30" t="str">
         <f>IF(B31="Single value","",IF(B31="Range of values","Step",IF(B31="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v>Step</v>
+        <v/>
       </c>
       <c r="E30" t="str">
         <f>IF(B31="Single value","",IF(B31="Range of values","End",IF(B31="Monte Carlo","","ERROR")))</f>
-        <v>End</v>
+        <v/>
       </c>
       <c r="F30" t="s">
         <v>47</v>
@@ -1640,7 +1640,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C31" s="3">
         <f>SUM(B:B)</f>
@@ -1722,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1792,15 +1792,15 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" t="str">
         <f>IF(B9="Single value","Value",IF(B9="Range of values","Start",IF(B9="Monte Carlo","Mean","ERROR")))</f>
-        <v>Start</v>
+        <v>Value</v>
       </c>
       <c r="D8" t="str">
         <f>IF(B9="Single value","",IF(B9="Range of values","Step",IF(B9="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v>Step</v>
+        <v/>
       </c>
       <c r="E8" t="str">
         <f>IF(B9="Single value","",IF(B9="Range of values","End",IF(B9="Monte Carlo","","ERROR")))</f>
-        <v>End</v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1808,7 +1808,7 @@
         <v>114</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1">
         <v>0.9</v>

</xml_diff>

<commit_message>
Added basic trajectory prediction to simulink model
It's super basic right now, I still need to come up with a better way to estimate the cd, and add in some inputs for the mass and area so they don't have to be hardcoded.
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465" tabRatio="551" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465" tabRatio="551"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,15 +857,15 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3" t="str">
         <f>IF(B4="Single value","Value",IF(B4="Range of values","Start",IF(B4="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
+        <v>Start</v>
       </c>
       <c r="D3" t="str">
         <f>IF(B4="Single value","",IF(B4="Range of values","Step",IF(B4="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
+        <v>Step</v>
       </c>
       <c r="E3" t="str">
         <f>IF(B4="Single value","",IF(B4="Range of values","End",IF(B4="Monte Carlo","","ERROR")))</f>
-        <v/>
+        <v>End</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -873,13 +873,17 @@
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1">
         <v>295</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>296</v>
+      </c>
       <c r="F4" t="s">
         <v>22</v>
       </c>
@@ -1072,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A27" sqref="A26:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,7 +1726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2242,7 +2246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Improvements to accelerometer modelling
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="124">
   <si>
     <t>Total inert mass</t>
   </si>
@@ -381,6 +381,31 @@
   </si>
   <si>
     <t>Launch angle</t>
+  </si>
+  <si>
+    <t>Sensor Modelling</t>
+  </si>
+  <si>
+    <t>Accelerometer stddev</t>
+  </si>
+  <si>
+    <r>
+      <t>m/s</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Average of X, Y, and Z values from a stationary tabletop test</t>
   </si>
 </sst>
 </file>
@@ -391,7 +416,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,6 +443,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -472,7 +505,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -493,6 +526,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -837,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,15 +893,15 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3" t="str">
         <f>IF(B4="Single value","Value",IF(B4="Range of values","Start",IF(B4="Monte Carlo","Mean","ERROR")))</f>
-        <v>Start</v>
+        <v>Value</v>
       </c>
       <c r="D3" t="str">
         <f>IF(B4="Single value","",IF(B4="Range of values","Step",IF(B4="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v>Step</v>
+        <v/>
       </c>
       <c r="E3" t="str">
         <f>IF(B4="Single value","",IF(B4="Range of values","End",IF(B4="Monte Carlo","","ERROR")))</f>
-        <v>End</v>
+        <v/>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -873,17 +909,13 @@
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
         <v>295</v>
       </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>296</v>
-      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="F4" t="s">
         <v>22</v>
       </c>
@@ -997,7 +1029,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>117</v>
       </c>
@@ -1005,12 +1037,12 @@
         <v>8</v>
       </c>
       <c r="C17" s="1">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C19" t="str">
         <f>IF(B20="Single value","Value",IF(B20="Range of values","Start",IF(B20="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
@@ -1024,7 +1056,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>118</v>
       </c>
@@ -1040,7 +1072,59 @@
         <v>31</v>
       </c>
     </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C25" t="str">
+        <f>IF(B26="Single value","Value",IF(B26="Range of values","Start",IF(B26="Monte Carlo","Mean","ERROR")))</f>
+        <v>Mean</v>
+      </c>
+      <c r="D25" t="str">
+        <f>IF(B26="Single value","",IF(B26="Range of values","Step",IF(B26="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v>Standard deviation</v>
+      </c>
+      <c r="E25" t="str">
+        <f>IF(B26="Single value","",IF(B26="Range of values","End",IF(B26="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" t="s">
+        <v>122</v>
+      </c>
+      <c r="G26" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="1">
+        <v>3.353376168248183E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A24:E24"/>
+  </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17">
       <formula1>1</formula1>
@@ -1058,7 +1142,7 @@
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B4 B13 B10 B7 B20</xm:sqref>
+          <xm:sqref>B4 B13 B10 B7 B20 B26</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -1076,7 +1160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A27" sqref="A26:A27"/>
     </sheetView>
   </sheetViews>
@@ -1726,7 +1810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2246,7 +2330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed sensor noise seeding issue
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -873,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,7 +1037,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1102,8 +1102,8 @@
       <c r="B26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C26">
-        <v>5</v>
+      <c r="C26" s="1">
+        <v>3.353376168248183E-2</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
@@ -1114,11 +1114,6 @@
       </c>
       <c r="G26" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G27" s="1">
-        <v>3.353376168248183E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed default acceleration offset
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -876,7 +876,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,7 +1037,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1084,11 +1084,11 @@
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C25" t="str">
         <f>IF(B26="Single value","Value",IF(B26="Range of values","Start",IF(B26="Monte Carlo","Mean","ERROR")))</f>
-        <v>Mean</v>
+        <v>Value</v>
       </c>
       <c r="D25" t="str">
         <f>IF(B26="Single value","",IF(B26="Range of values","Step",IF(B26="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v>Standard deviation</v>
+        <v/>
       </c>
       <c r="E25" t="str">
         <f>IF(B26="Single value","",IF(B26="Range of values","End",IF(B26="Monte Carlo","","ERROR")))</f>
@@ -1100,7 +1100,7 @@
         <v>121</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C26" s="1">
         <v>3.353376168248183E-2</v>

</xml_diff>

<commit_message>
Fixed accelerometer sensor model bug
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="126">
   <si>
     <t>Total inert mass</t>
   </si>
@@ -406,6 +406,12 @@
   </si>
   <si>
     <t>Average of X, Y, and Z values from a stationary tabletop test</t>
+  </si>
+  <si>
+    <t>Total pressure sensor stddev</t>
+  </si>
+  <si>
+    <t>Currently completely made up</t>
   </si>
 </sst>
 </file>
@@ -873,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,7 +1043,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1084,11 +1090,11 @@
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C25" t="str">
         <f>IF(B26="Single value","Value",IF(B26="Range of values","Start",IF(B26="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
+        <v>Mean</v>
       </c>
       <c r="D25" t="str">
         <f>IF(B26="Single value","",IF(B26="Range of values","Step",IF(B26="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
+        <v>Standard deviation</v>
       </c>
       <c r="E25" t="str">
         <f>IF(B26="Single value","",IF(B26="Range of values","End",IF(B26="Monte Carlo","","ERROR")))</f>
@@ -1100,7 +1106,7 @@
         <v>121</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C26" s="1">
         <v>3.353376168248183E-2</v>
@@ -1114,6 +1120,39 @@
       </c>
       <c r="G26" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C28" t="str">
+        <f>IF(B29="Single value","Value",IF(B29="Range of values","Start",IF(B29="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D28" t="str">
+        <f>IF(B29="Single value","",IF(B29="Range of values","Step",IF(B29="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E28" t="str">
+        <f>IF(B29="Single value","",IF(B29="Range of values","End",IF(B29="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1">
+        <v>10</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1137,7 +1176,7 @@
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B4 B13 B10 B7 B20 B26</xm:sqref>
+          <xm:sqref>B4 B13 B10 B7 B20 B26 B29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Added ullage volume configuration
Actual ullage thermo not yet implemented
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465" tabRatio="551"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465" tabRatio="551" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="132">
   <si>
     <t>Total inert mass</t>
   </si>
@@ -412,6 +412,24 @@
   </si>
   <si>
     <t>Currently completely made up</t>
+  </si>
+  <si>
+    <t>Tank Volumes</t>
+  </si>
+  <si>
+    <t>Oxidizer tank volume</t>
+  </si>
+  <si>
+    <t>Fuel tank volume</t>
+  </si>
+  <si>
+    <t>Oxidizer ullage volume</t>
+  </si>
+  <si>
+    <t>Fuel ullage volume</t>
+  </si>
+  <si>
+    <t>N2 Ullage, set to 0% for none</t>
   </si>
 </sst>
 </file>
@@ -488,7 +506,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -505,13 +523,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -535,11 +594,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -881,7 +955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -1675,7 +1749,7 @@
         <v>63</v>
       </c>
       <c r="B14" s="2">
-        <f>'Propellant Parameters (Tanks)'!N34*0.453592</f>
+        <f>'Propellant Parameters (Tanks)'!N26*0.453592</f>
         <v>11.669614475230308</v>
       </c>
       <c r="C14" t="s">
@@ -2362,10 +2436,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2409,373 +2483,477 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C5" t="str">
-        <f>IF(B6="Single value","Value",IF(B6="Range of values","Start",IF(B6="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D5" t="str">
-        <f>IF(B6="Single value","",IF(B6="Range of values","Step",IF(B6="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E5" t="str">
-        <f>IF(B6="Single value","",IF(B6="Range of values","End",IF(B6="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="F5" t="s">
+      <c r="A5" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22" t="str">
+        <f>IF(B7="Single value","Value",IF(B7="Range of values","Start",IF(B7="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D6" s="22" t="str">
+        <f>IF(B7="Single value","",IF(B7="Range of values","Step",IF(B7="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E6" s="22" t="str">
+        <f>IF(B7="Single value","",IF(B7="Range of values","End",IF(B7="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K6" t="s">
         <v>47</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="9">
-        <f>$N$6*J6</f>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="26">
+        <f>$N$7*J7</f>
         <v>2.2941940000000001E-2</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" t="s">
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J7" s="1">
         <v>1400</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K7" t="s">
         <v>42</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N7" s="6">
         <v>1.6387100000000001E-5</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="9">
-        <f>$N$6*J8</f>
+      <c r="A8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="26">
+        <f>$N$7*J9</f>
         <v>6.5548400000000001E-3</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" t="s">
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J9" s="1">
         <v>400</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="9">
-        <f>$N$6*J10</f>
-        <v>1.5271138490000002E-3</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="1"/>
-      <c r="F10" t="s">
-        <v>58</v>
-      </c>
-      <c r="J10" s="4">
+      <c r="A10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="23"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22" t="str">
+        <f>IF(B12="Single value","Value",IF(B12="Range of values","Start",IF(B12="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D11" s="22" t="str">
+        <f>IF(B12="Single value","",IF(B12="Range of values","Step",IF(B12="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E11" s="22" t="str">
+        <f>IF(B12="Single value","",IF(B12="Range of values","End",IF(B12="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="F11" s="23"/>
+      <c r="J11" s="4">
         <f>93.19</f>
         <v>93.19</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N11" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="27">
+        <v>0.15</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" t="s">
+        <v>131</v>
+      </c>
+      <c r="N12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="9">
-        <f>$N$12*J12</f>
-        <v>0.142875</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" t="s">
-        <v>31</v>
-      </c>
-      <c r="J12" s="4">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="23"/>
+      <c r="J13" s="4">
         <v>5.625</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K13" t="s">
         <v>5</v>
       </c>
-      <c r="N12">
+      <c r="N13">
         <v>2.5399999999999999E-2</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="9">
-        <f>$N$12*J14</f>
-        <v>0.15008859999999999</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="6"/>
-      <c r="J14" s="1">
+      <c r="A14" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="27">
+        <v>0.15</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="23"/>
+      <c r="J15" s="1">
         <v>5.9089999999999998</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="9">
-        <f>$N$12*J16</f>
-        <v>7.2135999999999988E-3</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G16" s="6"/>
-      <c r="J16" s="1">
+      <c r="A16" s="21"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22" t="str">
+        <f>IF(B17="Single value","Value",IF(B17="Range of values","Start",IF(B17="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D16" s="22" t="str">
+        <f>IF(B17="Single value","",IF(B17="Range of values","Step",IF(B17="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E16" s="22" t="str">
+        <f>IF(B17="Single value","",IF(B17="Range of values","End",IF(B17="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="F16" s="23"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="26">
+        <f>C7*(1-C12)</f>
+        <v>1.9500649000000002E-2</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="J17" s="1">
         <v>0.28399999999999997</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C18" t="str">
-        <f>IF(B19="Single value","Value",IF(B19="Range of values","Start",IF(B19="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D18" t="str">
-        <f>IF(B19="Single value","",IF(B19="Range of values","Step",IF(B19="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E18" t="str">
-        <f>IF(B19="Single value","",IF(B19="Range of values","End",IF(B19="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="1">
-        <v>295</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C21" t="str">
-        <f>IF(B22="Single value","Value",IF(B22="Range of values","Start",IF(B22="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D21" t="str">
-        <f>IF(B22="Single value","",IF(B22="Range of values","Step",IF(B22="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E21" t="str">
-        <f>IF(B22="Single value","",IF(B22="Range of values","End",IF(B22="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="23"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="30">
+        <f>C9*(1-C14)</f>
+        <v>5.5716139999999999E-3</v>
+      </c>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J20" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>65</v>
+      </c>
+      <c r="K21" t="s">
+        <v>68</v>
+      </c>
+      <c r="L21" t="s">
+        <v>53</v>
+      </c>
+      <c r="M21" t="s">
+        <v>66</v>
+      </c>
+      <c r="N21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>109</v>
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="1">
-        <v>290</v>
-      </c>
-      <c r="D22" s="1"/>
+      <c r="C22" s="9">
+        <f>$N$7*J11</f>
+        <v>1.5271138490000002E-3</v>
+      </c>
+      <c r="D22" s="4"/>
       <c r="E22" s="1"/>
       <c r="F22" t="s">
+        <v>58</v>
+      </c>
+      <c r="J22" t="s">
+        <v>67</v>
+      </c>
+      <c r="K22">
+        <v>2</v>
+      </c>
+      <c r="L22">
+        <v>2.52</v>
+      </c>
+      <c r="M22" t="s">
+        <v>69</v>
+      </c>
+      <c r="N22" s="13">
+        <f>K22*L22</f>
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G23" s="6"/>
+      <c r="J23" t="s">
+        <v>71</v>
+      </c>
+      <c r="K23" s="8">
+        <f>C46</f>
+        <v>56.337043866882304</v>
+      </c>
+      <c r="L23">
+        <v>0.249</v>
+      </c>
+      <c r="M23" t="s">
+        <v>73</v>
+      </c>
+      <c r="N23" s="13">
+        <f>K23*L23</f>
+        <v>14.027923922853693</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="9">
+        <f>$N$13*J13</f>
+        <v>0.142875</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" t="s">
+        <v>31</v>
+      </c>
+      <c r="J24" t="s">
+        <v>72</v>
+      </c>
+      <c r="K24" s="8">
+        <f>C49</f>
+        <v>16.096298247680657</v>
+      </c>
+      <c r="L24">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="M24" t="s">
+        <v>73</v>
+      </c>
+      <c r="N24" s="13">
+        <f>K24*L24</f>
+        <v>4.3781931233691394</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G25" s="6"/>
+      <c r="J25" t="s">
+        <v>74</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>2.2810000000000001</v>
+      </c>
+      <c r="M25" t="s">
+        <v>69</v>
+      </c>
+      <c r="N25">
+        <f>K25*L25</f>
+        <v>2.2810000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="9">
+        <f>$N$13*J15</f>
+        <v>0.15008859999999999</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" t="s">
+        <v>31</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="14">
+        <f>SUM(N22:N25)</f>
+        <v>25.727117046222833</v>
+      </c>
+      <c r="O26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="9">
+        <f>$N$13*J17</f>
+        <v>7.2135999999999988E-3</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C30" t="str">
+        <f>IF(B31="Single value","Value",IF(B31="Range of values","Start",IF(B31="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D30" t="str">
+        <f>IF(B31="Single value","",IF(B31="Range of values","Step",IF(B31="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E30" t="str">
+        <f>IF(B31="Single value","",IF(B31="Range of values","End",IF(B31="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="1">
+        <v>295</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C26" t="str">
-        <f>IF(B27="Single value","Value",IF(B27="Range of values","Start",IF(B27="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D26" t="str">
-        <f>IF(B27="Single value","",IF(B27="Range of values","Step",IF(B27="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E26" t="str">
-        <f>IF(B27="Single value","",IF(B27="Range of values","End",IF(B27="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="1">
-        <v>3</v>
-      </c>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J28" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C29" t="str">
-        <f>IF(B30="Single value","Value",IF(B30="Range of values","Start",IF(B30="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D29" t="str">
-        <f>IF(B30="Single value","",IF(B30="Range of values","Step",IF(B30="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E29" t="str">
-        <f>IF(B30="Single value","",IF(B30="Range of values","End",IF(B30="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="J29" t="s">
-        <v>65</v>
-      </c>
-      <c r="K29" t="s">
-        <v>68</v>
-      </c>
-      <c r="L29" t="s">
-        <v>53</v>
-      </c>
-      <c r="M29" t="s">
-        <v>66</v>
-      </c>
-      <c r="N29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="1">
-        <v>2</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="J30" t="s">
-        <v>67</v>
-      </c>
-      <c r="K30">
-        <v>2</v>
-      </c>
-      <c r="L30">
-        <v>2.52</v>
-      </c>
-      <c r="M30" t="s">
-        <v>69</v>
-      </c>
-      <c r="N30" s="13">
-        <f>K30*L30</f>
-        <v>5.04</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J31" t="s">
-        <v>71</v>
-      </c>
-      <c r="K31" s="8">
-        <f>C34</f>
-        <v>56.337043866882304</v>
-      </c>
-      <c r="L31">
-        <v>0.249</v>
-      </c>
-      <c r="M31" t="s">
-        <v>73</v>
-      </c>
-      <c r="N31" s="13">
-        <f>K31*L31</f>
-        <v>14.027923922853693</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>44</v>
-      </c>
-      <c r="J32" t="s">
-        <v>72</v>
-      </c>
-      <c r="K32" s="8">
-        <f>C37</f>
-        <v>16.096298247680657</v>
-      </c>
-      <c r="L32">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="M32" t="s">
-        <v>73</v>
-      </c>
-      <c r="N32" s="13">
-        <f>K32*L32</f>
-        <v>4.3781931233691394</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>51</v>
-      </c>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C33" t="str">
         <f>IF(B34="Single value","Value",IF(B34="Range of values","Start",IF(B34="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
@@ -2788,91 +2966,24 @@
         <f>IF(B34="Single value","",IF(B34="Range of values","End",IF(B34="Monte Carlo","","ERROR")))</f>
         <v/>
       </c>
-      <c r="J33" t="s">
-        <v>74</v>
-      </c>
-      <c r="K33">
-        <v>1</v>
-      </c>
-      <c r="L33">
-        <v>2.2810000000000001</v>
-      </c>
-      <c r="M33" t="s">
-        <v>69</v>
-      </c>
-      <c r="N33">
-        <f>K33*L33</f>
-        <v>2.2810000000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>41</v>
+        <v>109</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="8">
-        <f>C6/((PI()/4)*C12^2)/N12</f>
-        <v>56.337043866882304</v>
+      <c r="C34" s="1">
+        <v>290</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" t="s">
-        <v>5</v>
-      </c>
-      <c r="J34" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="14">
-        <f>SUM(N30:N33)</f>
-        <v>25.727117046222833</v>
-      </c>
-      <c r="O34" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" t="str">
-        <f>IF(B37="Single value","Value",IF(B37="Range of values","Start",IF(B37="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D36" t="str">
-        <f>IF(B37="Single value","",IF(B37="Range of values","Step",IF(B37="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E36" t="str">
-        <f>IF(B37="Single value","",IF(B37="Range of values","End",IF(B37="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="8">
-        <f>C8/((PI()/4)*C12^2)/N12</f>
-        <v>16.096298247680657</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" t="s">
-        <v>31</v>
-      </c>
-      <c r="J37" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C38" t="str">
         <f>IF(B39="Single value","Value",IF(B39="Range of values","Start",IF(B39="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
@@ -2886,150 +2997,273 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="1">
+        <v>3</v>
+      </c>
+      <c r="D39" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C41" t="str">
+        <f>IF(B42="Single value","Value",IF(B42="Range of values","Start",IF(B42="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D41" t="str">
+        <f>IF(B42="Single value","",IF(B42="Range of values","Step",IF(B42="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E41" t="str">
+        <f>IF(B42="Single value","",IF(B42="Range of values","End",IF(B42="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" t="str">
+        <f>IF(B46="Single value","Value",IF(B46="Range of values","Start",IF(B46="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D45" t="str">
+        <f>IF(B46="Single value","",IF(B46="Range of values","Step",IF(B46="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E45" t="str">
+        <f>IF(B46="Single value","",IF(B46="Range of values","End",IF(B46="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="8">
+        <f>C7/((PI()/4)*C24^2)/N13</f>
+        <v>56.337043866882304</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" t="str">
+        <f>IF(B49="Single value","Value",IF(B49="Range of values","Start",IF(B49="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D48" t="str">
+        <f>IF(B49="Single value","",IF(B49="Range of values","Step",IF(B49="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E48" t="str">
+        <f>IF(B49="Single value","",IF(B49="Range of values","End",IF(B49="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="8">
+        <f>C9/((PI()/4)*C24^2)/N13</f>
+        <v>16.096298247680657</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="str">
+        <f>IF(B51="Single value","Value",IF(B51="Range of values","Start",IF(B51="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D50" t="str">
+        <f>IF(B51="Single value","",IF(B51="Range of values","Step",IF(B51="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E50" t="str">
+        <f>IF(B51="Single value","",IF(B51="Range of values","End",IF(B51="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="7">
+      <c r="B51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="7">
         <f>41.668101-2</f>
         <v>39.668101</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D51" s="4">
         <v>0.25</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E51" s="7">
         <f>41.668101+2</f>
         <v>43.668101</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F51" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C40" t="str">
-        <f>IF(B41="Single value","Value",IF(B41="Range of values","Start",IF(B41="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D40" t="str">
-        <f>IF(B41="Single value","",IF(B41="Range of values","Step",IF(B41="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E40" t="str">
-        <f>IF(B41="Single value","",IF(B41="Range of values","End",IF(B41="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C52" t="str">
+        <f>IF(B53="Single value","Value",IF(B53="Range of values","Start",IF(B53="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D52" t="str">
+        <f>IF(B53="Single value","",IF(B53="Range of values","Step",IF(B53="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E52" t="str">
+        <f>IF(B53="Single value","",IF(B53="Range of values","End",IF(B53="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="7">
+      <c r="B53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="7">
         <v>5.0911735</v>
       </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="1"/>
-      <c r="F41" t="s">
+      <c r="D53" s="4"/>
+      <c r="E53" s="1"/>
+      <c r="F53" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="16"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
-      <c r="B49" s="16"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="16"/>
-      <c r="B50" s="16"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="16"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="16"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="16"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="16"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="16"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="16"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="16"/>
       <c r="B55" s="16"/>
       <c r="C55" s="16"/>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
     </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="16"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="16"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="16"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="16"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="16"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="16"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="16"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="16"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="16"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="16"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="16"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="16"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:F5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B6 B47 B8 B10 B50 B12 B39 B14 B54 B52 B34 B37 B41 B16:B17 B20 B22:B24</xm:sqref>
+          <xm:sqref>B7 B56 B31:B32 B22 B59 B24 B51 B26 B63 B61 B46 B49 B53 B28:B29 B34:B36 B17 B19 B9:B10 B12 B14:B15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>[1]Validation!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>B27 B30</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Validation!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>B19</xm:sqref>
+          <xm:sqref>B39 B42</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Added limited film cooling support
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465" tabRatio="551" activeTab="3"/>
@@ -16,12 +16,12 @@
   <externalReferences>
     <externalReference r:id="rId6"/>
   </externalReferences>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="133">
   <si>
     <t>Total inert mass</t>
   </si>
@@ -430,6 +430,9 @@
   </si>
   <si>
     <t>N2 Ullage, set to 0% for none</t>
+  </si>
+  <si>
+    <t>Fuel Diverted to Film Cooling</t>
   </si>
 </sst>
 </file>
@@ -591,9 +594,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -605,6 +605,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -956,7 +959,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,22 +1156,22 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C25" t="str">
         <f>IF(B26="Single value","Value",IF(B26="Range of values","Start",IF(B26="Monte Carlo","Mean","ERROR")))</f>
-        <v>Mean</v>
+        <v>Value</v>
       </c>
       <c r="D25" t="str">
         <f>IF(B26="Single value","",IF(B26="Range of values","Step",IF(B26="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v>Standard deviation</v>
+        <v/>
       </c>
       <c r="E25" t="str">
         <f>IF(B26="Single value","",IF(B26="Range of values","End",IF(B26="Monte Carlo","","ERROR")))</f>
@@ -1180,14 +1183,12 @@
         <v>121</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C26" s="1">
         <v>3.353376168248183E-2</v>
       </c>
-      <c r="D26" s="1">
-        <v>0</v>
-      </c>
+      <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" t="s">
         <v>122</v>
@@ -1210,7 +1211,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>124</v>
       </c>
@@ -1269,7 +1270,7 @@
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A26:A27"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1750,7 +1751,7 @@
       </c>
       <c r="B14" s="2">
         <f>'Propellant Parameters (Tanks)'!N26*0.453592</f>
-        <v>11.669614475230308</v>
+        <v>13.655527850445562</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -1840,7 +1841,7 @@
       </c>
       <c r="C31" s="3">
         <f>SUM(B:B)</f>
-        <v>32.551591109707303</v>
+        <v>34.537504484922557</v>
       </c>
       <c r="D31" s="1">
         <f>1/8</f>
@@ -1848,7 +1849,7 @@
       </c>
       <c r="E31" s="3">
         <f>C31+5</f>
-        <v>37.551591109707303</v>
+        <v>39.537504484922557</v>
       </c>
       <c r="F31" t="s">
         <v>3</v>
@@ -1918,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1980,7 +1981,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>4.99</v>
+        <v>4.75</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -2009,13 +2010,8 @@
       <c r="C9" s="1">
         <v>0.9</v>
       </c>
-      <c r="D9" s="1">
-        <f>0.0025/2</f>
-        <v>1.25E-3</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.95</v>
-      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" t="str">
@@ -2211,7 +2207,7 @@
         <v>104</v>
       </c>
       <c r="B34">
-        <v>24</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2315,7 +2311,7 @@
       </c>
       <c r="C45" s="9">
         <f>B34*B37</f>
-        <v>7.6006121864624678E-6</v>
+        <v>1.5201224372924936E-5</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -2438,8 +2434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2493,21 +2489,21 @@
       <c r="F5" s="32"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22" t="str">
+      <c r="A6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21" t="str">
         <f>IF(B7="Single value","Value",IF(B7="Range of values","Start",IF(B7="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
       </c>
-      <c r="D6" s="22" t="str">
+      <c r="D6" s="21" t="str">
         <f>IF(B7="Single value","",IF(B7="Range of values","Step",IF(B7="Monte Carlo","Standard deviation","ERROR")))</f>
         <v/>
       </c>
-      <c r="E6" s="22" t="str">
+      <c r="E6" s="21" t="str">
         <f>IF(B7="Single value","",IF(B7="Range of values","End",IF(B7="Monte Carlo","","ERROR")))</f>
         <v/>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="22" t="s">
         <v>47</v>
       </c>
       <c r="K6" t="s">
@@ -2518,19 +2514,19 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="26">
+      <c r="B7" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="25">
         <f>$N$7*J7</f>
         <v>2.2941940000000001E-2</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="23" t="s">
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="22" t="s">
         <v>58</v>
       </c>
       <c r="J7" s="1">
@@ -2544,60 +2540,60 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="23"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="B9" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="26">
+      <c r="B9" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="25">
         <f>$N$7*J9</f>
-        <v>6.5548400000000001E-3</v>
-      </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="23" t="s">
+        <v>1.310968E-2</v>
+      </c>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="22" t="s">
         <v>58</v>
       </c>
       <c r="J9" s="1">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="K9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22" t="str">
+      <c r="A11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21" t="str">
         <f>IF(B12="Single value","Value",IF(B12="Range of values","Start",IF(B12="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
       </c>
-      <c r="D11" s="22" t="str">
+      <c r="D11" s="21" t="str">
         <f>IF(B12="Single value","",IF(B12="Range of values","Step",IF(B12="Monte Carlo","Standard deviation","ERROR")))</f>
         <v/>
       </c>
-      <c r="E11" s="22" t="str">
+      <c r="E11" s="21" t="str">
         <f>IF(B12="Single value","",IF(B12="Range of values","End",IF(B12="Monte Carlo","","ERROR")))</f>
         <v/>
       </c>
-      <c r="F11" s="23"/>
+      <c r="F11" s="22"/>
       <c r="J11" s="4">
         <f>93.19</f>
         <v>93.19</v>
@@ -2607,18 +2603,18 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="27">
+      <c r="B12" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="26">
         <v>0.15</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="23" t="s">
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="22" t="s">
         <v>58</v>
       </c>
       <c r="G12" t="s">
@@ -2629,12 +2625,12 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="23"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
       <c r="J13" s="4">
         <v>5.625</v>
       </c>
@@ -2646,18 +2642,18 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="B14" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="27">
+      <c r="B14" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="26">
         <v>0.15</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="23" t="s">
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="22" t="s">
         <v>58</v>
       </c>
       <c r="G14" t="s">
@@ -2665,12 +2661,12 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="23"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
       <c r="J15" s="1">
         <v>5.9089999999999998</v>
       </c>
@@ -2679,36 +2675,36 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22" t="str">
+      <c r="A16" s="20"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21" t="str">
         <f>IF(B17="Single value","Value",IF(B17="Range of values","Start",IF(B17="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
       </c>
-      <c r="D16" s="22" t="str">
+      <c r="D16" s="21" t="str">
         <f>IF(B17="Single value","",IF(B17="Range of values","Step",IF(B17="Monte Carlo","Standard deviation","ERROR")))</f>
         <v/>
       </c>
-      <c r="E16" s="22" t="str">
+      <c r="E16" s="21" t="str">
         <f>IF(B17="Single value","",IF(B17="Range of values","End",IF(B17="Monte Carlo","","ERROR")))</f>
         <v/>
       </c>
-      <c r="F16" s="23"/>
+      <c r="F16" s="22"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="26">
+      <c r="B17" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="25">
         <f>C7*(1-C12)</f>
         <v>1.9500649000000002E-2</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="23" t="s">
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="22" t="s">
         <v>58</v>
       </c>
       <c r="J17" s="1">
@@ -2719,27 +2715,27 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="23"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="30">
+      <c r="B19" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="29">
         <f>C9*(1-C14)</f>
-        <v>5.5716139999999999E-3</v>
-      </c>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="31" t="s">
+        <v>1.1143228E-2</v>
+      </c>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="30" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2749,6 +2745,12 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
       <c r="J21" t="s">
         <v>65</v>
       </c>
@@ -2766,21 +2768,18 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="9">
-        <f>$N$7*J11</f>
-        <v>1.5271138490000002E-3</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="1"/>
-      <c r="F22" t="s">
-        <v>58</v>
-      </c>
+      <c r="A22" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="21"/>
       <c r="J22" t="s">
         <v>67</v>
       </c>
@@ -2804,7 +2803,7 @@
         <v>71</v>
       </c>
       <c r="K23" s="8">
-        <f>C46</f>
+        <f>C48</f>
         <v>56.337043866882304</v>
       </c>
       <c r="L23">
@@ -2820,26 +2819,26 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="9">
-        <f>$N$13*J13</f>
-        <v>0.142875</v>
-      </c>
-      <c r="D24" s="1"/>
+        <f>$N$7*J11</f>
+        <v>1.5271138490000002E-3</v>
+      </c>
+      <c r="D24" s="4"/>
       <c r="E24" s="1"/>
       <c r="F24" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="J24" t="s">
         <v>72</v>
       </c>
       <c r="K24" s="8">
-        <f>C49</f>
-        <v>16.096298247680657</v>
+        <f>C51</f>
+        <v>32.192596495361315</v>
       </c>
       <c r="L24">
         <v>0.27200000000000002</v>
@@ -2849,7 +2848,7 @@
       </c>
       <c r="N24" s="13">
         <f>K24*L24</f>
-        <v>4.3781931233691394</v>
+        <v>8.7563862467382787</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -2873,14 +2872,14 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="9">
-        <f>$N$13*J15</f>
-        <v>0.15008859999999999</v>
+        <f>$N$13*J13</f>
+        <v>0.142875</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -2895,7 +2894,7 @@
       <c r="M26" s="12"/>
       <c r="N26" s="14">
         <f>SUM(N22:N25)</f>
-        <v>25.727117046222833</v>
+        <v>30.105310169591974</v>
       </c>
       <c r="O26" t="s">
         <v>48</v>
@@ -2903,14 +2902,14 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C28" s="9">
-        <f>$N$13*J17</f>
-        <v>7.2135999999999988E-3</v>
+        <f>$N$13*J15</f>
+        <v>0.15008859999999999</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -2924,191 +2923,177 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C30" t="str">
-        <f>IF(B31="Single value","Value",IF(B31="Range of values","Start",IF(B31="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D30" t="str">
-        <f>IF(B31="Single value","",IF(B31="Range of values","Step",IF(B31="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E30" t="str">
-        <f>IF(B31="Single value","",IF(B31="Range of values","End",IF(B31="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="9">
+        <f>$N$13*J17</f>
+        <v>7.2135999999999988E-3</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C32" t="str">
+        <f>IF(B33="Single value","Value",IF(B33="Range of values","Start",IF(B33="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D32" t="str">
+        <f>IF(B33="Single value","",IF(B33="Range of values","Step",IF(B33="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E32" t="str">
+        <f>IF(B33="Single value","",IF(B33="Range of values","End",IF(B33="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="1">
+      <c r="B33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1">
         <v>295</v>
       </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" t="s">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C33" t="str">
-        <f>IF(B34="Single value","Value",IF(B34="Range of values","Start",IF(B34="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D33" t="str">
-        <f>IF(B34="Single value","",IF(B34="Range of values","Step",IF(B34="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E33" t="str">
-        <f>IF(B34="Single value","",IF(B34="Range of values","End",IF(B34="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C35" t="str">
+        <f>IF(B36="Single value","Value",IF(B36="Range of values","Start",IF(B36="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D35" t="str">
+        <f>IF(B36="Single value","",IF(B36="Range of values","Step",IF(B36="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E35" t="str">
+        <f>IF(B36="Single value","",IF(B36="Range of values","End",IF(B36="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="1">
-        <v>290</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" t="s">
+      <c r="B36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="1">
+        <v>295</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C38" t="str">
-        <f>IF(B39="Single value","Value",IF(B39="Range of values","Start",IF(B39="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D38" t="str">
-        <f>IF(B39="Single value","",IF(B39="Range of values","Step",IF(B39="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E38" t="str">
-        <f>IF(B39="Single value","",IF(B39="Range of values","End",IF(B39="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C40" t="str">
+        <f>IF(B41="Single value","Value",IF(B41="Range of values","Start",IF(B41="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D40" t="str">
+        <f>IF(B41="Single value","",IF(B41="Range of values","Step",IF(B41="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E40" t="str">
+        <f>IF(B41="Single value","",IF(B41="Range of values","End",IF(B41="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="1">
-        <v>3</v>
-      </c>
-      <c r="D39" s="1"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C41" t="str">
-        <f>IF(B42="Single value","Value",IF(B42="Range of values","Start",IF(B42="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D41" t="str">
-        <f>IF(B42="Single value","",IF(B42="Range of values","Step",IF(B42="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E41" t="str">
-        <f>IF(B42="Single value","",IF(B42="Range of values","End",IF(B42="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="B41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="1">
+        <v>20</v>
+      </c>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C43" t="str">
+        <f>IF(B44="Single value","Value",IF(B44="Range of values","Start",IF(B44="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D43" t="str">
+        <f>IF(B44="Single value","",IF(B44="Range of values","Step",IF(B44="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E43" t="str">
+        <f>IF(B44="Single value","",IF(B44="Range of values","End",IF(B44="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="1">
-        <v>2</v>
-      </c>
-      <c r="D42" s="1"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="1">
+        <v>20</v>
+      </c>
+      <c r="D44" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>51</v>
       </c>
-      <c r="C45" t="str">
-        <f>IF(B46="Single value","Value",IF(B46="Range of values","Start",IF(B46="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D45" t="str">
-        <f>IF(B46="Single value","",IF(B46="Range of values","Step",IF(B46="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E45" t="str">
-        <f>IF(B46="Single value","",IF(B46="Range of values","End",IF(B46="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="C47" t="str">
+        <f>IF(B48="Single value","Value",IF(B48="Range of values","Start",IF(B48="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D47" t="str">
+        <f>IF(B48="Single value","",IF(B48="Range of values","Step",IF(B48="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E47" t="str">
+        <f>IF(B48="Single value","",IF(B48="Range of values","End",IF(B48="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" s="8">
-        <f>C7/((PI()/4)*C24^2)/N13</f>
+      <c r="B48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="8">
+        <f>C7/((PI()/4)*C26^2)/N13</f>
         <v>56.337043866882304</v>
       </c>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" t="s">
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>52</v>
       </c>
-      <c r="C48" t="str">
-        <f>IF(B49="Single value","Value",IF(B49="Range of values","Start",IF(B49="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D48" t="str">
-        <f>IF(B49="Single value","",IF(B49="Range of values","Step",IF(B49="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E48" t="str">
-        <f>IF(B49="Single value","",IF(B49="Range of values","End",IF(B49="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C49" s="8">
-        <f>C9/((PI()/4)*C24^2)/N13</f>
-        <v>16.096298247680657</v>
-      </c>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C50" t="str">
         <f>IF(B51="Single value","Value",IF(B51="Range of values","Start",IF(B51="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
@@ -3124,24 +3109,19 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C51" s="7">
-        <f>41.668101-2</f>
-        <v>39.668101</v>
-      </c>
-      <c r="D51" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="E51" s="7">
-        <f>41.668101+2</f>
-        <v>43.668101</v>
-      </c>
+      <c r="C51" s="8">
+        <f>C9/((PI()/4)*C26^2)/N13</f>
+        <v>32.192596495361315</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
       <c r="F51" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -3160,26 +3140,55 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="7">
-        <v>5.0911735</v>
-      </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="1"/>
+        <f>41.668101-2</f>
+        <v>39.668101</v>
+      </c>
+      <c r="D53" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E53" s="7">
+        <f>41.668101+2</f>
+        <v>43.668101</v>
+      </c>
       <c r="F53" t="s">
         <v>48</v>
       </c>
     </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C54" t="str">
+        <f>IF(B55="Single value","Value",IF(B55="Range of values","Start",IF(B55="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D54" t="str">
+        <f>IF(B55="Single value","",IF(B55="Range of values","Step",IF(B55="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E54" t="str">
+        <f>IF(B55="Single value","",IF(B55="Range of values","End",IF(B55="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="16"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
+      <c r="A55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="7">
+        <v>5.0911735</v>
+      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="1"/>
+      <c r="F55" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="16"/>
@@ -3257,13 +3266,13 @@
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B7 B56 B31:B32 B22 B59 B24 B51 B26 B63 B61 B46 B49 B53 B28:B29 B34:B36 B17 B19 B9:B10 B12 B14:B15</xm:sqref>
+          <xm:sqref>B7 B33:B34 B24 B59 B26 B53 B28 B63 B61 B48 B51 B55:B56 B30:B31 B36:B38 B17 B19 B9:B10 B12 B14:B15 B22</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>[1]Validation!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>B39 B42</xm:sqref>
+          <xm:sqref>B41 B44</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Updated default configuration, added default output
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="135">
   <si>
     <t>Total inert mass</t>
   </si>
@@ -433,6 +433,12 @@
   </si>
   <si>
     <t>Fuel Diverted to Film Cooling</t>
+  </si>
+  <si>
+    <t>Fudge</t>
+  </si>
+  <si>
+    <t>Factor</t>
   </si>
 </sst>
 </file>
@@ -573,7 +579,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -611,6 +617,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -1270,7 +1277,7 @@
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,7 +1477,7 @@
         <v>37</v>
       </c>
       <c r="B6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -1539,8 +1546,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="2">
-        <f>P2</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -1702,8 +1708,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="2">
-        <f>P5</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
@@ -1751,7 +1756,7 @@
       </c>
       <c r="B14" s="2">
         <f>'Propellant Parameters (Tanks)'!N26*0.453592</f>
-        <v>13.655527850445562</v>
+        <v>15.160295301298001</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -1786,6 +1791,22 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15">
+        <f>SUM(B3:B14)*E15</f>
+        <v>5.8563407903662492</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>134</v>
+      </c>
+      <c r="E15" s="33">
+        <v>0.15</v>
+      </c>
       <c r="G15" s="1" t="s">
         <v>93</v>
       </c>
@@ -1841,7 +1862,7 @@
       </c>
       <c r="C31" s="3">
         <f>SUM(B:B)</f>
-        <v>34.537504484922557</v>
+        <v>44.898612726141245</v>
       </c>
       <c r="D31" s="1">
         <f>1/8</f>
@@ -1849,7 +1870,7 @@
       </c>
       <c r="E31" s="3">
         <f>C31+5</f>
-        <v>39.537504484922557</v>
+        <v>49.898612726141245</v>
       </c>
       <c r="F31" t="s">
         <v>3</v>
@@ -1920,7 +1941,7 @@
   <dimension ref="A2:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1981,7 +2002,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>4.75</v>
+        <v>4.99</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -2434,8 +2455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2522,7 +2543,7 @@
       </c>
       <c r="C7" s="25">
         <f>$N$7*J7</f>
-        <v>2.2941940000000001E-2</v>
+        <v>2.6219360000000001E-2</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
@@ -2530,7 +2551,7 @@
         <v>58</v>
       </c>
       <c r="J7" s="1">
-        <v>1400</v>
+        <v>1600</v>
       </c>
       <c r="K7" t="s">
         <v>42</v>
@@ -2556,7 +2577,7 @@
       </c>
       <c r="C9" s="25">
         <f>$N$7*J9</f>
-        <v>1.310968E-2</v>
+        <v>1.5076132000000001E-2</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
@@ -2564,7 +2585,7 @@
         <v>58</v>
       </c>
       <c r="J9" s="1">
-        <v>800</v>
+        <v>920</v>
       </c>
       <c r="K9" t="s">
         <v>42</v>
@@ -2700,7 +2721,7 @@
       </c>
       <c r="C17" s="25">
         <f>C7*(1-C12)</f>
-        <v>1.9500649000000002E-2</v>
+        <v>2.2286456E-2</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="24"/>
@@ -2731,7 +2752,7 @@
       </c>
       <c r="C19" s="29">
         <f>C9*(1-C14)</f>
-        <v>1.1143228E-2</v>
+        <v>1.28147122E-2</v>
       </c>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
@@ -2804,7 +2825,7 @@
       </c>
       <c r="K23" s="8">
         <f>C48</f>
-        <v>56.337043866882304</v>
+        <v>64.385192990722629</v>
       </c>
       <c r="L23">
         <v>0.249</v>
@@ -2814,7 +2835,7 @@
       </c>
       <c r="N23" s="13">
         <f>K23*L23</f>
-        <v>14.027923922853693</v>
+        <v>16.031913054689934</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -2838,7 +2859,7 @@
       </c>
       <c r="K24" s="8">
         <f>C51</f>
-        <v>32.192596495361315</v>
+        <v>37.02148596966552</v>
       </c>
       <c r="L24">
         <v>0.27200000000000002</v>
@@ -2848,7 +2869,7 @@
       </c>
       <c r="N24" s="13">
         <f>K24*L24</f>
-        <v>8.7563862467382787</v>
+        <v>10.069844183749023</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -2894,7 +2915,7 @@
       <c r="M26" s="12"/>
       <c r="N26" s="14">
         <f>SUM(N22:N25)</f>
-        <v>30.105310169591974</v>
+        <v>33.422757238438955</v>
       </c>
       <c r="O26" t="s">
         <v>48</v>
@@ -3082,7 +3103,7 @@
       </c>
       <c r="C48" s="8">
         <f>C7/((PI()/4)*C26^2)/N13</f>
-        <v>56.337043866882304</v>
+        <v>64.385192990722629</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -3116,7 +3137,7 @@
       </c>
       <c r="C51" s="8">
         <f>C9/((PI()/4)*C26^2)/N13</f>
-        <v>32.192596495361315</v>
+        <v>37.02148596966552</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>

</xml_diff>

<commit_message>
Some progress on making it less broken
Need to actually write N2-pressurized nitrous variant
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -2455,8 +2455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2960,6 +2960,9 @@
         <v>31</v>
       </c>
     </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N31" s="13"/>
+    </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C32" t="str">
         <f>IF(B33="Single value","Value",IF(B33="Range of values","Start",IF(B33="Monte Carlo","Mean","ERROR")))</f>
@@ -2974,7 +2977,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>110</v>
       </c>
@@ -2989,8 +2992,9 @@
       <c r="F33" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="O33" s="13"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C35" t="str">
         <f>IF(B36="Single value","Value",IF(B36="Range of values","Start",IF(B36="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
@@ -3004,7 +3008,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>109</v>
       </c>
@@ -3020,7 +3024,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C40" t="str">
         <f>IF(B41="Single value","Value",IF(B41="Range of values","Start",IF(B41="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
@@ -3034,7 +3038,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>99</v>
       </c>
@@ -3046,7 +3050,7 @@
       </c>
       <c r="D41" s="1"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C43" t="str">
         <f>IF(B44="Single value","Value",IF(B44="Range of values","Start",IF(B44="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
@@ -3060,7 +3064,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>100</v>
       </c>
@@ -3072,12 +3076,12 @@
       </c>
       <c r="D44" s="1"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -3094,7 +3098,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Added quick and dirty ignition time
Also changed launch angle to 84 degrees and lowered propellant temperature by 5 K
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Files\Documents\GitHub\IREC-ROCSIM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465" tabRatio="551" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="551" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
@@ -16,12 +21,12 @@
   <externalReferences>
     <externalReference r:id="rId6"/>
   </externalReferences>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="137">
   <si>
     <t>Total inert mass</t>
   </si>
@@ -440,11 +445,17 @@
   <si>
     <t>Factor</t>
   </si>
+  <si>
+    <t>Ignition Time</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -611,13 +622,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -630,6 +641,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -719,7 +733,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -752,9 +766,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -787,6 +818,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -962,11 +1010,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,7 +1114,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1163,13 +1211,13 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C25" t="str">
@@ -1242,25 +1290,25 @@
     <mergeCell ref="A24:E24"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G1" r:id="rId1" display="https://www.usclimatedata.com/climate/truth-or-consequences/new-mexico/united-states/usnm0332"/>
+    <hyperlink ref="G1" r:id="rId1" display="https://www.usclimatedata.com/climate/truth-or-consequences/new-mexico/united-states/usnm0332" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>B4 B13 B10 B7 B20 B26 B29</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>Validation!$A$2</xm:f>
           </x14:formula1>
@@ -1273,11 +1321,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,7 +1852,7 @@
       <c r="D15" t="s">
         <v>134</v>
       </c>
-      <c r="E15" s="33">
+      <c r="E15" s="31">
         <v>0.15</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -1924,7 +1972,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
@@ -1937,11 +1985,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:F59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2428,20 +2476,54 @@
         <v>98</v>
       </c>
     </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C58" t="str">
+        <f>IF(B59="Single value","Value",IF(B59="Range of values","Start",IF(B59="Monte Carlo","Mean","ERROR")))</f>
+        <v>Start</v>
+      </c>
+      <c r="D58" t="str">
+        <f>IF(B59="Single value","",IF(B59="Range of values","Step",IF(B59="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v>Step</v>
+      </c>
+      <c r="E58" t="str">
+        <f>IF(B59="Single value","",IF(B59="Range of values","End",IF(B59="Monte Carlo","","ERROR")))</f>
+        <v>End</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" s="1">
+        <v>0</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E59" s="1">
+        <v>1</v>
+      </c>
+      <c r="F59" t="s">
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B3 B6 B9 B12 B15 B18 B21 B24 B28</xm:sqref>
+          <xm:sqref>B3 B6 B9 B12 B15 B18 B21 B24 B28 B59</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>
-            <xm:f>[1]Validation!#REF!</xm:f>
+            <xm:f>'E:\Users\jpb0024\Downloads\[simconfig (1).xlsx]Validation'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B45 B48 B51 B54</xm:sqref>
         </x14:dataValidation>
@@ -2452,11 +2534,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A58" sqref="A57:F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2500,14 +2582,14 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
@@ -2982,7 +3064,7 @@
         <v>8</v>
       </c>
       <c r="C33" s="1">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -3012,7 +3094,7 @@
         <v>8</v>
       </c>
       <c r="C36" s="1">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -3217,20 +3299,6 @@
       <c r="C56" s="17"/>
       <c r="D56" s="16"/>
       <c r="E56" s="16"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="16"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="16"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="16"/>
@@ -3283,15 +3351,15 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B7 B33:B34 B24 B59 B26 B53 B28 B63 B61 B48 B51 B55:B56 B30:B31 B36:B38 B17 B19 B9:B10 B12 B14:B15 B22</xm:sqref>
+          <xm:sqref>B7 B33:B34 B24 B26 B53 B28 B63 B61 B48 B51 B55:B56 B30:B31 B36:B38 B17 B19 B9:B10 B12 B14:B15 B22 B59</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000001000000}">
           <x14:formula1>
-            <xm:f>[1]Validation!#REF!</xm:f>
+            <xm:f>'E:\Users\jpb0024\Downloads\[simconfig (1).xlsx]Validation'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B41 B44</xm:sqref>
         </x14:dataValidation>
@@ -3302,7 +3370,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Added Avionics Signal Calcs
Also added avionics section to simconfig, and added avionics parameters to matlab functions. Refactored INS section to include all avionics
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -9,24 +9,25 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="551" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="551" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
     <sheet name="Rocket Parameters (Mass)" sheetId="1" r:id="rId2"/>
     <sheet name="Engine Parameters" sheetId="4" r:id="rId3"/>
     <sheet name="Propellant Parameters (Tanks)" sheetId="5" r:id="rId4"/>
-    <sheet name="Validation" sheetId="3" r:id="rId5"/>
+    <sheet name="Avionics Parameters" sheetId="6" r:id="rId5"/>
+    <sheet name="Validation" sheetId="3" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="147">
   <si>
     <t>Total inert mass</t>
   </si>
@@ -462,6 +463,24 @@
   </si>
   <si>
     <t>Airframe</t>
+  </si>
+  <si>
+    <t>Ground Station Distance</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>MHz</t>
+  </si>
+  <si>
+    <t>Transmit Power</t>
+  </si>
+  <si>
+    <t>dBm</t>
+  </si>
+  <si>
+    <t>Receive Sensitivity</t>
   </si>
 </sst>
 </file>
@@ -2046,7 +2065,7 @@
   <dimension ref="A2:F59"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A14" sqref="A14:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2565,6 +2584,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -2590,7 +2610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -3432,6 +3452,158 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB3B354-9018-479A-B92D-A43716FA7D64}">
+  <dimension ref="A3:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" t="str">
+        <f>IF(B4="Single value","Value",IF(B4="Range of values","Start",IF(B4="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D3" t="str">
+        <f>IF(B4="Single value","",IF(B4="Range of values","Step",IF(B4="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E3" t="str">
+        <f>IF(B4="Single value","",IF(B4="Range of values","End",IF(B4="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>609.6</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C6" t="str">
+        <f>IF(B7="Single value","Value",IF(B7="Range of values","Start",IF(B7="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D6" t="str">
+        <f>IF(B7="Single value","",IF(B7="Range of values","Step",IF(B7="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E6" t="str">
+        <f>IF(B7="Single value","",IF(B7="Range of values","End",IF(B7="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1">
+        <v>915</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" t="str">
+        <f>IF(B10="Single value","Value",IF(B10="Range of values","Start",IF(B10="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D9" t="str">
+        <f>IF(B10="Single value","",IF(B10="Range of values","Step",IF(B10="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E9" t="str">
+        <f>IF(B10="Single value","",IF(B10="Range of values","End",IF(B10="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>23</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12" t="str">
+        <f>IF(B13="Single value","Value",IF(B13="Range of values","Start",IF(B13="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D12" t="str">
+        <f>IF(B13="Single value","",IF(B13="Range of values","Step",IF(B13="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E12" t="str">
+        <f>IF(B13="Single value","",IF(B13="Range of values","End",IF(B13="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-101</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{58C107EB-1257-4C54-A53B-0F2FDC42EB85}">
+          <x14:formula1>
+            <xm:f>Validation!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B4 B7 B10 B13</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated to MATLAB R2018A, Tried to fix a major bug and ended up just fixing a few little ones
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Files\Documents\GitHub\IREC-ROCSIM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Thomas\Documents\GitHub\IREC-ROCSIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13019AD1-B26F-4876-92C2-80587F74140A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="551" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="551" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
@@ -22,7 +23,7 @@
   <externalReferences>
     <externalReference r:id="rId7"/>
   </externalReferences>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -1046,7 +1047,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1988,14 +1989,8 @@
         <f>SUM(B:B)</f>
         <v>44.898612726141245</v>
       </c>
-      <c r="D31" s="1">
-        <f>1/8</f>
-        <v>0.125</v>
-      </c>
-      <c r="E31" s="3">
-        <f>C31+5</f>
-        <v>49.898612726141245</v>
-      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="3"/>
       <c r="F31" t="s">
         <v>3</v>
       </c>
@@ -2064,8 +2059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:E15"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2610,8 +2605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3138,7 +3133,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>110</v>
       </c>
@@ -3154,7 +3149,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C35" t="str">
         <f>IF(B36="Single value","Value",IF(B36="Range of values","Start",IF(B36="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
@@ -3168,7 +3163,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>109</v>
       </c>
@@ -3184,7 +3179,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C40" t="str">
         <f>IF(B41="Single value","Value",IF(B41="Range of values","Start",IF(B41="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
@@ -3198,7 +3193,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>99</v>
       </c>
@@ -3209,8 +3204,9 @@
         <v>24</v>
       </c>
       <c r="D41" s="1"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E41" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C43" t="str">
         <f>IF(B44="Single value","Value",IF(B44="Range of values","Start",IF(B44="Monte Carlo","Mean","ERROR")))</f>
         <v>Value</v>
@@ -3224,7 +3220,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>100</v>
       </c>
@@ -3235,13 +3231,17 @@
         <v>6</v>
       </c>
       <c r="D44" s="1"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E44" s="1"/>
+      <c r="G44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>41</v>
       </c>
@@ -3432,18 +3432,12 @@
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B7 B33:B34 B24 B26 B53 B28 B63 B61 B48 B51 B55:B56 B30:B31 B36:B38 B17 B19 B9:B10 B12 B14:B15 B22 B59</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000001000000}">
-          <x14:formula1>
-            <xm:f>'E:\Users\jpb0024\Downloads\[simconfig (1).xlsx]Validation'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B41 B44</xm:sqref>
+          <xm:sqref>B7 B30:B31 B24 B26 B53 B28 B63 B61 B48 B51 B55:B56 B59 B33:B34 B17 B19 B9:B10 B12 B14:B15 B22 B36:B38 B41 B44</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3455,8 +3449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB3B354-9018-479A-B92D-A43716FA7D64}">
   <dimension ref="A3:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Tested the fix, looks like a step in the right direction, but something's still fishy
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Thomas\Documents\GitHub\IREC-ROCSIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13019AD1-B26F-4876-92C2-80587F74140A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0148D1-CF5E-46A4-B24D-C5F4F8929429}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="551" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="551" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
@@ -2605,7 +2605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Finally sorta fixed cv bug
also introduced a bug where it crashes if the cv is too low, oops
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Thomas\Documents\GitHub\IREC-ROCSIM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0148D1-CF5E-46A4-B24D-C5F4F8929429}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="551" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="551" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
@@ -23,7 +17,7 @@
   <externalReferences>
     <externalReference r:id="rId7"/>
   </externalReferences>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -487,7 +481,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -766,7 +760,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -799,26 +793,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -851,23 +828,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1043,7 +1003,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1323,25 +1283,25 @@
     <mergeCell ref="A24:E24"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17">
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G1" r:id="rId1" display="https://www.usclimatedata.com/climate/truth-or-consequences/new-mexico/united-states/usnm0332" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G1" r:id="rId1" display="https://www.usclimatedata.com/climate/truth-or-consequences/new-mexico/united-states/usnm0332"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>B4 B13 B10 B7 B20 B26 B29</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Validation!$A$2</xm:f>
           </x14:formula1>
@@ -1354,7 +1314,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
@@ -2043,7 +2003,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
@@ -2056,10 +2016,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
@@ -2583,15 +2543,15 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>B3 B6 B9 B12 B15 B18 B21 B24 B28 B59</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'E:\Users\jpb0024\Downloads\[simconfig (1).xlsx]Validation'!#REF!</xm:f>
+            <xm:f>[1]Validation!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B45 B48 B51 B54</xm:sqref>
         </x14:dataValidation>
@@ -2602,11 +2562,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3201,10 +3161,17 @@
         <v>8</v>
       </c>
       <c r="C41" s="1">
+        <f>G41/F41</f>
         <v>24</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>24</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C43" t="str">
@@ -3228,10 +3195,14 @@
         <v>8</v>
       </c>
       <c r="C44" s="1">
+        <f>G44/F44</f>
         <v>6</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
+      <c r="F44">
+        <v>1</v>
+      </c>
       <c r="G44">
         <v>6</v>
       </c>
@@ -3433,7 +3404,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
@@ -3446,7 +3417,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB3B354-9018-479A-B92D-A43716FA7D64}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3585,7 +3556,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{58C107EB-1257-4C54-A53B-0F2FDC42EB85}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
@@ -3598,7 +3569,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>